<commit_message>
Update the test case file after out of the work on 31th,May
</commit_message>
<xml_diff>
--- a/src/MyItems/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="260">
   <si>
     <t>Test Case 001</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -768,160 +768,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>1. 输入</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>不存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹路径</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>（若是根目录格式为D:\\）</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.输入</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>任意</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>原来的文件夹名字
-3.输入更改的文件夹名字</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1. 输入</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹路径</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>（若是根目录格式为D:\\）</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.输入该路径下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>不存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>原来的文件夹名字
-3.输入更改的文件夹名字</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>重命名文件</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -930,238 +776,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>1. 输入</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹路径</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>（若是根目录格式为D:\\）</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.输入该路径下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>原来的文件名字
-3.输入更改的文件名字</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Test Case 036</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1. 输入</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹路径</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>（若是根目录格式为D:\\）</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.输入该路径下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>不存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>原来的文件名字
-3.输入更改的文件名字</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1. 输入</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>不存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹路径</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>（若是根目录格式为D:\\）</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.输入</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>任意</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>原来的文件名字
-3.输入更改的文件名字</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2720,258 +2335,6 @@
   </si>
   <si>
     <r>
-      <t>1. 输入</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>根层</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹路径</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>（若是根目录格式为D:\\）</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.输入该路径下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>原来的文件夹名字
-3.输入更改的文件夹名字</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Input your folder path(if on disk should type like this -&gt; E:\ )</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Input your folder name:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-3.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please Input what words you want to replace:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入新的想要被替换的文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.显示指定的文件夹名已被换成新命名的名字（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Rename succeed!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.在本地计算机中能够查看到新命名的文件夹</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>1.显示目标文件夹路径不存在（</t>
     </r>
     <r>
@@ -3002,36 +2365,6 @@
   </si>
   <si>
     <r>
-      <t>1.显示需要被更改名字的文件夹不存在（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test1 is not exists!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.文件夹不应被重命名成功</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>1.能够出现提示输入的信息
 2.显示指定文件被找到的信息（</t>
     </r>
@@ -3121,201 +2454,6 @@
   </si>
   <si>
     <t>测试数据</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Input your folder path(if on disk should type like this -&gt; E:\ )</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">D:\Test
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Input your file name:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>456.txt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-3.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Input new file name want to replace:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入新的想要被替换的文件名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>988.txt</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.显示指定的文件名已被换成新命名的名字（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Rename succeed!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.在本地计算机中能够查看到新命名的文件</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.显示需要被更改名字的文件不存在（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\456.txt is not exists!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.文件不应被重命名成功</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -3902,161 +3040,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>1. 输入</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹路径</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>（若是根目录格式为D:\\）</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.输入该路径下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>非文件夹</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>的名字，而输入文件名字
-3.输入更改的文件夹名字</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Test Case 055</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1. 输入</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹路径</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>（若是根目录格式为D:\\）</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.输入该路径下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>非文件</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>的名字，而输入文件夹名字
-3.输入更改的文件名字</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -4086,307 +3070,6 @@
       </rPr>
       <t>）
 2.文件重命名失败</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Input your folder path(if on disk should type like this -&gt; E:\ )</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Input your folder name:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-3.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please Input what words you want to replace:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入新的想要被替换的文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test.txt</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Input your folder path(if on disk should type like this -&gt; E:\ )</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Input your folder name:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ABC.txt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-3.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please Input what words you want to replace:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入新的想要被替换的文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.显示目标文件夹路径不存在
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test is not exists!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.文件不应被重命名成功</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -7399,6 +6082,944 @@
   </si>
   <si>
     <t>Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Input your folder name:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\TesT39</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please Input what words you want to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test4</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示指定的文件夹名已被换成新命名的名字（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\TesT39 has been renamed as D:\Test4 successfully!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.在本地计算机中能够查看到新命名的文件夹</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示需要被更改名字的文件夹不存在（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\Honda is not exists!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.文件夹不应被重命名成功</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test case 056</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示需要更改的文件夹已经存在（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test4 has already exists, can not be renamed!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.文件夹不应被重命名成功</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Input your folder name:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\Alonso.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please Input what words you want to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test Case 057</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>原来的文件名字
+2.输入替换的文件名字</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>不存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>原来的文件名字
+2.输入替换的文件名字</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>非文件</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的名字，而输入文件夹名字
+2.输入替换的文件名字</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+1.输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>原来的文件夹名字
+2.输入替换的文件夹名字</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>不存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>原来的文件夹名字
+2.输入替换的文件夹名字</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>不存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹路径
+2.输入替换的文件夹名字</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>原来的文件夹名字
+2.输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的替换</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的文件夹名字</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>非文件夹</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的名字，而输入文件名字
+3.输入替换的文件夹名字</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Input your file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\ALO.bmp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please Input what words you want to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BUT.txt</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示需要被更改名字的文件不存在（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\ALO.bmp is not exists!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.文件不应被重命名成功</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>不存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的路径名字
+2.输入替换的文件名字</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示目标文件夹路径不存在
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\AAA\111.TXT is not exists!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.文件不应被重命名成功</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>原来的文件名字
+2.输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的替换</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的文件名字</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示指定的文件名已被换成新命名的名字（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\ALO.bmp has been renamed as D:\Test\BUT.txt successfully!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.在本地计算机中能够查看到新命名的文件</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Input your folder name:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please Input what words you want to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test2</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示需要更改的文件夹已经存在（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\Alonso.accdb has already exists, can not be renamed!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.文件夹不应被重命名成功</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -7606,7 +7227,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -7670,8 +7291,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -7685,15 +7309,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7703,11 +7318,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8033,18 +7648,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="A1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -8053,10 +7668,10 @@
         <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -8072,23 +7687,23 @@
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>102</v>
+      <c r="B3" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>97</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>143</v>
+        <v>72</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>138</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -8096,17 +7711,17 @@
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
       <c r="D4" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E4" s="30"/>
+        <v>73</v>
+      </c>
+      <c r="E4" s="28"/>
       <c r="F4" s="2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -8114,38 +7729,38 @@
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
       <c r="D5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="30"/>
+      <c r="E5" s="28"/>
       <c r="F5" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
+        <v>74</v>
+      </c>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="31"/>
+      <c r="E6" s="29"/>
       <c r="F6" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
@@ -8170,10 +7785,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H6"/>
+  <dimension ref="A2:H7"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8201,7 +7816,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -8213,89 +7828,109 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>63</v>
+        <v>66</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>175</v>
+        <v>242</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>250</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>176</v>
+        <v>257</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
+        <v>84</v>
+      </c>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
       <c r="D4" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="30"/>
+        <v>243</v>
+      </c>
+      <c r="E4" s="28"/>
       <c r="F4" s="2" t="s">
-        <v>177</v>
+        <v>251</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
+        <v>85</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
       <c r="D5" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" s="31"/>
+        <v>252</v>
+      </c>
+      <c r="E5" s="28"/>
       <c r="F5" s="2" t="s">
-        <v>195</v>
+        <v>253</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" s="13" customFormat="1" ht="142.5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" s="13" customFormat="1" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A6" s="11" t="s">
-        <v>190</v>
+        <v>241</v>
       </c>
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
       <c r="D6" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>193</v>
-      </c>
+        <v>254</v>
+      </c>
+      <c r="E6" s="29"/>
       <c r="F6" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+        <v>259</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" spans="1:8" s="13" customFormat="1" ht="99.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>258</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="H7" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="E3:E6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8307,7 +7942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H8"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3:E5"/>
     </sheetView>
   </sheetViews>
@@ -8333,10 +7968,10 @@
         <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -8350,63 +7985,63 @@
     </row>
     <row r="3" spans="1:8" ht="327.75" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="30" t="s">
         <v>68</v>
       </c>
+      <c r="C3" s="30" t="s">
+        <v>63</v>
+      </c>
       <c r="D3" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>178</v>
+        <v>167</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>166</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
+        <v>87</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
       <c r="D4" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E4" s="30"/>
+        <v>69</v>
+      </c>
+      <c r="E4" s="28"/>
       <c r="F4" s="2" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+        <v>88</v>
+      </c>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5" s="31"/>
+        <v>67</v>
+      </c>
+      <c r="E5" s="29"/>
       <c r="F5" s="2" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -8460,10 +8095,10 @@
         <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -8477,97 +8112,97 @@
     </row>
     <row r="3" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B3" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C3" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F3" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>135</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
+        <v>123</v>
+      </c>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
       <c r="D4" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="F4" s="24"/>
+        <v>172</v>
+      </c>
+      <c r="F4" s="25"/>
       <c r="G4" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
+        <v>124</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
       <c r="D5" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F5" s="24"/>
+        <v>173</v>
+      </c>
+      <c r="F5" s="25"/>
       <c r="G5" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F6" s="25"/>
+      <c r="G6" s="5" t="s">
         <v>133</v>
-      </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="F6" s="24"/>
-      <c r="G6" s="5" t="s">
-        <v>138</v>
       </c>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
+        <v>131</v>
+      </c>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
       <c r="D7" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="F7" s="25"/>
+        <v>174</v>
+      </c>
+      <c r="F7" s="26"/>
       <c r="G7" s="5" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="H7" s="5"/>
     </row>
@@ -8605,14 +8240,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="A1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -8625,10 +8260,10 @@
         <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -8642,67 +8277,67 @@
     </row>
     <row r="3" spans="1:9" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="24" t="s">
         <v>24</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="24"/>
+        <v>76</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" s="25"/>
       <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="25"/>
+        <v>77</v>
+      </c>
+      <c r="B5" s="30"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -8718,7 +8353,7 @@
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B8" s="27"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="4"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -8729,7 +8364,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
-      <c r="B9" s="27"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="4"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -8740,7 +8375,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
-      <c r="B10" s="27"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="4"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -8771,7 +8406,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
-      <c r="B13" s="27"/>
+      <c r="B13" s="31"/>
       <c r="C13" s="4"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -8782,7 +8417,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
-      <c r="B14" s="27"/>
+      <c r="B14" s="31"/>
       <c r="C14" s="4"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -8793,7 +8428,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
-      <c r="B15" s="27"/>
+      <c r="B15" s="31"/>
       <c r="C15" s="4"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -8804,7 +8439,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
-      <c r="B16" s="27"/>
+      <c r="B16" s="31"/>
       <c r="C16" s="4"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -8815,7 +8450,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
-      <c r="B17" s="27"/>
+      <c r="B17" s="31"/>
       <c r="C17" s="4"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -8911,10 +8546,10 @@
         <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -8928,67 +8563,67 @@
     </row>
     <row r="3" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="24" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="24"/>
+        <v>79</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" s="25"/>
       <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="H4" s="14" t="s">
         <v>155</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="25"/>
+        <v>80</v>
+      </c>
+      <c r="B5" s="30"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -9046,10 +8681,10 @@
         <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -9063,45 +8698,45 @@
     </row>
     <row r="3" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B3" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="30" t="s">
         <v>27</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>222</v>
+        <v>187</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>205</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
       <c r="D4" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="E4" s="30"/>
+        <v>188</v>
+      </c>
+      <c r="E4" s="28"/>
       <c r="F4" s="2" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -9109,37 +8744,37 @@
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="E5" s="30"/>
+        <v>189</v>
+      </c>
+      <c r="E5" s="28"/>
       <c r="F5" s="2" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="E6" s="31"/>
+        <v>190</v>
+      </c>
+      <c r="E6" s="29"/>
       <c r="F6" s="2" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -9147,39 +8782,39 @@
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="E7" s="28" t="s">
-        <v>223</v>
+        <v>191</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>206</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" s="13" customFormat="1" ht="114" x14ac:dyDescent="0.15">
       <c r="A8" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
+        <v>111</v>
+      </c>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="11" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>203</v>
+        <v>205</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>186</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="H8" s="17"/>
     </row>
@@ -9239,10 +8874,10 @@
         <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F2" s="16" t="s">
         <v>10</v>
@@ -9256,25 +8891,25 @@
     </row>
     <row r="3" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="B3" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="23" t="s">
-        <v>118</v>
+      <c r="C3" s="24" t="s">
+        <v>113</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>226</v>
+        <v>198</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>209</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H3" s="16"/>
     </row>
@@ -9282,17 +8917,17 @@
       <c r="A4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
       <c r="D4" s="16" t="s">
-        <v>216</v>
-      </c>
-      <c r="E4" s="30"/>
+        <v>199</v>
+      </c>
+      <c r="E4" s="28"/>
       <c r="F4" s="16" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H4" s="16"/>
     </row>
@@ -9300,17 +8935,17 @@
       <c r="A5" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
       <c r="D5" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="E5" s="30"/>
+        <v>200</v>
+      </c>
+      <c r="E5" s="28"/>
       <c r="F5" s="16" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H5" s="16"/>
     </row>
@@ -9318,17 +8953,17 @@
       <c r="A6" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
       <c r="D6" s="16" t="s">
-        <v>218</v>
-      </c>
-      <c r="E6" s="31"/>
+        <v>201</v>
+      </c>
+      <c r="E6" s="29"/>
       <c r="F6" s="16" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H6" s="16"/>
     </row>
@@ -9336,42 +8971,42 @@
       <c r="A7" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
       <c r="D7" s="16" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H7" s="16"/>
     </row>
     <row r="8" spans="1:8" s="13" customFormat="1" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A8" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
+        <v>106</v>
+      </c>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
       <c r="D8" s="11" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -9393,7 +9028,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+    <sheetView topLeftCell="D10" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -9419,10 +9054,10 @@
         <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -9438,23 +9073,23 @@
       <c r="A3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="24" t="s">
         <v>35</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>228</v>
+        <v>219</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>211</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -9462,17 +9097,17 @@
       <c r="A4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
       <c r="D4" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="E4" s="30"/>
+        <v>220</v>
+      </c>
+      <c r="E4" s="28"/>
       <c r="F4" s="2" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -9480,17 +9115,17 @@
       <c r="A5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
       <c r="D5" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="E5" s="30"/>
+        <v>221</v>
+      </c>
+      <c r="E5" s="28"/>
       <c r="F5" s="2" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -9498,57 +9133,57 @@
       <c r="A6" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
       <c r="D6" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="E6" s="30"/>
+        <v>222</v>
+      </c>
+      <c r="E6" s="28"/>
       <c r="F6" s="2" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" s="13" customFormat="1" ht="156.75" x14ac:dyDescent="0.15">
       <c r="A7" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="E7" s="29"/>
+      <c r="F7" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="H7" s="18" t="s">
         <v>232</v>
-      </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="E7" s="31"/>
-      <c r="F7" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>251</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
       <c r="D8" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>229</v>
+        <v>224</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>212</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H8" s="2"/>
     </row>
@@ -9556,17 +9191,17 @@
       <c r="A9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
       <c r="D9" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="E9" s="30"/>
+        <v>225</v>
+      </c>
+      <c r="E9" s="28"/>
       <c r="F9" s="2" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H9" s="2"/>
     </row>
@@ -9574,17 +9209,17 @@
       <c r="A10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
       <c r="D10" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="E10" s="30"/>
+        <v>226</v>
+      </c>
+      <c r="E10" s="28"/>
       <c r="F10" s="2" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H10" s="5"/>
     </row>
@@ -9592,38 +9227,38 @@
       <c r="A11" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
       <c r="D11" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="E11" s="30"/>
+        <v>227</v>
+      </c>
+      <c r="E11" s="28"/>
       <c r="F11" s="2" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" s="13" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A12" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
+        <v>110</v>
+      </c>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
       <c r="D12" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="E12" s="31"/>
+        <v>228</v>
+      </c>
+      <c r="E12" s="29"/>
       <c r="F12" s="11" t="s">
-        <v>248</v>
+        <v>231</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -9671,10 +9306,10 @@
         <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -9688,94 +9323,94 @@
     </row>
     <row r="3" spans="1:9" ht="156.75" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="30" t="s">
         <v>44</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="29" t="s">
-        <v>197</v>
+      <c r="E3" s="27" t="s">
+        <v>180</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
+        <v>96</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
       <c r="D4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="30"/>
+      <c r="E4" s="28"/>
       <c r="F4" s="2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="30"/>
+      <c r="E5" s="28"/>
       <c r="F5" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+        <v>95</v>
+      </c>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="31"/>
+      <c r="E6" s="29"/>
       <c r="F6" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="I6" s="20" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
@@ -9807,7 +9442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H9"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3:E5"/>
     </sheetView>
   </sheetViews>
@@ -9833,10 +9468,10 @@
         <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -9852,23 +9487,23 @@
       <c r="A3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="30" t="s">
         <v>53</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="29" t="s">
-        <v>164</v>
+      <c r="E3" s="27" t="s">
+        <v>159</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -9876,37 +9511,37 @@
       <c r="A4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
       <c r="D4" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="30"/>
+      <c r="E4" s="28"/>
       <c r="F4" s="2" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="31"/>
+      <c r="E5" s="29"/>
       <c r="F5" s="2" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -9930,10 +9565,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H6"/>
+  <dimension ref="A2:H7"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9943,7 +9578,7 @@
     <col min="3" max="3" width="15.375" customWidth="1"/>
     <col min="4" max="4" width="30.875" customWidth="1"/>
     <col min="5" max="5" width="35.375" customWidth="1"/>
-    <col min="6" max="6" width="26.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.75" customWidth="1"/>
     <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9958,10 +9593,10 @@
         <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -9975,87 +9610,107 @@
     </row>
     <row r="3" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="24" t="s">
         <v>59</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>167</v>
+        <v>245</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>235</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>168</v>
+        <v>236</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
+        <v>64</v>
+      </c>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
       <c r="D4" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" s="30"/>
+        <v>246</v>
+      </c>
+      <c r="E4" s="28"/>
       <c r="F4" s="2" t="s">
-        <v>170</v>
+        <v>237</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
+        <v>65</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
       <c r="D5" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="31"/>
+        <v>247</v>
+      </c>
+      <c r="E5" s="28"/>
       <c r="F5" s="2" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" s="13" customFormat="1" ht="142.5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" s="13" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="11" t="s">
-        <v>188</v>
+        <v>238</v>
       </c>
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
       <c r="D6" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="E6" s="32" t="s">
-        <v>194</v>
-      </c>
+        <v>248</v>
+      </c>
+      <c r="E6" s="29"/>
       <c r="F6" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+        <v>239</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" spans="1:8" s="13" customFormat="1" ht="99.75" x14ac:dyDescent="0.15">
+      <c r="A7" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="H7" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="E3:E6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update the test case file
</commit_message>
<xml_diff>
--- a/src/MyItems/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Test Cases for FileOperation.xlsx
@@ -4,26 +4,25 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
-    <sheet name="2.删除文件夹" sheetId="1" r:id="rId2"/>
-    <sheet name="3.复制文件夹到文件夹" sheetId="3" r:id="rId3"/>
-    <sheet name="4.移动文件或文件夹到文件夹" sheetId="7" r:id="rId4"/>
-    <sheet name="5.在Txt文件内查找指定内容" sheetId="8" r:id="rId5"/>
+    <sheet name="2.删除文件" sheetId="1" r:id="rId2"/>
+    <sheet name="3.复制文件" sheetId="3" r:id="rId3"/>
+    <sheet name="4.移动文件" sheetId="7" r:id="rId4"/>
+    <sheet name="5.在Txt文件内搜索" sheetId="8" r:id="rId5"/>
     <sheet name="6.在文件夹中查找文件" sheetId="9" r:id="rId6"/>
     <sheet name="7.重命名文件夹" sheetId="10" r:id="rId7"/>
-    <sheet name="8.重命名文件" sheetId="12" r:id="rId8"/>
-    <sheet name="9.根据文件已有字段被替换为新名称" sheetId="13" r:id="rId9"/>
-    <sheet name="10.特殊字符测试" sheetId="15" r:id="rId10"/>
+    <sheet name="8.根据文件已有字段被替换为新名称" sheetId="13" r:id="rId8"/>
+    <sheet name="9.特殊字符测试" sheetId="15" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="252">
   <si>
     <t>Test Case 001</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2111,10 +2110,6 @@
       </rPr>
       <t>）</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>测试数据</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2706,66 +2701,6 @@
   </si>
   <si>
     <r>
-      <t>1.显示这是个非文件夹，提示有错误信息 （</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>This is a folder not a file,cannot be renamed here</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.文件重命名失败</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.显示这是个非文件夹，提示有错误信息 （</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>This is a file not a folder,cannot be renamed here</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.文件夹重命名失败</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>1.在"</t>
     </r>
     <r>
@@ -4928,8 +4863,501 @@
   </si>
   <si>
     <r>
+      <t>1.显示需要被更改名字的文件夹不存在（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\Honda is not exists!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.文件夹不应被重命名成功</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test case 056</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示需要更改的文件夹已经存在（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test4 has already exists, can not be renamed!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.文件夹不应被重命名成功</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test Case 057</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>原来的文件名字
+2.输入替换的文件名字</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>不存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>原来的文件名字
+2.输入替换的文件名字</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>非文件</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的名字，而输入文件夹名字
+2.输入替换的文件名字</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">
-1.在"</t>
+1.输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>原来的文件夹名字
+2.输入替换的文件夹名字</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>不存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>原来的文件夹名字
+2.输入替换的文件夹名字</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>不存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹路径
+2.输入替换的文件夹名字</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>原来的文件夹名字
+2.输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的替换</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的文件夹名字</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>非文件夹</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的名字，而输入文件名字
+3.输入替换的文件夹名字</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示需要被更改名字的文件不存在（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\ALO.bmp is not exists!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.文件不应被重命名成功</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>不存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的路径名字
+2.输入替换的文件名字</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示目标文件夹路径不存在
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\AAA\111.TXT is not exists!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.文件不应被重命名成功</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入该路径下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>原来的文件名字
+2.输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的替换</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的文件名字</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
     </r>
     <r>
       <rPr>
@@ -4964,7 +5392,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>D:\TesT39</t>
+      <t>D:\Test</t>
     </r>
     <r>
       <rPr>
@@ -5011,55 +5439,25 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Test4</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.显示指定的文件夹名已被换成新命名的名字（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\TesT39 has been renamed as D:\Test4 successfully!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.在本地计算机中能够查看到新命名的文件夹</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.显示需要被更改名字的文件夹不存在（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\Honda is not exists!</t>
+      <t>Test2</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示需要更改的文件夹已经存在（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\Alonso.accdb has already exists, can not be renamed!</t>
     </r>
     <r>
       <rPr>
@@ -5076,795 +5474,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Test case 056</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.显示需要更改的文件夹已经存在（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test4 has already exists, can not be renamed!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.文件夹不应被重命名成功</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Input your folder name:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\Alonso.txt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please Input what words you want to replace:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入新的想要被替换的文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test Case 057</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.输入该路径下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>原来的文件名字
-2.输入替换的文件名字</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.输入该路径下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>不存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>原来的文件名字
-2.输入替换的文件名字</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.输入该路径下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>非文件</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>的名字，而输入文件夹名字
-2.输入替换的文件名字</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">
-1.输入该路径下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>原来的文件夹名字
-2.输入替换的文件夹名字</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.输入该路径下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>不存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>原来的文件夹名字
-2.输入替换的文件夹名字</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.输入</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>不存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹路径
-2.输入替换的文件夹名字</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.输入该路径下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>原来的文件夹名字
-2.输入</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的替换</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>的文件夹名字</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.输入该路径下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>非文件夹</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>的名字，而输入文件名字
-3.输入替换的文件夹名字</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">
-1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Input your file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件路径，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\ALO.bmp</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please Input what words you want to replace:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入新的想要被替换的文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>BUT.txt</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.显示需要被更改名字的文件不存在（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\ALO.bmp is not exists!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.文件不应被重命名成功</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.输入</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>不存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>的路径名字
-2.输入替换的文件名字</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.显示目标文件夹路径不存在
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\AAA\111.TXT is not exists!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.文件不应被重命名成功</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.输入该路径下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>原来的文件名字
-2.输入</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的替换</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>的文件名字</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pass</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pass</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.显示指定的文件名已被换成新命名的名字（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\ALO.bmp has been renamed as D:\Test\BUT.txt successfully!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.在本地计算机中能够查看到新命名的文件</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Input your folder name:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please Input what words you want to replace:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入新的想要被替换的文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test2</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.显示需要更改的文件夹已经存在（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\Alonso.accdb has already exists, can not be renamed!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.文件夹不应被重命名成功</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2. Delete Folders or Files</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -5902,18 +5511,6 @@
   </si>
   <si>
     <t>6. Find Files on Folder</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7. Rename Folder</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8. Rename File</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>9. Replace File Name With SpecificName</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -6838,6 +6435,352 @@
       </rPr>
       <t>）</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Input your file or folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\TesT39</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please Input what words you want to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test4</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Input your file or folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\Alonso.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please Input what words you want to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Input your file or folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\ALO.bmp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please Input what words you want to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BUT.txt</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示指定的文件夹名已被换成新命名的名字（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\TesT39 has been renamed as D:\Test4 successfully!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.在本地计算机中能够查看到新命名的文件夹</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示指定的文件名已被换成新命名的名字（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\ALO.bmp has been renamed as D:\Test\BUT.txt successfully!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.在本地计算机中能够查看到新命名的文件</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>模块，合并，该测试用例或无效</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>模块，合并，该测试用例或无效</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7. Rename File or Folder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7. Rename File or Folder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8. Replace File Name With SpecificName</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -7515,7 +7458,7 @@
         <v>60</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>62</v>
@@ -7604,160 +7547,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.625" customWidth="1"/>
-    <col min="6" max="6" width="29" customWidth="1"/>
-    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="F4" s="24"/>
-      <c r="G4" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F5" s="24"/>
-      <c r="G5" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" ht="114" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F6" s="24"/>
-      <c r="G6" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" ht="57" x14ac:dyDescent="0.15">
-      <c r="A7" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="H7" s="5"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C3:C7"/>
-    <mergeCell ref="F3:F7"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7826,13 +7615,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>130</v>
@@ -7852,16 +7641,16 @@
         <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>132</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
@@ -7874,7 +7663,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>131</v>
@@ -7930,13 +7719,13 @@
         <v>8</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>132</v>
@@ -7957,16 +7746,16 @@
         <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>130</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="I10" s="3"/>
     </row>
@@ -7980,7 +7769,7 @@
         <v>16</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>133</v>
@@ -8106,8 +7895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="E4" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8165,16 +7954,16 @@
         <v>17</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>79</v>
@@ -8190,11 +7979,11 @@
       <c r="B4" s="29"/>
       <c r="C4" s="29"/>
       <c r="D4" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>91</v>
@@ -8208,11 +7997,11 @@
       <c r="B5" s="29"/>
       <c r="C5" s="29"/>
       <c r="D5" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="2" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>79</v>
@@ -8228,11 +8017,11 @@
       <c r="B6" s="29"/>
       <c r="C6" s="29"/>
       <c r="D6" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="2" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>90</v>
@@ -8246,19 +8035,19 @@
       <c r="B7" s="29"/>
       <c r="C7" s="29"/>
       <c r="D7" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>90</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>224</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="13" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
@@ -8268,13 +8057,13 @@
       <c r="B8" s="29"/>
       <c r="C8" s="29"/>
       <c r="D8" s="11" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="G8" s="16" t="s">
         <v>100</v>
@@ -8315,16 +8104,16 @@
         <v>22</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="G13" s="15" t="s">
         <v>79</v>
@@ -8338,11 +8127,11 @@
       <c r="B14" s="24"/>
       <c r="C14" s="24"/>
       <c r="D14" s="15" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E14" s="27"/>
       <c r="F14" s="15" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="G14" s="15" t="s">
         <v>79</v>
@@ -8356,11 +8145,11 @@
       <c r="B15" s="24"/>
       <c r="C15" s="24"/>
       <c r="D15" s="15" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E15" s="27"/>
       <c r="F15" s="15" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="G15" s="15" t="s">
         <v>79</v>
@@ -8374,11 +8163,11 @@
       <c r="B16" s="24"/>
       <c r="C16" s="24"/>
       <c r="D16" s="15" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E16" s="28"/>
       <c r="F16" s="15" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="G16" s="15" t="s">
         <v>79</v>
@@ -8392,19 +8181,19 @@
       <c r="B17" s="24"/>
       <c r="C17" s="24"/>
       <c r="D17" s="15" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G17" s="15" t="s">
         <v>79</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
@@ -8414,13 +8203,13 @@
       <c r="B18" s="25"/>
       <c r="C18" s="25"/>
       <c r="D18" s="11" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="G18" s="16" t="s">
         <v>79</v>
@@ -8453,7 +8242,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C3" sqref="C3:C12"/>
     </sheetView>
   </sheetViews>
@@ -8502,16 +8291,16 @@
         <v>30</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>96</v>
@@ -8525,11 +8314,11 @@
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
       <c r="D4" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>97</v>
@@ -8543,11 +8332,11 @@
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
       <c r="D5" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>95</v>
@@ -8561,11 +8350,11 @@
       <c r="B6" s="24"/>
       <c r="C6" s="24"/>
       <c r="D6" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E6" s="27"/>
       <c r="F6" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>95</v>
@@ -8574,22 +8363,22 @@
     </row>
     <row r="7" spans="1:8" s="13" customFormat="1" ht="156.75" x14ac:dyDescent="0.15">
       <c r="A7" s="11" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B7" s="24"/>
       <c r="C7" s="24"/>
       <c r="D7" s="11" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E7" s="28"/>
       <c r="F7" s="11" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
@@ -8599,13 +8388,13 @@
       <c r="B8" s="24"/>
       <c r="C8" s="24"/>
       <c r="D8" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>79</v>
@@ -8619,11 +8408,11 @@
       <c r="B9" s="24"/>
       <c r="C9" s="24"/>
       <c r="D9" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E9" s="27"/>
       <c r="F9" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>79</v>
@@ -8637,11 +8426,11 @@
       <c r="B10" s="24"/>
       <c r="C10" s="24"/>
       <c r="D10" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E10" s="27"/>
       <c r="F10" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>79</v>
@@ -8655,11 +8444,11 @@
       <c r="B11" s="24"/>
       <c r="C11" s="24"/>
       <c r="D11" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E11" s="27"/>
       <c r="F11" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>79</v>
@@ -8673,17 +8462,17 @@
       <c r="B12" s="25"/>
       <c r="C12" s="25"/>
       <c r="D12" s="11" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E12" s="28"/>
       <c r="F12" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="G12" s="12" t="s">
-        <v>196</v>
-      </c>
       <c r="H12" s="17" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -8754,13 +8543,13 @@
         <v>38</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>40</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>138</v>
@@ -8916,7 +8705,7 @@
         <v>43</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>47</v>
@@ -8990,10 +8779,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H7"/>
+  <dimension ref="A2:H15"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9005,6 +8794,7 @@
     <col min="5" max="5" width="35.375" customWidth="1"/>
     <col min="6" max="6" width="30.75" customWidth="1"/>
     <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
@@ -9041,16 +8831,16 @@
         <v>51</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>232</v>
+        <v>249</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>197</v>
+        <v>242</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>198</v>
+        <v>245</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>83</v>
@@ -9064,11 +8854,11 @@
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
       <c r="D4" s="2" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>81</v>
@@ -9082,7 +8872,7 @@
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
       <c r="D5" s="2" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="2" t="s">
@@ -9095,47 +8885,178 @@
     </row>
     <row r="6" spans="1:8" s="13" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="11" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B6" s="24"/>
       <c r="C6" s="24"/>
       <c r="D6" s="11" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="11" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="H6" s="11"/>
     </row>
-    <row r="7" spans="1:8" s="13" customFormat="1" ht="99.75" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" s="13" customFormat="1" ht="114" x14ac:dyDescent="0.15">
       <c r="A7" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>
       <c r="D7" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="G7" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="E7" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="H7" s="12"/>
+      <c r="H7" s="12" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="114" x14ac:dyDescent="0.15">
+      <c r="A11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>250</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>244</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
+      <c r="A12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E12" s="27"/>
+      <c r="F12" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
+      <c r="A13" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E13" s="27"/>
+      <c r="F13" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
+      <c r="A14" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="E14" s="28"/>
+      <c r="F14" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="H14" s="11"/>
+    </row>
+    <row r="15" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
+      <c r="A15" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>248</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="C3:C7"/>
     <mergeCell ref="E3:E6"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="E11:E14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9145,172 +9066,17 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H7"/>
-  <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.5" customWidth="1"/>
-    <col min="5" max="5" width="45.5" customWidth="1"/>
-    <col min="6" max="6" width="27.125" customWidth="1"/>
-    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>233</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>212</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="E4" s="27"/>
-      <c r="F4" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E5" s="27"/>
-      <c r="F5" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" s="13" customFormat="1" ht="99.75" x14ac:dyDescent="0.15">
-      <c r="A6" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>218</v>
-      </c>
-      <c r="H6" s="11"/>
-    </row>
-    <row r="7" spans="1:8" s="13" customFormat="1" ht="99.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>220</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="H7" s="12"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C3:C7"/>
-    <mergeCell ref="E3:E6"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.25" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="40.25" customWidth="1"/>
     <col min="6" max="6" width="28.75" customWidth="1"/>
     <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
@@ -9351,16 +9117,16 @@
         <v>58</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>234</v>
+        <v>251</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>146</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>79</v>
@@ -9378,7 +9144,7 @@
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>88</v>
@@ -9398,7 +9164,7 @@
       </c>
       <c r="E5" s="28"/>
       <c r="F5" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>81</v>
@@ -9422,4 +9188,158 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.625" customWidth="1"/>
+    <col min="6" max="6" width="29" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F4" s="24"/>
+      <c r="G4" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F5" s="24"/>
+      <c r="G5" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" ht="114" x14ac:dyDescent="0.15">
+      <c r="A6" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F6" s="24"/>
+      <c r="G6" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" ht="57" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F7" s="25"/>
+      <c r="G7" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="F3:F7"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update the test case file on the afternoon of 1th,June
</commit_message>
<xml_diff>
--- a/src/MyItems/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="251">
   <si>
     <t>Test Case 001</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -5474,14 +5474,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2. Delete Folders or Files</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2. Delete Folders or Files</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>模块，合并，该测试用例或无效</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -5490,19 +5482,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3. Copy Files or Folder to Folder</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3. Copy Files or Folder to Folder</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1. Replace Content on txt files</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4. Move Folder or files to Folder</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -6781,6 +6761,22 @@
   </si>
   <si>
     <t>8. Replace File Name With SpecificName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. Delete File or Folder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. Copy File or Folder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. Copy File or Folder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. Move File or Folder</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -7399,7 +7395,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C6"/>
+      <selection activeCell="B3" sqref="B3:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7409,7 +7405,7 @@
     <col min="3" max="3" width="23.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.25" customWidth="1"/>
     <col min="5" max="5" width="34.875" customWidth="1"/>
-    <col min="6" max="6" width="26.5" customWidth="1"/>
+    <col min="6" max="6" width="32.5" customWidth="1"/>
     <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.375" bestFit="1" customWidth="1"/>
   </cols>
@@ -7458,7 +7454,7 @@
         <v>60</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>62</v>
@@ -7510,7 +7506,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>64</v>
       </c>
@@ -7554,8 +7550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -7615,13 +7611,13 @@
         <v>2</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>214</v>
+        <v>247</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>130</v>
@@ -7641,16 +7637,16 @@
         <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>132</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
@@ -7663,7 +7659,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>131</v>
@@ -7719,13 +7715,13 @@
         <v>8</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>215</v>
+        <v>247</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>132</v>
@@ -7746,16 +7742,16 @@
         <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>130</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="I10" s="3"/>
     </row>
@@ -7769,7 +7765,7 @@
         <v>16</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>133</v>
@@ -7895,8 +7891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView topLeftCell="E4" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7954,16 +7950,16 @@
         <v>17</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>218</v>
+        <v>249</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>156</v>
       </c>
       <c r="E3" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>227</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>232</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>79</v>
@@ -7983,7 +7979,7 @@
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>91</v>
@@ -8001,7 +7997,7 @@
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="2" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>79</v>
@@ -8021,7 +8017,7 @@
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="2" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>90</v>
@@ -8038,16 +8034,16 @@
         <v>160</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>90</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="13" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
@@ -8060,10 +8056,10 @@
         <v>161</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="G8" s="16" t="s">
         <v>100</v>
@@ -8104,16 +8100,16 @@
         <v>22</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>219</v>
+        <v>248</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>163</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="G13" s="15" t="s">
         <v>79</v>
@@ -8131,7 +8127,7 @@
       </c>
       <c r="E14" s="27"/>
       <c r="F14" s="15" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="G14" s="15" t="s">
         <v>79</v>
@@ -8149,7 +8145,7 @@
       </c>
       <c r="E15" s="27"/>
       <c r="F15" s="15" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="G15" s="15" t="s">
         <v>79</v>
@@ -8167,7 +8163,7 @@
       </c>
       <c r="E16" s="28"/>
       <c r="F16" s="15" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="G16" s="15" t="s">
         <v>79</v>
@@ -8184,7 +8180,7 @@
         <v>167</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="F17" s="15" t="s">
         <v>162</v>
@@ -8193,7 +8189,7 @@
         <v>79</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
@@ -8206,10 +8202,10 @@
         <v>168</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="G18" s="16" t="s">
         <v>79</v>
@@ -8242,8 +8238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H12"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C12"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8291,7 +8287,7 @@
         <v>30</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>221</v>
+        <v>250</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>178</v>
@@ -8543,7 +8539,7 @@
         <v>38</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>40</v>
@@ -8705,7 +8701,7 @@
         <v>43</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>47</v>
@@ -8831,16 +8827,16 @@
         <v>51</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>201</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>83</v>
@@ -8911,16 +8907,16 @@
         <v>205</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>211</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
@@ -8957,16 +8953,16 @@
         <v>52</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>198</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>79</v>
@@ -9040,13 +9036,13 @@
         <v>212</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>79</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -9117,7 +9113,7 @@
         <v>58</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>144</v>

</xml_diff>

<commit_message>
Update the test case file again on the afternoon of 1th,June
</commit_message>
<xml_diff>
--- a/src/MyItems/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="253">
   <si>
     <t>Test Case 001</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1667,36 +1667,6 @@
   </si>
   <si>
     <r>
-      <t>1.有显示该文件夹被删除的消息 (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The contents of folder: D:\Test1\cCc have been deleted succeeded!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)
-2.本地计算机上该文件夹确实被删除</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>1.显示该文件夹路径不存在，有错误提示信息（</t>
     </r>
     <r>
@@ -1722,36 +1692,6 @@
       </rPr>
       <t>）
 2.文件夹删除失败</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.有显示该文件被删除的消息（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The file: D:\Test1\456.txt have been deleted succeeded!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）        
-2.本地计算机上该文件确实被删除</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -6777,6 +6717,126 @@
   </si>
   <si>
     <t>4. Move File or Folder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.有显示该文件被删除的消息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test1\456.txt has been deleted succeeded!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）        
+2.本地计算机上该文件确实被删除</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.有显示该文件夹被删除的消息 (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test1\cCc has been deleted succeeded!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)
+2.本地计算机上该文件夹确实被删除</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.有显示该文件被删除的消息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> D:\Test1\456.txt has been deleted succeeded!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）        
+2.本地计算机上该文件确实被删除</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.有显示该文件夹被删除的消息 (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> D:\Test1\cCc has been deleted succeeded!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)
+2.本地计算机上该文件夹确实被删除</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -7454,7 +7514,7 @@
         <v>60</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>62</v>
@@ -7550,8 +7610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -7603,7 +7663,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="85.5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>65</v>
       </c>
@@ -7611,16 +7671,16 @@
         <v>2</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>130</v>
+        <v>250</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>84</v>
@@ -7637,16 +7697,16 @@
         <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>132</v>
+        <v>249</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
@@ -7659,10 +7719,10 @@
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>84</v>
@@ -7715,16 +7775,16 @@
         <v>8</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>132</v>
+        <v>251</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>79</v>
@@ -7732,7 +7792,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="85.5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>69</v>
       </c>
@@ -7742,16 +7802,16 @@
         <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>130</v>
+        <v>252</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I10" s="3"/>
     </row>
@@ -7765,10 +7825,10 @@
         <v>16</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>79</v>
@@ -7950,16 +8010,16 @@
         <v>17</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>79</v>
@@ -7975,11 +8035,11 @@
       <c r="B4" s="29"/>
       <c r="C4" s="29"/>
       <c r="D4" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>91</v>
@@ -7993,11 +8053,11 @@
       <c r="B5" s="29"/>
       <c r="C5" s="29"/>
       <c r="D5" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>79</v>
@@ -8013,11 +8073,11 @@
       <c r="B6" s="29"/>
       <c r="C6" s="29"/>
       <c r="D6" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>90</v>
@@ -8031,19 +8091,19 @@
       <c r="B7" s="29"/>
       <c r="C7" s="29"/>
       <c r="D7" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>90</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="13" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
@@ -8053,13 +8113,13 @@
       <c r="B8" s="29"/>
       <c r="C8" s="29"/>
       <c r="D8" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G8" s="16" t="s">
         <v>100</v>
@@ -8100,16 +8160,16 @@
         <v>22</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G13" s="15" t="s">
         <v>79</v>
@@ -8123,11 +8183,11 @@
       <c r="B14" s="24"/>
       <c r="C14" s="24"/>
       <c r="D14" s="15" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E14" s="27"/>
       <c r="F14" s="15" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G14" s="15" t="s">
         <v>79</v>
@@ -8141,11 +8201,11 @@
       <c r="B15" s="24"/>
       <c r="C15" s="24"/>
       <c r="D15" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E15" s="27"/>
       <c r="F15" s="15" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G15" s="15" t="s">
         <v>79</v>
@@ -8159,11 +8219,11 @@
       <c r="B16" s="24"/>
       <c r="C16" s="24"/>
       <c r="D16" s="15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E16" s="28"/>
       <c r="F16" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G16" s="15" t="s">
         <v>79</v>
@@ -8177,19 +8237,19 @@
       <c r="B17" s="24"/>
       <c r="C17" s="24"/>
       <c r="D17" s="15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G17" s="15" t="s">
         <v>79</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
@@ -8199,13 +8259,13 @@
       <c r="B18" s="25"/>
       <c r="C18" s="25"/>
       <c r="D18" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G18" s="16" t="s">
         <v>79</v>
@@ -8287,16 +8347,16 @@
         <v>30</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>96</v>
@@ -8310,11 +8370,11 @@
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
       <c r="D4" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>97</v>
@@ -8328,11 +8388,11 @@
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
       <c r="D5" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>95</v>
@@ -8346,11 +8406,11 @@
       <c r="B6" s="24"/>
       <c r="C6" s="24"/>
       <c r="D6" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E6" s="27"/>
       <c r="F6" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>95</v>
@@ -8359,22 +8419,22 @@
     </row>
     <row r="7" spans="1:8" s="13" customFormat="1" ht="156.75" x14ac:dyDescent="0.15">
       <c r="A7" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B7" s="24"/>
       <c r="C7" s="24"/>
       <c r="D7" s="11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E7" s="28"/>
       <c r="F7" s="11" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
@@ -8384,13 +8444,13 @@
       <c r="B8" s="24"/>
       <c r="C8" s="24"/>
       <c r="D8" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>79</v>
@@ -8404,11 +8464,11 @@
       <c r="B9" s="24"/>
       <c r="C9" s="24"/>
       <c r="D9" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E9" s="27"/>
       <c r="F9" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>79</v>
@@ -8422,11 +8482,11 @@
       <c r="B10" s="24"/>
       <c r="C10" s="24"/>
       <c r="D10" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E10" s="27"/>
       <c r="F10" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>79</v>
@@ -8440,11 +8500,11 @@
       <c r="B11" s="24"/>
       <c r="C11" s="24"/>
       <c r="D11" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E11" s="27"/>
       <c r="F11" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>79</v>
@@ -8458,17 +8518,17 @@
       <c r="B12" s="25"/>
       <c r="C12" s="25"/>
       <c r="D12" s="11" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E12" s="28"/>
       <c r="F12" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="H12" s="17" t="s">
         <v>190</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -8539,16 +8599,16 @@
         <v>38</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>40</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>106</v>
@@ -8569,7 +8629,7 @@
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>88</v>
@@ -8592,7 +8652,7 @@
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>80</v>
@@ -8611,7 +8671,7 @@
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>88</v>
@@ -8701,16 +8761,16 @@
         <v>43</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>47</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>79</v>
@@ -8728,7 +8788,7 @@
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>88</v>
@@ -8748,7 +8808,7 @@
       </c>
       <c r="E5" s="28"/>
       <c r="F5" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>79</v>
@@ -8777,7 +8837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -8827,16 +8887,16 @@
         <v>51</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>83</v>
@@ -8850,11 +8910,11 @@
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
       <c r="D4" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>81</v>
@@ -8868,11 +8928,11 @@
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
       <c r="D5" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>82</v>
@@ -8881,42 +8941,42 @@
     </row>
     <row r="6" spans="1:8" s="13" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="11" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B6" s="24"/>
       <c r="C6" s="24"/>
       <c r="D6" s="11" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="11" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:8" s="13" customFormat="1" ht="114" x14ac:dyDescent="0.15">
       <c r="A7" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>
       <c r="D7" s="11" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F7" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="H7" s="12" t="s">
         <v>241</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
@@ -8953,16 +9013,16 @@
         <v>52</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E11" s="26" t="s">
+        <v>237</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>241</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>79</v>
@@ -8976,11 +9036,11 @@
       <c r="B12" s="24"/>
       <c r="C12" s="24"/>
       <c r="D12" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E12" s="27"/>
       <c r="F12" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>79</v>
@@ -8994,11 +9054,11 @@
       <c r="B13" s="24"/>
       <c r="C13" s="24"/>
       <c r="D13" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E13" s="27"/>
       <c r="F13" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>79</v>
@@ -9007,16 +9067,16 @@
     </row>
     <row r="14" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A14" s="11" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B14" s="24"/>
       <c r="C14" s="24"/>
       <c r="D14" s="11" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E14" s="28"/>
       <c r="F14" s="11" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>79</v>
@@ -9025,24 +9085,24 @@
     </row>
     <row r="15" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A15" s="11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B15" s="25"/>
       <c r="C15" s="25"/>
       <c r="D15" s="11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>79</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -9113,16 +9173,16 @@
         <v>58</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E3" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>79</v>
@@ -9140,7 +9200,7 @@
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>88</v>
@@ -9160,7 +9220,7 @@
       </c>
       <c r="E5" s="28"/>
       <c r="F5" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>81</v>
@@ -9246,7 +9306,7 @@
         <v>112</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F3" s="23" t="s">
         <v>117</v>
@@ -9266,7 +9326,7 @@
         <v>113</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F4" s="24"/>
       <c r="G4" s="2" t="s">
@@ -9284,7 +9344,7 @@
         <v>114</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F5" s="24"/>
       <c r="G5" s="2" t="s">
@@ -9302,7 +9362,7 @@
         <v>116</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F6" s="24"/>
       <c r="G6" s="5" t="s">
@@ -9320,7 +9380,7 @@
         <v>119</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="5" t="s">

</xml_diff>

<commit_message>
Update the test case file on 5pm on 1th,June
</commit_message>
<xml_diff>
--- a/src/MyItems/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -1566,66 +1566,6 @@
   <si>
     <r>
       <t>1. 能够出现提示输入的信息
-2. 提示查找的文件夹路径不存在(</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>This folder path not exist!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1. 能够出现提示输入的信息
-2. 显示该文件夹下不存在txt文件 (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>There is no txt files under folder:文件夹路径</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1. 能够出现提示输入的信息
 2. 显示指定的内容已经被查到，并替换成功，并能够在本地文件中查看到替换之处，如测试数据所示，应将</t>
     </r>
     <r>
@@ -1662,66 +1602,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>Alonso</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.显示该文件夹路径不存在，有错误提示信息（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>This folder path not exist!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.文件夹删除失败</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.显示该文件路径不存在，有错误提示信息（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>This file path not exist!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.文件删除失败</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1758,36 +1638,6 @@
   <si>
     <r>
       <t>1. 能够出现提示输入的信息
-2.提示查找的文件夹路径不存在(</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test not exists!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1. 能够出现提示输入的信息
 2.显示该文件夹下不存在txt文件（</t>
     </r>
     <r>
@@ -1935,36 +1785,6 @@
   </si>
   <si>
     <r>
-      <t>1.显示目标文件夹路径不存在（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test3\Test5 is not exists!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.文件夹不应被重命名成功</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>1.能够出现提示输入的信息
 2.显示指定文件被找到的信息（</t>
     </r>
@@ -2008,36 +1828,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>File: 9888.png didn't found on D:\Test1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.能够出现提示输入的信息
-2.显示该文件夹不存在的信息（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test1 not exists!</t>
     </r>
     <r>
       <rPr>
@@ -2343,36 +2133,6 @@
   </si>
   <si>
     <r>
-      <t>1. 显示指定的文件夹路径不存在 （</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Target Folder path: D:\Test1 is not exists!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2. 重命名失败</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>在需要输入文件夹或者文件的提示框内，输入如：</t>
     </r>
     <r>
@@ -3715,36 +3475,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>1.显示需要被移动的文件路径不存在（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\Alonso.txt is not exists!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.文件移动失败</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Test Case 046</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3775,66 +3505,6 @@
       </rPr>
       <t>）
 2.本地计算机中能查到新文件夹路径</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.显示需要被移动的文件夹路径不存在（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test is not exists!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.文件移动失败</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.显示需要被移动的文件路径不存在（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E:\Program Files\Test\Test is not exists!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.文件移动失败</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -5954,36 +5624,6 @@
   </si>
   <si>
     <r>
-      <t>1.显示被复制的文件夹路径不存在（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>source File or Folder: D:\Test129 is NOT Exist!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.文件夹不应被复制到指定路径</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>1.新创建目标文件夹
 2.文件夹复制到新创建的指定路径，且目录下包含原名称的子文件夹（</t>
     </r>
@@ -6009,35 +5649,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.显示被复制的文件夹路径不存在 （</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>source File or Folder: D:\TTTTTT is NOT Exist!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.文件夹不应该被复制到指定路径</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -6074,36 +5685,6 @@
   </si>
   <si>
     <r>
-      <t>1.显示被复制的文件路径不存在（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>source File or Folder: D:\Test\Alo.txt is NOT Exist!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.文件不应被复制到指定路径</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>1.新建目标文件夹路径
 2.显示文件复制到了新建路径（</t>
     </r>
@@ -6134,36 +5715,6 @@
   </si>
   <si>
     <r>
-      <t>1.显示被复制的文件路径不存在（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>source File or Folder: D:\Test\Ric.txt is NOT Exist!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.文件不应该被复制到指定路径</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">
 1.在"</t>
     </r>
@@ -6551,36 +6102,6 @@
       </rPr>
       <t>）        
 2.本地计算机上该文件确实被删除</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.有显示该文件夹被删除的消息 (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test1\cCc has been deleted succeeded!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)
-2.本地计算机上该文件夹确实被删除</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -6836,6 +6357,508 @@
       <t>）
 2.若选择覆盖后，原有文件夹应被移动替换为新的文件夹路径 
 3.本地计算机中能查到新文件路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.有显示该文件夹被删除的消息 (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test1\cCc has been deleted succeeded!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)
+2.本地计算机上该文件夹确实被删除</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示该文件夹路径不存在，有错误提示信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test1\cCc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>is NOT Exist!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.文件夹删除失败</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示该文件路径不存在，有错误提示信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test1\456.txt is NOT Exist!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.文件删除失败</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 能够出现提示输入的信息
+2. 显示该文件夹下不存在txt文件 (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>There is no txt files under folder:文件夹路径</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 能够出现提示输入的信息
+2. 提示查找的文件夹路径不存在(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test is NOT Exist!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示被复制的文件夹路径不存在 （</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test is NOT Exist!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.文件夹不应该被复制到指定路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示被复制的文件路径不存在（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\123.txt is NOT Exist!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.文件不应该被复制到指定路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示被复制的文件路径不存在（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\123.txt is NOT Exist!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.文件不应被复制到指定路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示被复制的文件夹路径不存在（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test is NOT Exist!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.文件夹不应被复制到指定路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示需要被移动的文件路径不存在（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\Alonso.txt is NOT exists!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.文件移动失败</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示需要被移动的文件路径不存在（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\Program Files\Test\Test is NOT exists!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.文件移动失败</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示需要被移动的文件夹路径不存在（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test is NOT exists!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.文件移动失败</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 能够出现提示输入的信息
+2.提示查找的文件夹路径不存在(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test is NOT exists!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.能够出现提示输入的信息
+2.显示该文件夹不存在的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test1 is NOT exist!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示目标文件夹路径不存在（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test3\Test5 is NOT exist!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.文件夹不应被重命名成功</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 显示指定的文件夹路径不存在 （</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test1 is NOT exist!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2. 重命名失败</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -7455,7 +7478,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7514,7 +7537,7 @@
         <v>60</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>62</v>
@@ -7523,7 +7546,7 @@
         <v>125</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>80</v>
@@ -7548,7 +7571,7 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -7559,7 +7582,7 @@
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="2" t="s">
-        <v>127</v>
+        <v>241</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>82</v>
@@ -7577,7 +7600,7 @@
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="2" t="s">
-        <v>128</v>
+        <v>240</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>88</v>
@@ -7610,8 +7633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -7671,16 +7694,16 @@
         <v>2</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>84</v>
@@ -7697,16 +7720,16 @@
         <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
@@ -7719,10 +7742,10 @@
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>130</v>
+        <v>238</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>84</v>
@@ -7775,16 +7798,16 @@
         <v>8</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>79</v>
@@ -7802,16 +7825,16 @@
         <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="I10" s="3"/>
     </row>
@@ -7825,10 +7848,10 @@
         <v>16</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>131</v>
+        <v>239</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>79</v>
@@ -7951,8 +7974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8010,16 +8033,16 @@
         <v>17</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>79</v>
@@ -8028,18 +8051,18 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="29"/>
       <c r="C4" s="29"/>
       <c r="D4" s="2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>224</v>
+        <v>245</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>91</v>
@@ -8053,11 +8076,11 @@
       <c r="B5" s="29"/>
       <c r="C5" s="29"/>
       <c r="D5" s="2" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="2" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>79</v>
@@ -8066,18 +8089,18 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="29"/>
       <c r="C6" s="29"/>
       <c r="D6" s="2" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="2" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>90</v>
@@ -8091,19 +8114,19 @@
       <c r="B7" s="29"/>
       <c r="C7" s="29"/>
       <c r="D7" s="2" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>90</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="13" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
@@ -8113,13 +8136,13 @@
       <c r="B8" s="29"/>
       <c r="C8" s="29"/>
       <c r="D8" s="11" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="G8" s="16" t="s">
         <v>100</v>
@@ -8160,34 +8183,34 @@
         <v>22</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="G13" s="15" t="s">
         <v>79</v>
       </c>
       <c r="H13" s="15"/>
     </row>
-    <row r="14" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A14" s="15" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="24"/>
       <c r="C14" s="24"/>
       <c r="D14" s="15" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="E14" s="27"/>
       <c r="F14" s="15" t="s">
-        <v>228</v>
+        <v>244</v>
       </c>
       <c r="G14" s="15" t="s">
         <v>79</v>
@@ -8201,29 +8224,29 @@
       <c r="B15" s="24"/>
       <c r="C15" s="24"/>
       <c r="D15" s="15" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="E15" s="27"/>
       <c r="F15" s="15" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="G15" s="15" t="s">
         <v>79</v>
       </c>
       <c r="H15" s="15"/>
     </row>
-    <row r="16" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A16" s="15" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="24"/>
       <c r="C16" s="24"/>
       <c r="D16" s="15" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="E16" s="28"/>
       <c r="F16" s="15" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
       <c r="G16" s="15" t="s">
         <v>79</v>
@@ -8237,19 +8260,19 @@
       <c r="B17" s="24"/>
       <c r="C17" s="24"/>
       <c r="D17" s="15" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="G17" s="15" t="s">
         <v>79</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="114" x14ac:dyDescent="0.15">
@@ -8259,13 +8282,13 @@
       <c r="B18" s="25"/>
       <c r="C18" s="25"/>
       <c r="D18" s="11" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="G18" s="16" t="s">
         <v>79</v>
@@ -8299,7 +8322,7 @@
   <dimension ref="A2:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8347,16 +8370,16 @@
         <v>30</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>96</v>
@@ -8370,11 +8393,11 @@
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
       <c r="D4" s="2" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>170</v>
+        <v>246</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>97</v>
@@ -8388,11 +8411,11 @@
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
       <c r="D5" s="2" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="2" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>95</v>
@@ -8406,11 +8429,11 @@
       <c r="B6" s="24"/>
       <c r="C6" s="24"/>
       <c r="D6" s="2" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="E6" s="27"/>
       <c r="F6" s="2" t="s">
-        <v>170</v>
+        <v>246</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>95</v>
@@ -8419,22 +8442,22 @@
     </row>
     <row r="7" spans="1:8" s="13" customFormat="1" ht="156.75" x14ac:dyDescent="0.15">
       <c r="A7" s="11" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B7" s="24"/>
       <c r="C7" s="24"/>
       <c r="D7" s="11" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="E7" s="28"/>
       <c r="F7" s="11" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
@@ -8444,13 +8467,13 @@
       <c r="B8" s="24"/>
       <c r="C8" s="24"/>
       <c r="D8" s="2" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>79</v>
@@ -8464,11 +8487,11 @@
       <c r="B9" s="24"/>
       <c r="C9" s="24"/>
       <c r="D9" s="2" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="E9" s="27"/>
       <c r="F9" s="2" t="s">
-        <v>173</v>
+        <v>248</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>79</v>
@@ -8482,11 +8505,11 @@
       <c r="B10" s="24"/>
       <c r="C10" s="24"/>
       <c r="D10" s="2" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="E10" s="27"/>
       <c r="F10" s="2" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>79</v>
@@ -8500,11 +8523,11 @@
       <c r="B11" s="24"/>
       <c r="C11" s="24"/>
       <c r="D11" s="2" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="E11" s="27"/>
       <c r="F11" s="2" t="s">
-        <v>174</v>
+        <v>247</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>79</v>
@@ -8518,17 +8541,17 @@
       <c r="B12" s="25"/>
       <c r="C12" s="25"/>
       <c r="D12" s="11" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="E12" s="28"/>
       <c r="F12" s="11" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -8549,7 +8572,7 @@
   <dimension ref="A2:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C6"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8559,7 +8582,7 @@
     <col min="3" max="3" width="15.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.5" customWidth="1"/>
     <col min="5" max="5" width="34.25" customWidth="1"/>
-    <col min="6" max="6" width="24.25" customWidth="1"/>
+    <col min="6" max="6" width="34" customWidth="1"/>
     <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.625" customWidth="1"/>
@@ -8599,16 +8622,16 @@
         <v>38</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>40</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>106</v>
@@ -8629,7 +8652,7 @@
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>88</v>
@@ -8641,7 +8664,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="85.5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>44</v>
       </c>
@@ -8652,7 +8675,7 @@
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="2" t="s">
-        <v>133</v>
+        <v>249</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>80</v>
@@ -8671,7 +8694,7 @@
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>88</v>
@@ -8713,7 +8736,7 @@
   <dimension ref="A2:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8761,16 +8784,16 @@
         <v>43</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>47</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>79</v>
@@ -8788,7 +8811,7 @@
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>88</v>
@@ -8808,7 +8831,7 @@
       </c>
       <c r="E5" s="28"/>
       <c r="F5" s="2" t="s">
-        <v>140</v>
+        <v>250</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>79</v>
@@ -8838,7 +8861,7 @@
   <dimension ref="A2:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8887,16 +8910,16 @@
         <v>51</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>83</v>
@@ -8910,11 +8933,11 @@
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
       <c r="D4" s="2" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>81</v>
@@ -8928,11 +8951,11 @@
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
       <c r="D5" s="2" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="2" t="s">
-        <v>137</v>
+        <v>251</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>82</v>
@@ -8941,42 +8964,42 @@
     </row>
     <row r="6" spans="1:8" s="13" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="11" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="B6" s="24"/>
       <c r="C6" s="24"/>
       <c r="D6" s="11" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="11" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:8" s="13" customFormat="1" ht="114" x14ac:dyDescent="0.15">
       <c r="A7" s="11" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>
       <c r="D7" s="11" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
@@ -9013,16 +9036,16 @@
         <v>52</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>79</v>
@@ -9036,11 +9059,11 @@
       <c r="B12" s="24"/>
       <c r="C12" s="24"/>
       <c r="D12" s="2" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="E12" s="27"/>
       <c r="F12" s="2" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>79</v>
@@ -9054,11 +9077,11 @@
       <c r="B13" s="24"/>
       <c r="C13" s="24"/>
       <c r="D13" s="2" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="E13" s="27"/>
       <c r="F13" s="2" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>79</v>
@@ -9067,16 +9090,16 @@
     </row>
     <row r="14" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A14" s="11" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="B14" s="24"/>
       <c r="C14" s="24"/>
       <c r="D14" s="11" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="E14" s="28"/>
       <c r="F14" s="11" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>79</v>
@@ -9085,24 +9108,24 @@
     </row>
     <row r="15" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A15" s="11" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B15" s="25"/>
       <c r="C15" s="25"/>
       <c r="D15" s="11" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>79</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -9124,8 +9147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H8"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9173,16 +9196,16 @@
         <v>58</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>79</v>
@@ -9200,7 +9223,7 @@
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>88</v>
@@ -9220,7 +9243,7 @@
       </c>
       <c r="E5" s="28"/>
       <c r="F5" s="2" t="s">
-        <v>145</v>
+        <v>252</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>81</v>
@@ -9306,7 +9329,7 @@
         <v>112</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F3" s="23" t="s">
         <v>117</v>
@@ -9326,7 +9349,7 @@
         <v>113</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="F4" s="24"/>
       <c r="G4" s="2" t="s">
@@ -9344,7 +9367,7 @@
         <v>114</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="F5" s="24"/>
       <c r="G5" s="2" t="s">
@@ -9362,7 +9385,7 @@
         <v>116</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="F6" s="24"/>
       <c r="G6" s="5" t="s">
@@ -9380,7 +9403,7 @@
         <v>119</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="5" t="s">

</xml_diff>

<commit_message>
Update the test case file on the morning of 2nd,June
</commit_message>
<xml_diff>
--- a/src/MyItems/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="255">
   <si>
     <t>Test Case 001</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -248,10 +248,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>复制文件夹到文件夹</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Test Case 012</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -265,10 +261,6 @@
   </si>
   <si>
     <t>Test Case 015</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>复制文件到文件夹</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1400,141 +1392,6 @@
   </si>
   <si>
     <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please Input your folder Path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please Input what words you want to find:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入txt文件内存在的内容，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Alonso
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please Input what words you want to replace:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入想要替换成的新内容，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alo</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>1. 能够出现提示输入的信息
 2. 显示指定的内容没有被查到，并替换失败（</t>
     </r>
@@ -1667,93 +1524,6 @@
   </si>
   <si>
     <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input your folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What file you want to find on this folder?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入文件名，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>456.txt</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>1. 能够出现提示输入的信息
 2. 显示该内容在查到的txt文件内被查到几次（</t>
     </r>
@@ -1839,141 +1609,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input folder:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What word do you want find?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alonso</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-3.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What word do you want replace?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入新的想要被替换的文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Button</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2401,106 +2036,6 @@
   </si>
   <si>
     <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder path with txt files:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What content you want to find on txt file?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入txt文件内存在的内容，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Alonso
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t/>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>1.找到本地计算机中</t>
     </r>
     <r>
@@ -2849,36 +2384,6 @@
   </si>
   <si>
     <r>
-      <t>1.显示被复制的是文件夹路径，不是文件路径（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>This is a folder NOT a file, if wanna copy a file please back to menu to choose again!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.文件不应该被复制到指定路径</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>1.找到本地计算机中</t>
     </r>
     <r>
@@ -3299,182 +2804,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input sourceFolder or Filepath</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:" 输入被复制文件的路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\Alonso.txt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input Target Folder:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入需要复制到目标文件夹的路径，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E:\Program Files\Test</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input sourceFolder or Filepath</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:" 输入被复制文件的路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input Target Folder:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入需要复制到目标文件夹的路径，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E:\Program Files</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Test Case 046</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4880,94 +4209,6 @@
   </si>
   <si>
     <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Input your folder name:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please Input what words you want to replace:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入新的想要被替换的文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test2</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>1.显示需要更改的文件夹已经存在（</t>
     </r>
     <r>
@@ -5095,499 +4336,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>D:\Test1\456.txt</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please Input your folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"输入文件夹路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test1</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please Input your folder or file Path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入被复制文件夹的路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>please input TargetFolder:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入需要复制到目标文件夹的路径，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E:\Program Files</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please Input your folder or file Path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入被复制文件的路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\Alonso.txt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>please input TargetFolder:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入需要复制到目标文件夹的路径，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E:\Program Files</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please Input your folder or file Path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入被复制文件的路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\Alonso.txt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input Target Folder:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入需要复制到目标文件夹的路径，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E:\Program Files\Test</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please Input your folder or file Path</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入被复制文件的路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input Target Folder:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入需要复制到目标文件夹的路径，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E:\Program Files\Test</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please Input your folder or file Path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入被复制文件的路径，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:D:\Test\Alonso.txt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input Target Folder:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入需要复制到目标文件夹的路径，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E:\Program Files\Test</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -5715,272 +4463,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">
-1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Input your file or folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\TesT39</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please Input what words you want to replace:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入新的想要被替换的文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test4</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Input your file or folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\Alonso.txt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please Input what words you want to replace:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入新的想要被替换的文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">
-1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Input your file or folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件路径，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\ALO.bmp</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please Input what words you want to replace:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入新的想要被替换的文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>BUT.txt</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>1.显示指定的文件夹名已被换成新命名的名字（</t>
     </r>
     <r>
@@ -6859,6 +5341,1596 @@
       </rPr>
       <t>）
 2. 重命名失败</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>复制文件夹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>复制文件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示文件成功被复制到指定路径（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\Alonso.txt has been copied to E:\Program Files successfully!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">）
+2.本地计算机上存在复制后的新文件
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示文件夹成功被复制到指定路径（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test have copied successfully to folder E:\Program Files\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.本地计算机上存在复制后的新路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what word you want to find:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入txt文件内存在的内容，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Alonso
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what word you want to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入想要替换成的新内容，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alo</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"输入文件夹路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test1\456.txt</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"输入文件夹路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test1</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入被复制文件夹的路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入需要复制到目标文件夹的路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\Program Files</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入被复制文件的路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input Target Folder:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入需要复制到目标文件夹的路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\Program Files\Test</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入被复制文件的路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:D:\Test\Alonso.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入需要复制到目标文件夹的路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\Program Files\Test</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入被复制文件的路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\Alonso.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入需要复制到目标文件夹的路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\Program Files\Test</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入被复制文件的路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\Alonso.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入需要复制到目标文件夹的路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\Program Files</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the source folder or file path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:" 输入被复制文件的路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\Alonso.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入需要复制到目标文件夹的路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\Program Files\Test</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the source folder or file path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:" 输入被复制文件的路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入需要复制到目标文件夹的路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\Program Files</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What content you want to find on txt file?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入txt文件内存在的内容，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Alonso
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What file you want to find on this folder?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入文件名，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>456.txt</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\TesT39</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what word you want to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test4</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\Alonso.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what word you want to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\ALO.bmp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what word you want to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BUT.txt</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what word you want to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test2</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What word do you want find?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alonso</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What word do you want replace?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Button</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -7477,8 +7549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7505,19 +7577,19 @@
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -7534,22 +7606,22 @@
         <v>0</v>
       </c>
       <c r="B3" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="23" t="s">
-        <v>201</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="E3" s="26" t="s">
-        <v>125</v>
+        <v>238</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -7560,14 +7632,14 @@
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
       <c r="D4" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -7578,35 +7650,35 @@
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
       <c r="D5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="2" t="s">
-        <v>241</v>
+        <v>222</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
       <c r="D6" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="2" t="s">
-        <v>240</v>
+        <v>221</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
@@ -7633,8 +7705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -7668,13 +7740,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -7688,31 +7760,31 @@
     </row>
     <row r="3" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B3" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>226</v>
+        <v>207</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>237</v>
+        <v>218</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B4" s="29"/>
       <c r="C4" s="24"/>
@@ -7720,21 +7792,21 @@
         <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B5" s="29"/>
       <c r="C5" s="25"/>
@@ -7742,13 +7814,13 @@
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -7771,13 +7843,13 @@
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>10</v>
@@ -7792,32 +7864,32 @@
     </row>
     <row r="9" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B9" s="29" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>226</v>
+        <v>207</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>205</v>
+        <v>239</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>231</v>
+        <v>212</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B10" s="29"/>
       <c r="C10" s="24"/>
@@ -7825,22 +7897,22 @@
         <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>206</v>
+        <v>240</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B11" s="29"/>
       <c r="C11" s="25"/>
@@ -7848,13 +7920,13 @@
         <v>16</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>205</v>
+        <v>239</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>239</v>
+        <v>220</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="3"/>
@@ -7974,8 +8046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8007,13 +8079,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -8027,125 +8099,125 @@
     </row>
     <row r="3" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>17</v>
+        <v>234</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>207</v>
+        <v>241</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="29"/>
       <c r="C4" s="29"/>
       <c r="D4" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>245</v>
+        <v>226</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="29"/>
       <c r="C5" s="29"/>
       <c r="D5" s="2" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="2" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="29"/>
       <c r="C6" s="29"/>
       <c r="D6" s="2" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="2" t="s">
-        <v>242</v>
+        <v>223</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="29"/>
       <c r="C7" s="29"/>
       <c r="D7" s="2" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>208</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>242</v>
+        <v>245</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>236</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>221</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="13" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A8" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B8" s="29"/>
       <c r="C8" s="29"/>
       <c r="D8" s="11" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>207</v>
+        <v>241</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H8" s="16"/>
     </row>
@@ -8157,13 +8229,13 @@
         <v>7</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F12" s="15" t="s">
         <v>10</v>
@@ -8177,124 +8249,124 @@
     </row>
     <row r="13" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A13" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>22</v>
+        <v>235</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>209</v>
+        <v>244</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H13" s="15"/>
     </row>
     <row r="14" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A14" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B14" s="24"/>
       <c r="C14" s="24"/>
       <c r="D14" s="15" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E14" s="27"/>
       <c r="F14" s="15" t="s">
-        <v>244</v>
+        <v>225</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H14" s="15"/>
     </row>
     <row r="15" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A15" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15" s="24"/>
       <c r="C15" s="24"/>
       <c r="D15" s="15" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E15" s="27"/>
       <c r="F15" s="15" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H15" s="15"/>
     </row>
     <row r="16" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A16" s="15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B16" s="24"/>
       <c r="C16" s="24"/>
       <c r="D16" s="15" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="E16" s="28"/>
       <c r="F16" s="15" t="s">
-        <v>243</v>
+        <v>224</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H16" s="15"/>
     </row>
-    <row r="17" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A17" s="15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B17" s="24"/>
       <c r="C17" s="24"/>
       <c r="D17" s="15" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>210</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>152</v>
+        <v>242</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>237</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A18" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25"/>
       <c r="D18" s="11" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>211</v>
+        <v>243</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -8322,7 +8394,7 @@
   <dimension ref="A2:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8344,13 +8416,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -8364,194 +8436,194 @@
     </row>
     <row r="3" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>160</v>
+        <v>246</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
       <c r="D4" s="2" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
       <c r="D5" s="2" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" s="24"/>
       <c r="C6" s="24"/>
       <c r="D6" s="2" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="E6" s="27"/>
       <c r="F6" s="2" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" s="13" customFormat="1" ht="156.75" x14ac:dyDescent="0.15">
       <c r="A7" s="11" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="B7" s="24"/>
       <c r="C7" s="24"/>
       <c r="D7" s="11" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="E7" s="28"/>
       <c r="F7" s="11" t="s">
-        <v>235</v>
+        <v>216</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" s="24"/>
       <c r="C8" s="24"/>
       <c r="D8" s="2" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>161</v>
+        <v>247</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B9" s="24"/>
       <c r="C9" s="24"/>
       <c r="D9" s="2" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="E9" s="27"/>
       <c r="F9" s="2" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B10" s="24"/>
       <c r="C10" s="24"/>
       <c r="D10" s="2" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="E10" s="27"/>
       <c r="F10" s="2" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B11" s="24"/>
       <c r="C11" s="24"/>
       <c r="D11" s="2" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="E11" s="27"/>
       <c r="F11" s="2" t="s">
-        <v>247</v>
+        <v>228</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" s="13" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A12" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B12" s="25"/>
       <c r="C12" s="25"/>
       <c r="D12" s="11" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="E12" s="28"/>
       <c r="F12" s="11" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -8572,7 +8644,7 @@
   <dimension ref="A2:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E3" sqref="E3:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8596,13 +8668,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -8614,96 +8686,96 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="156.75" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B3" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>192</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="29" t="s">
-        <v>202</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="E3" s="26" t="s">
-        <v>145</v>
+        <v>248</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" ht="99.75" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B4" s="29"/>
       <c r="C4" s="29"/>
       <c r="D4" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I4" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B5" s="29"/>
       <c r="C5" s="29"/>
       <c r="D5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="2" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:9" ht="99.75" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B6" s="29"/>
       <c r="C6" s="29"/>
       <c r="D6" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H6" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="I6" s="19" t="s">
         <v>103</v>
-      </c>
-      <c r="I6" s="19" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
@@ -8736,7 +8808,7 @@
   <dimension ref="A2:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E3" sqref="E3:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8758,13 +8830,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -8778,63 +8850,63 @@
     </row>
     <row r="3" spans="1:8" ht="114" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="29" t="s">
-        <v>203</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="E3" s="26" t="s">
-        <v>130</v>
+        <v>249</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="114" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" s="29"/>
       <c r="C4" s="29"/>
       <c r="D4" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B5" s="29"/>
       <c r="C5" s="29"/>
       <c r="D5" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E5" s="28"/>
       <c r="F5" s="2" t="s">
-        <v>250</v>
+        <v>231</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -8861,7 +8933,7 @@
   <dimension ref="A2:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8884,13 +8956,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -8904,102 +8976,102 @@
     </row>
     <row r="3" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>223</v>
+        <v>204</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>216</v>
+        <v>250</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
       <c r="D4" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
       <c r="D5" s="2" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="2" t="s">
-        <v>251</v>
+        <v>232</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" s="13" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="11" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B6" s="24"/>
       <c r="C6" s="24"/>
       <c r="D6" s="11" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="11" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:8" s="13" customFormat="1" ht="114" x14ac:dyDescent="0.15">
       <c r="A7" s="11" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>
       <c r="D7" s="11" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>217</v>
+        <v>251</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
@@ -9010,13 +9082,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>10</v>
@@ -9030,102 +9102,102 @@
     </row>
     <row r="11" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>218</v>
+        <v>252</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B12" s="24"/>
       <c r="C12" s="24"/>
       <c r="D12" s="2" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="E12" s="27"/>
       <c r="F12" s="2" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B13" s="24"/>
       <c r="C13" s="24"/>
       <c r="D13" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="E13" s="27"/>
       <c r="F13" s="2" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A14" s="11" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B14" s="24"/>
       <c r="C14" s="24"/>
       <c r="D14" s="11" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="E14" s="28"/>
       <c r="F14" s="11" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H14" s="11"/>
     </row>
     <row r="15" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A15" s="11" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B15" s="25"/>
       <c r="C15" s="25"/>
       <c r="D15" s="11" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>197</v>
+        <v>253</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -9147,8 +9219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9170,13 +9242,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -9190,63 +9262,63 @@
     </row>
     <row r="3" spans="1:8" ht="327.75" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>134</v>
+        <v>254</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B4" s="29"/>
       <c r="C4" s="29"/>
       <c r="D4" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B5" s="29"/>
       <c r="C5" s="29"/>
       <c r="D5" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E5" s="28"/>
       <c r="F5" s="2" t="s">
-        <v>252</v>
+        <v>233</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -9297,13 +9369,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -9317,97 +9389,97 @@
     </row>
     <row r="3" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
       <c r="D4" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F4" s="24"/>
       <c r="G4" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
       <c r="D5" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F5" s="24"/>
       <c r="G5" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B6" s="24"/>
       <c r="C6" s="24"/>
       <c r="D6" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F6" s="24"/>
       <c r="G6" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>
       <c r="D7" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H7" s="5"/>
     </row>

</xml_diff>

<commit_message>
Update the test cases file on the morning of 5th,June
</commit_message>
<xml_diff>
--- a/src/MyItems/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -1465,36 +1465,6 @@
   <si>
     <r>
       <t>1. 能够出现提示输入的信息
-2.显示该内容未在指定文件内查询到(</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>WCC didn't found on 456 - 副本.txt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1. 能够出现提示输入的信息
 2.显示该文件夹下不存在txt文件（</t>
     </r>
     <r>
@@ -1508,37 +1478,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>There is no txt files under folder D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1. 能够出现提示输入的信息
-2. 显示该内容在查到的txt文件内被查到几次（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alonso found on 456 - 副本 (2).txt for 2 times
-Alonso found on 456 - 副本.txt for 1 times</t>
     </r>
     <r>
       <rPr>
@@ -6931,6 +6870,66 @@
       </rPr>
       <t>=)
 2.可以在本地计算机中查到新名称文件</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 能够出现提示输入的信息
+2.显示该内容未在指定文件内查询到(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>WCC didn't found on D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 能够出现提示输入的信息
+2. 显示该内容在查到的txt文件内被查到几次（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Button found on D:\Test9\ADSK.txt for 2 times</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -7549,7 +7548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3:C6"/>
     </sheetView>
   </sheetViews>
@@ -7609,13 +7608,13 @@
         <v>58</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>60</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>124</v>
@@ -7654,7 +7653,7 @@
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>80</v>
@@ -7672,7 +7671,7 @@
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>86</v>
@@ -7705,7 +7704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -7766,16 +7765,16 @@
         <v>2</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>82</v>
@@ -7792,16 +7791,16 @@
         <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
@@ -7814,10 +7813,10 @@
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>82</v>
@@ -7870,16 +7869,16 @@
         <v>8</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>77</v>
@@ -7897,16 +7896,16 @@
         <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I10" s="3"/>
     </row>
@@ -7920,10 +7919,10 @@
         <v>16</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>77</v>
@@ -8102,19 +8101,19 @@
         <v>69</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>77</v>
@@ -8130,11 +8129,11 @@
       <c r="B4" s="29"/>
       <c r="C4" s="29"/>
       <c r="D4" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>89</v>
@@ -8148,11 +8147,11 @@
       <c r="B5" s="29"/>
       <c r="C5" s="29"/>
       <c r="D5" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>77</v>
@@ -8168,11 +8167,11 @@
       <c r="B6" s="29"/>
       <c r="C6" s="29"/>
       <c r="D6" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>88</v>
@@ -8186,19 +8185,19 @@
       <c r="B7" s="29"/>
       <c r="C7" s="29"/>
       <c r="D7" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>88</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="13" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
@@ -8208,13 +8207,13 @@
       <c r="B8" s="29"/>
       <c r="C8" s="29"/>
       <c r="D8" s="11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G8" s="16" t="s">
         <v>98</v>
@@ -8252,19 +8251,19 @@
         <v>70</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G13" s="15" t="s">
         <v>77</v>
@@ -8278,11 +8277,11 @@
       <c r="B14" s="24"/>
       <c r="C14" s="24"/>
       <c r="D14" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E14" s="27"/>
       <c r="F14" s="15" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G14" s="15" t="s">
         <v>77</v>
@@ -8296,11 +8295,11 @@
       <c r="B15" s="24"/>
       <c r="C15" s="24"/>
       <c r="D15" s="15" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E15" s="27"/>
       <c r="F15" s="15" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G15" s="15" t="s">
         <v>77</v>
@@ -8314,11 +8313,11 @@
       <c r="B16" s="24"/>
       <c r="C16" s="24"/>
       <c r="D16" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E16" s="28"/>
       <c r="F16" s="15" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G16" s="15" t="s">
         <v>77</v>
@@ -8332,19 +8331,19 @@
       <c r="B17" s="24"/>
       <c r="C17" s="24"/>
       <c r="D17" s="15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G17" s="15" t="s">
         <v>77</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="114" x14ac:dyDescent="0.15">
@@ -8354,13 +8353,13 @@
       <c r="B18" s="25"/>
       <c r="C18" s="25"/>
       <c r="D18" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G18" s="16" t="s">
         <v>77</v>
@@ -8442,16 +8441,16 @@
         <v>28</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>94</v>
@@ -8465,11 +8464,11 @@
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
       <c r="D4" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>95</v>
@@ -8483,11 +8482,11 @@
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
       <c r="D5" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>93</v>
@@ -8501,11 +8500,11 @@
       <c r="B6" s="24"/>
       <c r="C6" s="24"/>
       <c r="D6" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E6" s="27"/>
       <c r="F6" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>93</v>
@@ -8514,22 +8513,22 @@
     </row>
     <row r="7" spans="1:8" s="13" customFormat="1" ht="156.75" x14ac:dyDescent="0.15">
       <c r="A7" s="11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B7" s="24"/>
       <c r="C7" s="24"/>
       <c r="D7" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E7" s="28"/>
       <c r="F7" s="11" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
@@ -8539,13 +8538,13 @@
       <c r="B8" s="24"/>
       <c r="C8" s="24"/>
       <c r="D8" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>77</v>
@@ -8559,11 +8558,11 @@
       <c r="B9" s="24"/>
       <c r="C9" s="24"/>
       <c r="D9" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E9" s="27"/>
       <c r="F9" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>77</v>
@@ -8577,11 +8576,11 @@
       <c r="B10" s="24"/>
       <c r="C10" s="24"/>
       <c r="D10" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E10" s="27"/>
       <c r="F10" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>77</v>
@@ -8595,11 +8594,11 @@
       <c r="B11" s="24"/>
       <c r="C11" s="24"/>
       <c r="D11" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E11" s="27"/>
       <c r="F11" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>77</v>
@@ -8613,17 +8612,17 @@
       <c r="B12" s="25"/>
       <c r="C12" s="25"/>
       <c r="D12" s="11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E12" s="28"/>
       <c r="F12" s="11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -8643,8 +8642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8686,7 +8685,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="99.75" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>71</v>
       </c>
@@ -8694,16 +8693,16 @@
         <v>36</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>127</v>
+        <v>254</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>104</v>
@@ -8724,7 +8723,7 @@
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>125</v>
+        <v>253</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>86</v>
@@ -8747,7 +8746,7 @@
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>78</v>
@@ -8766,7 +8765,7 @@
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>86</v>
@@ -8856,16 +8855,16 @@
         <v>41</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>77</v>
@@ -8883,7 +8882,7 @@
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>86</v>
@@ -8903,7 +8902,7 @@
       </c>
       <c r="E5" s="28"/>
       <c r="F5" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>77</v>
@@ -8982,16 +8981,16 @@
         <v>49</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>81</v>
@@ -9005,11 +9004,11 @@
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
       <c r="D4" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>79</v>
@@ -9023,11 +9022,11 @@
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
       <c r="D5" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>80</v>
@@ -9036,42 +9035,42 @@
     </row>
     <row r="6" spans="1:8" s="13" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="11" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B6" s="24"/>
       <c r="C6" s="24"/>
       <c r="D6" s="11" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:8" s="13" customFormat="1" ht="114" x14ac:dyDescent="0.15">
       <c r="A7" s="11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>
       <c r="D7" s="11" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
@@ -9108,16 +9107,16 @@
         <v>50</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>77</v>
@@ -9131,11 +9130,11 @@
       <c r="B12" s="24"/>
       <c r="C12" s="24"/>
       <c r="D12" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E12" s="27"/>
       <c r="F12" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>77</v>
@@ -9149,11 +9148,11 @@
       <c r="B13" s="24"/>
       <c r="C13" s="24"/>
       <c r="D13" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E13" s="27"/>
       <c r="F13" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>77</v>
@@ -9162,16 +9161,16 @@
     </row>
     <row r="14" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A14" s="11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B14" s="24"/>
       <c r="C14" s="24"/>
       <c r="D14" s="11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E14" s="28"/>
       <c r="F14" s="11" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>77</v>
@@ -9180,24 +9179,24 @@
     </row>
     <row r="15" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A15" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B15" s="25"/>
       <c r="C15" s="25"/>
       <c r="D15" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>77</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -9268,16 +9267,16 @@
         <v>56</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>77</v>
@@ -9295,7 +9294,7 @@
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>86</v>
@@ -9315,7 +9314,7 @@
       </c>
       <c r="E5" s="28"/>
       <c r="F5" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>79</v>
@@ -9401,7 +9400,7 @@
         <v>110</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F3" s="23" t="s">
         <v>115</v>
@@ -9421,7 +9420,7 @@
         <v>111</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F4" s="24"/>
       <c r="G4" s="2" t="s">
@@ -9439,7 +9438,7 @@
         <v>112</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F5" s="24"/>
       <c r="G5" s="2" t="s">
@@ -9447,7 +9446,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="114" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>113</v>
       </c>
@@ -9457,7 +9456,7 @@
         <v>114</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F6" s="24"/>
       <c r="G6" s="5" t="s">
@@ -9465,7 +9464,7 @@
       </c>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="57" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>116</v>
       </c>
@@ -9475,7 +9474,7 @@
         <v>117</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="5" t="s">

</xml_diff>

<commit_message>
Update the test cases file on the afternoon of 5th,June(1)
</commit_message>
<xml_diff>
--- a/src/MyItems/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -1393,78 +1393,6 @@
   <si>
     <r>
       <t>1. 能够出现提示输入的信息
-2. 显示指定的内容没有被查到，并替换失败（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Not found on File!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1. 能够出现提示输入的信息
-2. 显示指定的内容已经被查到，并替换成功，并能够在本地文件中查看到替换之处，如测试数据所示，应将</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>替换成</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alonso</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1. 能够出现提示输入的信息
 2.显示该文件夹下不存在txt文件（</t>
     </r>
     <r>
@@ -6930,6 +6858,78 @@
         <scheme val="minor"/>
       </rPr>
       <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 能够出现提示输入的信息
+2. 显示指定的内容没有被查到，并替换失败（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Button didn't found on D:\Test9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 能够出现提示输入的信息
+2. 显示指定的内容已经被查到，并替换成功，并能够在本地文件中查看到替换之处，如测试数据所示，应将</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>替换成</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alonso (But has been replaced as Button on file D:\Test9\99888.txt succeeded!)</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -7548,8 +7548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7600,7 +7600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -7608,16 +7608,16 @@
         <v>58</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>60</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>124</v>
+        <v>254</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>78</v>
@@ -7635,7 +7635,7 @@
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>123</v>
+        <v>253</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>79</v>
@@ -7653,7 +7653,7 @@
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>80</v>
@@ -7671,7 +7671,7 @@
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>86</v>
@@ -7765,16 +7765,16 @@
         <v>2</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>82</v>
@@ -7791,16 +7791,16 @@
         <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
@@ -7813,10 +7813,10 @@
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>82</v>
@@ -7869,16 +7869,16 @@
         <v>8</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>77</v>
@@ -7896,16 +7896,16 @@
         <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I10" s="3"/>
     </row>
@@ -7919,10 +7919,10 @@
         <v>16</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>77</v>
@@ -8101,19 +8101,19 @@
         <v>69</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>77</v>
@@ -8129,11 +8129,11 @@
       <c r="B4" s="29"/>
       <c r="C4" s="29"/>
       <c r="D4" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>89</v>
@@ -8147,11 +8147,11 @@
       <c r="B5" s="29"/>
       <c r="C5" s="29"/>
       <c r="D5" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>77</v>
@@ -8167,11 +8167,11 @@
       <c r="B6" s="29"/>
       <c r="C6" s="29"/>
       <c r="D6" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>88</v>
@@ -8185,19 +8185,19 @@
       <c r="B7" s="29"/>
       <c r="C7" s="29"/>
       <c r="D7" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>88</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="13" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
@@ -8207,13 +8207,13 @@
       <c r="B8" s="29"/>
       <c r="C8" s="29"/>
       <c r="D8" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G8" s="16" t="s">
         <v>98</v>
@@ -8251,19 +8251,19 @@
         <v>70</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G13" s="15" t="s">
         <v>77</v>
@@ -8277,11 +8277,11 @@
       <c r="B14" s="24"/>
       <c r="C14" s="24"/>
       <c r="D14" s="15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E14" s="27"/>
       <c r="F14" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G14" s="15" t="s">
         <v>77</v>
@@ -8295,11 +8295,11 @@
       <c r="B15" s="24"/>
       <c r="C15" s="24"/>
       <c r="D15" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E15" s="27"/>
       <c r="F15" s="15" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G15" s="15" t="s">
         <v>77</v>
@@ -8313,11 +8313,11 @@
       <c r="B16" s="24"/>
       <c r="C16" s="24"/>
       <c r="D16" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E16" s="28"/>
       <c r="F16" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G16" s="15" t="s">
         <v>77</v>
@@ -8331,19 +8331,19 @@
       <c r="B17" s="24"/>
       <c r="C17" s="24"/>
       <c r="D17" s="15" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G17" s="15" t="s">
         <v>77</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="114" x14ac:dyDescent="0.15">
@@ -8353,13 +8353,13 @@
       <c r="B18" s="25"/>
       <c r="C18" s="25"/>
       <c r="D18" s="11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G18" s="16" t="s">
         <v>77</v>
@@ -8441,16 +8441,16 @@
         <v>28</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>94</v>
@@ -8464,11 +8464,11 @@
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
       <c r="D4" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>95</v>
@@ -8482,11 +8482,11 @@
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
       <c r="D5" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>93</v>
@@ -8500,11 +8500,11 @@
       <c r="B6" s="24"/>
       <c r="C6" s="24"/>
       <c r="D6" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E6" s="27"/>
       <c r="F6" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>93</v>
@@ -8513,22 +8513,22 @@
     </row>
     <row r="7" spans="1:8" s="13" customFormat="1" ht="156.75" x14ac:dyDescent="0.15">
       <c r="A7" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B7" s="24"/>
       <c r="C7" s="24"/>
       <c r="D7" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E7" s="28"/>
       <c r="F7" s="11" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
@@ -8538,13 +8538,13 @@
       <c r="B8" s="24"/>
       <c r="C8" s="24"/>
       <c r="D8" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>77</v>
@@ -8558,11 +8558,11 @@
       <c r="B9" s="24"/>
       <c r="C9" s="24"/>
       <c r="D9" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E9" s="27"/>
       <c r="F9" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>77</v>
@@ -8576,11 +8576,11 @@
       <c r="B10" s="24"/>
       <c r="C10" s="24"/>
       <c r="D10" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E10" s="27"/>
       <c r="F10" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>77</v>
@@ -8594,11 +8594,11 @@
       <c r="B11" s="24"/>
       <c r="C11" s="24"/>
       <c r="D11" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E11" s="27"/>
       <c r="F11" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>77</v>
@@ -8612,17 +8612,17 @@
       <c r="B12" s="25"/>
       <c r="C12" s="25"/>
       <c r="D12" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E12" s="28"/>
       <c r="F12" s="11" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -8642,7 +8642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -8693,16 +8693,16 @@
         <v>36</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>104</v>
@@ -8723,7 +8723,7 @@
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>86</v>
@@ -8746,7 +8746,7 @@
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>78</v>
@@ -8765,7 +8765,7 @@
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>86</v>
@@ -8855,16 +8855,16 @@
         <v>41</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>77</v>
@@ -8882,7 +8882,7 @@
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>86</v>
@@ -8902,7 +8902,7 @@
       </c>
       <c r="E5" s="28"/>
       <c r="F5" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>77</v>
@@ -8981,16 +8981,16 @@
         <v>49</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>81</v>
@@ -9004,11 +9004,11 @@
       <c r="B4" s="24"/>
       <c r="C4" s="24"/>
       <c r="D4" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>79</v>
@@ -9022,11 +9022,11 @@
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
       <c r="D5" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>80</v>
@@ -9035,42 +9035,42 @@
     </row>
     <row r="6" spans="1:8" s="13" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B6" s="24"/>
       <c r="C6" s="24"/>
       <c r="D6" s="11" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:8" s="13" customFormat="1" ht="114" x14ac:dyDescent="0.15">
       <c r="A7" s="11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>
       <c r="D7" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
@@ -9107,16 +9107,16 @@
         <v>50</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>77</v>
@@ -9130,11 +9130,11 @@
       <c r="B12" s="24"/>
       <c r="C12" s="24"/>
       <c r="D12" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E12" s="27"/>
       <c r="F12" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>77</v>
@@ -9148,11 +9148,11 @@
       <c r="B13" s="24"/>
       <c r="C13" s="24"/>
       <c r="D13" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E13" s="27"/>
       <c r="F13" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>77</v>
@@ -9161,16 +9161,16 @@
     </row>
     <row r="14" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A14" s="11" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B14" s="24"/>
       <c r="C14" s="24"/>
       <c r="D14" s="11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E14" s="28"/>
       <c r="F14" s="11" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>77</v>
@@ -9179,24 +9179,24 @@
     </row>
     <row r="15" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A15" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B15" s="25"/>
       <c r="C15" s="25"/>
       <c r="D15" s="11" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>77</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -9267,16 +9267,16 @@
         <v>56</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>77</v>
@@ -9294,7 +9294,7 @@
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>86</v>
@@ -9314,7 +9314,7 @@
       </c>
       <c r="E5" s="28"/>
       <c r="F5" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>79</v>
@@ -9400,7 +9400,7 @@
         <v>110</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F3" s="23" t="s">
         <v>115</v>
@@ -9420,7 +9420,7 @@
         <v>111</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F4" s="24"/>
       <c r="G4" s="2" t="s">
@@ -9438,7 +9438,7 @@
         <v>112</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F5" s="24"/>
       <c r="G5" s="2" t="s">
@@ -9456,7 +9456,7 @@
         <v>114</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F6" s="24"/>
       <c r="G6" s="5" t="s">
@@ -9474,7 +9474,7 @@
         <v>117</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="5" t="s">

</xml_diff>

<commit_message>
Update the test cases file on the afternoon of 6th,June
</commit_message>
<xml_diff>
--- a/src/MyItems/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Test Cases for FileOperation.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="270">
   <si>
     <t>Test Case 001</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4865,6 +4865,88 @@
   </si>
   <si>
     <r>
+      <t>在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"输入文件夹路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test1\456.txt</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"输入文件夹路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test1</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
       <t>1.在"</t>
     </r>
     <r>
@@ -4877,18 +4959,18 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Please input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入被复制文件夹的路径，如:</t>
     </r>
     <r>
       <rPr>
@@ -4924,42 +5006,36 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Please input what word you want to find:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入txt文件内存在的内容，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Alonso
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3.在"</t>
+      <t>Please input target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入需要复制到目标文件夹的路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\Program Files</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
     </r>
     <r>
       <rPr>
@@ -4967,40 +5043,11 @@
         <sz val="12"/>
         <color theme="4"/>
         <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input what word you want to replace:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入想要替换成的新内容，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alo</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>在"</t>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path</t>
     </r>
     <r>
       <rPr>
@@ -5012,100 +5059,18 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Please input the folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"输入文件夹路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test1\456.txt</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"输入文件夹路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test1</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入被复制文件夹的路径，如:</t>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入被复制文件的路径，如:</t>
     </r>
     <r>
       <rPr>
@@ -5124,7 +5089,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="3"/>
+        <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -5141,14 +5106,14 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Please input target folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
+      <t>Please input Target Folder:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -5164,7 +5129,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>E:\Program Files</t>
+      <t>E:\Program Files\Test</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -5178,30 +5143,18 @@
         <sz val="12"/>
         <color theme="4"/>
         <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder or file path</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -5217,14 +5170,14 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
+      <t>D:\Test\Alonso.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -5241,14 +5194,14 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Please input Target Folder:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
+      <t>Please input target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
@@ -5293,19 +5246,19 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>" 输入被复制文件的路径，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:D:\Test\Alonso.txt</t>
+      <t>" 输入被复制文件的路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\Alonso.txt</t>
     </r>
     <r>
       <rPr>
@@ -5352,7 +5305,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>E:\Program Files\Test</t>
+      <t>E:\Program Files</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -5370,18 +5323,18 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Please input the folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入被复制文件的路径，如:</t>
+      <t>Please input the source folder or file path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:" 输入被复制文件的路径，如:</t>
     </r>
     <r>
       <rPr>
@@ -5417,7 +5370,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Please input target folder path:</t>
+      <t>Please input the target folder path:</t>
     </r>
     <r>
       <rPr>
@@ -5458,30 +5411,29 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Please input the folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入被复制文件的路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\Alonso.txt</t>
+      <t>Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test1</t>
     </r>
     <r>
       <rPr>
@@ -5505,36 +5457,37 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Please input target folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入需要复制到目标文件夹的路径，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E:\Program Files</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
+      <t>What file you want to find on this folder?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入文件名，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>456.txt</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+1.在"</t>
     </r>
     <r>
       <rPr>
@@ -5546,30 +5499,30 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Please input the source folder or file path</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:" 输入被复制文件的路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\Alonso.txt</t>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\TesT39</t>
     </r>
     <r>
       <rPr>
@@ -5593,30 +5546,30 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Please input the target folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入需要复制到目标文件夹的路径，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E:\Program Files\Test</t>
+      <t>Please input what word you want to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test4</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -5634,30 +5587,30 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Please input the source folder or file path</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:" 输入被复制文件的路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test</t>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\Alonso.txt</t>
     </r>
     <r>
       <rPr>
@@ -5681,36 +5634,37 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Please input the target folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入需要复制到目标文件夹的路径，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E:\Program Files</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
+      <t>Please input what word you want to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+1.在"</t>
     </r>
     <r>
       <rPr>
@@ -5722,30 +5676,30 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Please input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test</t>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\ALO.bmp</t>
     </r>
     <r>
       <rPr>
@@ -5769,42 +5723,30 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>What content you want to find on txt file?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入txt文件内存在的内容，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Alonso
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t/>
+      <t>Please input what word you want to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BUT.txt</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -5822,29 +5764,30 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Please input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test1</t>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
     </r>
     <r>
       <rPr>
@@ -5868,95 +5811,6 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>What file you want to find on this folder?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入文件名，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>456.txt</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">
-1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\TesT39</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Please input what word you want to replace:</t>
     </r>
     <r>
@@ -5980,407 +5834,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Test4</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\Alonso.txt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input what word you want to replace:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入新的想要被替换的文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Test</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">
-1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件路径，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\ALO.bmp</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input what word you want to replace:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入新的想要被替换的文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>BUT.txt</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input what word you want to replace:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入新的想要被替换的文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Test2</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What word do you want find?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入原文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alonso</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-3.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What word do you want replace?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入新的想要被替换的文件夹名字，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Button</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -6931,6 +6385,750 @@
       </rPr>
       <t>Alonso (But has been replaced as Button on file D:\Test9\99888.txt succeeded!)</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test Case 058</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提示输入文件夹或者文件路径时，输入一串空字符</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what word you want to find:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入txt文件内存在的内容，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Alonso
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input what word you want to replace:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入想要替换成的新内容，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alo</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>在提示信息"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"出现时，输入一串空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>提示请不要输入空的信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please do not input the empty infos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test Case 059</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"输入文件夹路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test1\456.txt</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>在提示信息"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"出现时，输入一串空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test Case 060</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入被复制文件的路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:D:\Test\Alonso.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入需要复制到目标文件夹的路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\Program Files\Test</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test Case 061</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the source folder or file path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:" 输入被复制文件的路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入需要复制到目标文件夹的路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\Program Files</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>在提示信息"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the source folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"出现时，输入一串空字符</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test Case 062</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What content you want to find on txt file?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入txt文件内存在的内容，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Alonso
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test Case 063</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test Case 064</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What word do you want find?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入原文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alonso</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What word do you want replace?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入新的想要被替换的文件夹名字，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Button</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test Case 065</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -7049,7 +7247,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7065,6 +7263,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -7147,7 +7351,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -7240,6 +7444,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7549,7 +7759,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7614,10 +7824,10 @@
         <v>60</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>78</v>
@@ -7635,7 +7845,7 @@
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>79</v>
@@ -7679,6 +7889,26 @@
       <c r="H6" s="19" t="s">
         <v>100</v>
       </c>
+    </row>
+    <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A7" s="31" t="s">
+        <v>250</v>
+      </c>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>253</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>254</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="H7" s="32"/>
     </row>
     <row r="9" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A9" s="9"/>
@@ -7705,7 +7935,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -7733,7 +7963,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -7875,10 +8105,10 @@
         <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>223</v>
+        <v>257</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>77</v>
@@ -7896,7 +8126,7 @@
         <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>201</v>
@@ -7919,7 +8149,7 @@
         <v>16</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>206</v>
@@ -7930,14 +8160,25 @@
       <c r="H11" s="2"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C12" s="10"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+    <row r="12" spans="1:9" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A12" s="31" t="s">
+        <v>256</v>
+      </c>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>258</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>254</v>
+      </c>
+      <c r="G12" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="H12" s="32"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
@@ -8043,10 +8284,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8072,7 +8313,7 @@
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -8110,10 +8351,10 @@
         <v>135</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>77</v>
@@ -8151,7 +8392,7 @@
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="2" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>77</v>
@@ -8188,10 +8429,10 @@
         <v>139</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>88</v>
@@ -8210,10 +8451,10 @@
         <v>140</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="G8" s="16" t="s">
         <v>98</v>
@@ -8260,10 +8501,10 @@
         <v>141</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="G13" s="15" t="s">
         <v>77</v>
@@ -8299,7 +8540,7 @@
       </c>
       <c r="E15" s="27"/>
       <c r="F15" s="15" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="G15" s="15" t="s">
         <v>77</v>
@@ -8334,10 +8575,10 @@
         <v>145</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="G17" s="15" t="s">
         <v>77</v>
@@ -8356,10 +8597,10 @@
         <v>146</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>227</v>
+        <v>260</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="G18" s="16" t="s">
         <v>77</v>
@@ -8367,6 +8608,26 @@
       <c r="H18" s="17" t="s">
         <v>99</v>
       </c>
+    </row>
+    <row r="19" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A19" s="31" t="s">
+        <v>259</v>
+      </c>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>258</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>254</v>
+      </c>
+      <c r="G19" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="H19" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -8390,10 +8651,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H12"/>
+  <dimension ref="A2:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8409,7 +8670,7 @@
   <sheetData>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -8447,7 +8708,7 @@
         <v>150</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>147</v>
@@ -8541,7 +8802,7 @@
         <v>155</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>231</v>
+        <v>262</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>149</v>
@@ -8624,6 +8885,26 @@
       <c r="H12" s="17" t="s">
         <v>163</v>
       </c>
+    </row>
+    <row r="13" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A13" s="31" t="s">
+        <v>261</v>
+      </c>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>263</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>254</v>
+      </c>
+      <c r="G13" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="H13" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -8643,7 +8924,7 @@
   <dimension ref="A2:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8661,7 +8942,7 @@
   <sheetData>
     <row r="2" spans="1:9" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -8699,10 +8980,10 @@
         <v>38</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>232</v>
+        <v>265</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>104</v>
@@ -8723,7 +9004,7 @@
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="2" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>86</v>
@@ -8776,6 +9057,26 @@
       <c r="I6" s="19" t="s">
         <v>103</v>
       </c>
+    </row>
+    <row r="7" spans="1:9" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A7" s="31" t="s">
+        <v>264</v>
+      </c>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>253</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>254</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="H7" s="32"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B8" s="8"/>
@@ -8807,7 +9108,7 @@
   <dimension ref="A2:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8823,7 +9124,7 @@
   <sheetData>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -8861,7 +9162,7 @@
         <v>45</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>124</v>
@@ -8908,6 +9209,26 @@
         <v>77</v>
       </c>
       <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A6" s="31" t="s">
+        <v>266</v>
+      </c>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>253</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>254</v>
+      </c>
+      <c r="G6" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="H6" s="32"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B9" s="8"/>
@@ -8929,10 +9250,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H15"/>
+  <dimension ref="A2:H16"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -8949,7 +9270,7 @@
   <sheetData>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -8987,10 +9308,10 @@
         <v>172</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>81</v>
@@ -9061,10 +9382,10 @@
         <v>176</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>182</v>
@@ -9113,10 +9434,10 @@
         <v>169</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>77</v>
@@ -9187,10 +9508,10 @@
         <v>171</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>77</v>
@@ -9198,6 +9519,26 @@
       <c r="H15" s="12" t="s">
         <v>192</v>
       </c>
+    </row>
+    <row r="16" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A16" s="31" t="s">
+        <v>267</v>
+      </c>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>258</v>
+      </c>
+      <c r="F16" s="31" t="s">
+        <v>254</v>
+      </c>
+      <c r="G16" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="H16" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -9218,8 +9559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H8"/>
   <sheetViews>
-    <sheetView topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9235,7 +9576,7 @@
   <sheetData>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -9273,10 +9614,10 @@
         <v>126</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>238</v>
+        <v>268</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>77</v>
@@ -9320,6 +9661,26 @@
         <v>79</v>
       </c>
       <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A6" s="31" t="s">
+        <v>269</v>
+      </c>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>258</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>254</v>
+      </c>
+      <c r="G6" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="H6" s="32"/>
     </row>
     <row r="8" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A8" s="9"/>
@@ -9345,7 +9706,7 @@
   <dimension ref="A2:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9362,7 +9723,7 @@
   <sheetData>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Update test case file as a new function has been added
</commit_message>
<xml_diff>
--- a/src/MyItems/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="274">
   <si>
     <t>Test Case 001</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -597,59 +597,6 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件名</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.输入</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹路径
-2.输入文件夹下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>不存在的</t>
     </r>
     <r>
@@ -1423,35 +1370,6 @@
   <si>
     <r>
       <t>1.能够出现提示输入的信息
-2.显示指定文件被找到的信息（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>File: 456.txt has found on D:\Test1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.能够出现提示输入的信息
 2.显示指定文件未被找到的信息（</t>
     </r>
     <r>
@@ -4085,10 +4003,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>6. Find Files on Folder</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>在"</t>
     </r>
@@ -5394,93 +5308,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>E:\Program Files\Test</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What file you want to find on this folder?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入文件名，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>456.txt</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -7129,6 +6956,354 @@
   </si>
   <si>
     <t>Test Case 065</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6. Find Files or Folder on Folder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test Case 066</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹路径
+2.输入文件夹下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件名</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹路径
+2.输入文件夹下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹名</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.能够出现提示输入的信息
+2.显示指定文件被找到的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>File: 456.txt has found on D:\Test1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.能够出现提示输入的信息
+2.显示指定文件被找到的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Folder: McLaren has found on D:\Test9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What file or folder you want to find on this folder?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入文件名，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>456.txt</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What file or folder you want to find on this folder?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入文件夹名，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>McLaren</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -7351,7 +7526,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -7418,6 +7593,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -7445,11 +7626,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7758,7 +7936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -7775,18 +7953,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="A1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -7795,10 +7973,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -7814,23 +7992,23 @@
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>186</v>
+      <c r="B3" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>184</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>252</v>
+        <v>59</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>248</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -7838,17 +8016,17 @@
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" s="27"/>
+        <v>60</v>
+      </c>
+      <c r="E4" s="29"/>
       <c r="F4" s="2" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -7856,59 +8034,59 @@
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="27"/>
+      <c r="E5" s="29"/>
       <c r="F5" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
+        <v>61</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="28"/>
+      <c r="E6" s="30"/>
       <c r="F6" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="F7" s="22" t="s">
         <v>250</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="31" t="s">
+      <c r="G7" s="23" t="s">
         <v>251</v>
       </c>
-      <c r="E7" s="31" t="s">
-        <v>253</v>
-      </c>
-      <c r="F7" s="31" t="s">
-        <v>254</v>
-      </c>
-      <c r="G7" s="32" t="s">
-        <v>255</v>
-      </c>
-      <c r="H7" s="32"/>
+      <c r="H7" s="23"/>
     </row>
     <row r="9" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A9" s="9"/>
@@ -7952,18 +8130,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="A1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -7972,10 +8150,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -7989,67 +8167,67 @@
     </row>
     <row r="3" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="23" t="s">
-        <v>196</v>
+      <c r="C3" s="25" t="s">
+        <v>193</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="24"/>
+        <v>63</v>
+      </c>
+      <c r="B4" s="31"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="25"/>
+        <v>64</v>
+      </c>
+      <c r="B5" s="31"/>
+      <c r="C5" s="27"/>
       <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -8075,10 +8253,10 @@
         <v>21</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>10</v>
@@ -8093,96 +8271,96 @@
     </row>
     <row r="9" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="23" t="s">
-        <v>196</v>
+      <c r="C9" s="25" t="s">
+        <v>193</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="24"/>
+        <v>66</v>
+      </c>
+      <c r="B10" s="31"/>
+      <c r="C10" s="26"/>
       <c r="D10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="25"/>
+        <v>67</v>
+      </c>
+      <c r="B11" s="31"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:9" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A12" s="31" t="s">
-        <v>256</v>
-      </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="31" t="s">
+      <c r="A12" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="G12" s="23" t="s">
         <v>251</v>
       </c>
-      <c r="E12" s="31" t="s">
-        <v>258</v>
-      </c>
-      <c r="F12" s="31" t="s">
-        <v>254</v>
-      </c>
-      <c r="G12" s="32" t="s">
-        <v>255</v>
-      </c>
-      <c r="H12" s="32"/>
+      <c r="H12" s="23"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
-      <c r="B13" s="30"/>
+      <c r="B13" s="32"/>
       <c r="C13" s="4"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -8193,7 +8371,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
-      <c r="B14" s="30"/>
+      <c r="B14" s="32"/>
       <c r="C14" s="4"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -8204,7 +8382,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
-      <c r="B15" s="30"/>
+      <c r="B15" s="32"/>
       <c r="C15" s="4"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -8215,7 +8393,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
-      <c r="B16" s="30"/>
+      <c r="B16" s="32"/>
       <c r="C16" s="4"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -8226,7 +8404,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
-      <c r="B17" s="30"/>
+      <c r="B17" s="32"/>
       <c r="C17" s="4"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -8313,7 +8491,7 @@
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -8322,10 +8500,10 @@
         <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -8339,45 +8517,45 @@
     </row>
     <row r="3" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" s="29" t="s">
-        <v>220</v>
-      </c>
-      <c r="C3" s="29" t="s">
-        <v>198</v>
+        <v>68</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>217</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>195</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>224</v>
+        <v>133</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>221</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
       <c r="D4" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E4" s="27"/>
+        <v>134</v>
+      </c>
+      <c r="E4" s="29"/>
       <c r="F4" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -8385,37 +8563,37 @@
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
       <c r="D5" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E5" s="27"/>
+        <v>135</v>
+      </c>
+      <c r="E5" s="29"/>
       <c r="F5" s="2" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
       <c r="D6" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E6" s="28"/>
+        <v>136</v>
+      </c>
+      <c r="E6" s="30"/>
       <c r="F6" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -8423,41 +8601,41 @@
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
       <c r="D7" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="13" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A8" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="G8" s="16" t="s">
         <v>97</v>
-      </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>239</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>98</v>
       </c>
       <c r="H8" s="16"/>
     </row>
@@ -8472,10 +8650,10 @@
         <v>21</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F12" s="15" t="s">
         <v>10</v>
@@ -8489,25 +8667,25 @@
     </row>
     <row r="13" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A13" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>221</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>197</v>
+        <v>69</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>194</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="E13" s="26" t="s">
-        <v>226</v>
+        <v>139</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>223</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H13" s="15"/>
     </row>
@@ -8515,17 +8693,17 @@
       <c r="A14" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
       <c r="D14" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="E14" s="27"/>
+        <v>140</v>
+      </c>
+      <c r="E14" s="29"/>
       <c r="F14" s="15" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H14" s="15"/>
     </row>
@@ -8533,17 +8711,17 @@
       <c r="A15" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
       <c r="D15" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="E15" s="27"/>
+        <v>141</v>
+      </c>
+      <c r="E15" s="29"/>
       <c r="F15" s="15" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H15" s="15"/>
     </row>
@@ -8551,17 +8729,17 @@
       <c r="A16" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
       <c r="D16" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="E16" s="28"/>
+        <v>142</v>
+      </c>
+      <c r="E16" s="30"/>
       <c r="F16" s="15" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H16" s="15"/>
     </row>
@@ -8569,65 +8747,65 @@
       <c r="A17" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
       <c r="D17" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A18" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
+        <v>91</v>
+      </c>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
       <c r="D18" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A19" s="31" t="s">
-        <v>259</v>
-      </c>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="31" t="s">
+      <c r="A19" s="22" t="s">
+        <v>255</v>
+      </c>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="G19" s="23" t="s">
         <v>251</v>
       </c>
-      <c r="E19" s="31" t="s">
-        <v>258</v>
-      </c>
-      <c r="F19" s="31" t="s">
-        <v>254</v>
-      </c>
-      <c r="G19" s="32" t="s">
-        <v>255</v>
-      </c>
-      <c r="H19" s="32"/>
+      <c r="H19" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -8670,7 +8848,7 @@
   <sheetData>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -8679,10 +8857,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -8698,23 +8876,23 @@
       <c r="A3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="23" t="s">
-        <v>199</v>
+      <c r="C3" s="25" t="s">
+        <v>196</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>228</v>
+        <v>148</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>225</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -8722,17 +8900,17 @@
       <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E4" s="27"/>
+        <v>149</v>
+      </c>
+      <c r="E4" s="29"/>
       <c r="F4" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -8740,17 +8918,17 @@
       <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E5" s="27"/>
+        <v>150</v>
+      </c>
+      <c r="E5" s="29"/>
       <c r="F5" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -8758,57 +8936,57 @@
       <c r="A6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E6" s="27"/>
+        <v>151</v>
+      </c>
+      <c r="E6" s="29"/>
       <c r="F6" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" s="13" customFormat="1" ht="156.75" x14ac:dyDescent="0.15">
       <c r="A7" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
+        <v>146</v>
+      </c>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
       <c r="D7" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="E7" s="28"/>
+        <v>152</v>
+      </c>
+      <c r="E7" s="30"/>
       <c r="F7" s="11" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
       <c r="D8" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E8" s="26" t="s">
-        <v>262</v>
+        <v>153</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>258</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H8" s="2"/>
     </row>
@@ -8816,17 +8994,17 @@
       <c r="A9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
       <c r="D9" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E9" s="27"/>
+        <v>154</v>
+      </c>
+      <c r="E9" s="29"/>
       <c r="F9" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H9" s="2"/>
     </row>
@@ -8834,17 +9012,17 @@
       <c r="A10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
       <c r="D10" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E10" s="27"/>
+        <v>155</v>
+      </c>
+      <c r="E10" s="29"/>
       <c r="F10" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H10" s="5"/>
     </row>
@@ -8852,59 +9030,59 @@
       <c r="A11" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
       <c r="D11" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E11" s="27"/>
+        <v>156</v>
+      </c>
+      <c r="E11" s="29"/>
       <c r="F11" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" s="13" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A12" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
+        <v>95</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
       <c r="D12" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="E12" s="28"/>
+        <v>157</v>
+      </c>
+      <c r="E12" s="30"/>
       <c r="F12" s="11" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A13" s="31" t="s">
-        <v>261</v>
-      </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="31" t="s">
+      <c r="A13" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>259</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="G13" s="23" t="s">
         <v>251</v>
       </c>
-      <c r="E13" s="31" t="s">
-        <v>263</v>
-      </c>
-      <c r="F13" s="31" t="s">
-        <v>254</v>
-      </c>
-      <c r="G13" s="32" t="s">
-        <v>255</v>
-      </c>
-      <c r="H13" s="32"/>
+      <c r="H13" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -8942,7 +9120,7 @@
   <sheetData>
     <row r="2" spans="1:9" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -8951,10 +9129,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -8968,115 +9146,115 @@
     </row>
     <row r="3" spans="1:9" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="29" t="s">
-        <v>187</v>
+      <c r="C3" s="31" t="s">
+        <v>185</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="26" t="s">
-        <v>265</v>
+      <c r="E3" s="28" t="s">
+        <v>261</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
+        <v>83</v>
+      </c>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
       <c r="D4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="29"/>
       <c r="F4" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H4" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="I4" s="19" t="s">
         <v>101</v>
-      </c>
-      <c r="I4" s="19" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
       <c r="D5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="27"/>
+      <c r="E5" s="29"/>
       <c r="F5" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
+        <v>82</v>
+      </c>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
       <c r="D6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="28"/>
+      <c r="E6" s="30"/>
       <c r="F6" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I6" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A7" s="31" t="s">
-        <v>264</v>
-      </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="31" t="s">
+      <c r="A7" s="22" t="s">
+        <v>260</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="G7" s="23" t="s">
         <v>251</v>
       </c>
-      <c r="E7" s="31" t="s">
-        <v>253</v>
-      </c>
-      <c r="F7" s="31" t="s">
-        <v>254</v>
-      </c>
-      <c r="G7" s="32" t="s">
-        <v>255</v>
-      </c>
-      <c r="H7" s="32"/>
+      <c r="H7" s="23"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B8" s="8"/>
@@ -9105,11 +9283,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H9"/>
+  <dimension ref="A2:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -9124,7 +9300,7 @@
   <sheetData>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -9133,10 +9309,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -9152,23 +9328,23 @@
       <c r="A3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="29" t="s">
-        <v>188</v>
+      <c r="C3" s="25" t="s">
+        <v>266</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>229</v>
+        <v>268</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>272</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>124</v>
+        <v>270</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -9176,68 +9352,86 @@
       <c r="A4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="27"/>
+        <v>45</v>
+      </c>
+      <c r="E4" s="29"/>
       <c r="F4" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
+        <v>47</v>
+      </c>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="28"/>
+        <v>46</v>
+      </c>
+      <c r="E5" s="30"/>
       <c r="F5" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A6" s="31" t="s">
-        <v>266</v>
-      </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="31" t="s">
+    <row r="6" spans="1:8" ht="114" x14ac:dyDescent="0.15">
+      <c r="A6" s="22" t="s">
+        <v>267</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>273</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+    </row>
+    <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
+      <c r="A7" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="G7" s="23" t="s">
         <v>251</v>
       </c>
-      <c r="E6" s="31" t="s">
-        <v>253</v>
-      </c>
-      <c r="F6" s="31" t="s">
-        <v>254</v>
-      </c>
-      <c r="G6" s="32" t="s">
-        <v>255</v>
-      </c>
-      <c r="H6" s="32"/>
+      <c r="H7" s="23"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B9" s="8"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B10" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
     <mergeCell ref="E3:E5"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C3:C6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -9270,7 +9464,7 @@
   <sheetData>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -9279,10 +9473,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -9296,102 +9490,102 @@
     </row>
     <row r="3" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>193</v>
+        <v>50</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>190</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>230</v>
+        <v>170</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>226</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
+        <v>51</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E4" s="27"/>
+        <v>171</v>
+      </c>
+      <c r="E4" s="29"/>
       <c r="F4" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
+        <v>52</v>
+      </c>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="E5" s="27"/>
+        <v>172</v>
+      </c>
+      <c r="E5" s="29"/>
       <c r="F5" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" s="13" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
+        <v>164</v>
+      </c>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="E6" s="28"/>
+        <v>173</v>
+      </c>
+      <c r="E6" s="30"/>
       <c r="F6" s="11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:8" s="13" customFormat="1" ht="114" x14ac:dyDescent="0.15">
       <c r="A7" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
+        <v>131</v>
+      </c>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="11" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
@@ -9408,7 +9602,7 @@
         <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>10</v>
@@ -9422,123 +9616,123 @@
     </row>
     <row r="11" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>194</v>
+        <v>53</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>191</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="E11" s="26" t="s">
-        <v>232</v>
+        <v>167</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>228</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
+        <v>71</v>
+      </c>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
       <c r="D12" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="E12" s="27"/>
+        <v>168</v>
+      </c>
+      <c r="E12" s="29"/>
       <c r="F12" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
+        <v>72</v>
+      </c>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
       <c r="D13" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="E13" s="27"/>
+        <v>176</v>
+      </c>
+      <c r="E13" s="29"/>
       <c r="F13" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A14" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
+        <v>166</v>
+      </c>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
       <c r="D14" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="E14" s="28"/>
+        <v>178</v>
+      </c>
+      <c r="E14" s="30"/>
       <c r="F14" s="11" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H14" s="11"/>
     </row>
     <row r="15" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A15" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
+        <v>132</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
       <c r="D15" s="11" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A16" s="31" t="s">
-        <v>267</v>
-      </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="31" t="s">
+      <c r="A16" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="G16" s="23" t="s">
         <v>251</v>
       </c>
-      <c r="E16" s="31" t="s">
-        <v>258</v>
-      </c>
-      <c r="F16" s="31" t="s">
-        <v>254</v>
-      </c>
-      <c r="G16" s="32" t="s">
-        <v>255</v>
-      </c>
-      <c r="H16" s="32"/>
+      <c r="H16" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -9576,7 +9770,7 @@
   <sheetData>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -9585,10 +9779,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -9602,85 +9796,85 @@
     </row>
     <row r="3" spans="1:8" ht="185.25" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="29" t="s">
-        <v>195</v>
+        <v>73</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>192</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>268</v>
+        <v>124</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>264</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
+        <v>74</v>
+      </c>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
       <c r="D4" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" s="27"/>
+        <v>56</v>
+      </c>
+      <c r="E4" s="29"/>
       <c r="F4" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" s="14" t="s">
         <v>86</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
+        <v>75</v>
+      </c>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
       <c r="D5" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" s="28"/>
+        <v>54</v>
+      </c>
+      <c r="E5" s="30"/>
       <c r="F5" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A6" s="31" t="s">
-        <v>269</v>
-      </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="31" t="s">
+      <c r="A6" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="G6" s="23" t="s">
         <v>251</v>
       </c>
-      <c r="E6" s="31" t="s">
-        <v>258</v>
-      </c>
-      <c r="F6" s="31" t="s">
-        <v>254</v>
-      </c>
-      <c r="G6" s="32" t="s">
-        <v>255</v>
-      </c>
-      <c r="H6" s="32"/>
+      <c r="H6" s="23"/>
     </row>
     <row r="8" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A8" s="9"/>
@@ -9723,7 +9917,7 @@
   <sheetData>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -9732,10 +9926,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
@@ -9749,97 +9943,97 @@
     </row>
     <row r="3" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B3" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="C3" s="23" t="s">
-        <v>106</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>115</v>
+        <v>126</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>114</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
+        <v>107</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="F4" s="24"/>
+        <v>127</v>
+      </c>
+      <c r="F4" s="26"/>
       <c r="G4" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
+        <v>108</v>
+      </c>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F5" s="24"/>
+        <v>128</v>
+      </c>
+      <c r="F5" s="26"/>
       <c r="G5" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F6" s="24"/>
+        <v>130</v>
+      </c>
+      <c r="F6" s="26"/>
       <c r="G6" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F7" s="27"/>
+      <c r="G7" s="5" t="s">
         <v>117</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="5" t="s">
-        <v>118</v>
       </c>
       <c r="H7" s="5"/>
     </row>

</xml_diff>

<commit_message>
Update the test case file on the morning of 7th,June
</commit_message>
<xml_diff>
--- a/src/MyItems/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -3995,14 +3995,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1. Replace Content on txt files</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5. Find Contents on txt files</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>在"</t>
     </r>
@@ -4094,30 +4086,6 @@
   </si>
   <si>
     <t>7. Rename File or Folder</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7. Rename File or Folder</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8. Replace File Name With SpecificName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2. Delete File or Folder</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3. Copy File or Folder</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3. Copy File or Folder</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4. Move File or Folder</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -6959,10 +6927,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>6. Find Files or Folder on Folder</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Test Case 066</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -7304,6 +7268,42 @@
       </rPr>
       <t>McLaren</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Replace content on txt files</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. Delete file or folder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. Copy file or folder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. Copy file or folder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. Move file or folder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5. Find contents on txt files</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6. Find files or folder on folder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7. Rename file or folder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8. Rename file with specificname</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -7599,6 +7599,9 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -7625,9 +7628,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7936,8 +7936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -7953,14 +7953,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="24"/>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="A1" s="25"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -7992,20 +7992,20 @@
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="25" t="s">
-        <v>184</v>
+      <c r="C3" s="26" t="s">
+        <v>265</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="28" t="s">
-        <v>248</v>
+      <c r="E3" s="29" t="s">
+        <v>240</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>77</v>
@@ -8016,14 +8016,14 @@
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="29"/>
+      <c r="E4" s="30"/>
       <c r="F4" s="2" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>78</v>
@@ -8034,14 +8034,14 @@
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
       <c r="D5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="29"/>
+      <c r="E5" s="30"/>
       <c r="F5" s="2" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>79</v>
@@ -8052,14 +8052,14 @@
       <c r="A6" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
       <c r="D6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="30"/>
+      <c r="E6" s="31"/>
       <c r="F6" s="2" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>85</v>
@@ -8070,21 +8070,21 @@
     </row>
     <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A7" s="22" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="23"/>
       <c r="D7" s="22" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="H7" s="23"/>
     </row>
@@ -8113,7 +8113,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -8130,14 +8130,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="24"/>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="A1" s="25"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -8169,20 +8169,20 @@
       <c r="A3" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="25" t="s">
-        <v>193</v>
+      <c r="C3" s="26" t="s">
+        <v>266</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>81</v>
@@ -8193,16 +8193,16 @@
       <c r="A4" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="26"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>183</v>
@@ -8215,16 +8215,16 @@
       <c r="A5" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="27"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="28"/>
       <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>81</v>
@@ -8273,20 +8273,20 @@
       <c r="A9" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="25" t="s">
-        <v>193</v>
+      <c r="C9" s="26" t="s">
+        <v>266</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>76</v>
@@ -8298,16 +8298,16 @@
       <c r="A10" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="26"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>183</v>
@@ -8321,16 +8321,16 @@
       <c r="A11" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="27"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="28"/>
       <c r="D11" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>76</v>
@@ -8340,27 +8340,27 @@
     </row>
     <row r="12" spans="1:9" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A12" s="22" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="B12" s="23"/>
       <c r="C12" s="23"/>
       <c r="D12" s="22" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="G12" s="23" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="H12" s="23"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
-      <c r="B13" s="32"/>
+      <c r="B13" s="33"/>
       <c r="C13" s="4"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -8371,7 +8371,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
-      <c r="B14" s="32"/>
+      <c r="B14" s="33"/>
       <c r="C14" s="4"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -8382,7 +8382,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
-      <c r="B15" s="32"/>
+      <c r="B15" s="33"/>
       <c r="C15" s="4"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -8393,7 +8393,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
-      <c r="B16" s="32"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="4"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -8404,7 +8404,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
-      <c r="B17" s="32"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="4"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -8464,9 +8464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -8519,20 +8517,20 @@
       <c r="A3" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="31" t="s">
-        <v>217</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>195</v>
+      <c r="B3" s="32" t="s">
+        <v>209</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>268</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E3" s="28" t="s">
-        <v>221</v>
+      <c r="E3" s="29" t="s">
+        <v>213</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>76</v>
@@ -8545,14 +8543,14 @@
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
       <c r="D4" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E4" s="29"/>
+      <c r="E4" s="30"/>
       <c r="F4" s="2" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>88</v>
@@ -8563,14 +8561,14 @@
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
       <c r="D5" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E5" s="29"/>
+      <c r="E5" s="30"/>
       <c r="F5" s="2" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>76</v>
@@ -8583,14 +8581,14 @@
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
       <c r="D6" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E6" s="30"/>
+      <c r="E6" s="31"/>
       <c r="F6" s="2" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>87</v>
@@ -8601,38 +8599,38 @@
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
       <c r="D7" s="2" t="s">
         <v>137</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>87</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="13" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A8" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
       <c r="D8" s="11" t="s">
         <v>138</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="G8" s="16" t="s">
         <v>97</v>
@@ -8669,20 +8667,20 @@
       <c r="A13" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="25" t="s">
-        <v>218</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>194</v>
+      <c r="B13" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>267</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="E13" s="28" t="s">
-        <v>223</v>
+      <c r="E13" s="29" t="s">
+        <v>215</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="G13" s="15" t="s">
         <v>76</v>
@@ -8693,14 +8691,14 @@
       <c r="A14" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
       <c r="D14" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="E14" s="29"/>
+      <c r="E14" s="30"/>
       <c r="F14" s="15" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="G14" s="15" t="s">
         <v>76</v>
@@ -8711,14 +8709,14 @@
       <c r="A15" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
       <c r="D15" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="E15" s="29"/>
+      <c r="E15" s="30"/>
       <c r="F15" s="15" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="G15" s="15" t="s">
         <v>76</v>
@@ -8729,14 +8727,14 @@
       <c r="A16" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
       <c r="D16" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="E16" s="30"/>
+      <c r="E16" s="31"/>
       <c r="F16" s="15" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="G16" s="15" t="s">
         <v>76</v>
@@ -8747,16 +8745,16 @@
       <c r="A17" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
       <c r="D17" s="15" t="s">
         <v>143</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="G17" s="15" t="s">
         <v>76</v>
@@ -8769,16 +8767,16 @@
       <c r="A18" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
       <c r="D18" s="11" t="s">
         <v>144</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="G18" s="16" t="s">
         <v>76</v>
@@ -8789,21 +8787,21 @@
     </row>
     <row r="19" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A19" s="22" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="B19" s="23"/>
       <c r="C19" s="23"/>
       <c r="D19" s="22" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="F19" s="22" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="G19" s="23" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="H19" s="23"/>
     </row>
@@ -8831,9 +8829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -8876,17 +8872,17 @@
       <c r="A3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="25" t="s">
-        <v>196</v>
+      <c r="C3" s="26" t="s">
+        <v>269</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E3" s="28" t="s">
-        <v>225</v>
+      <c r="E3" s="29" t="s">
+        <v>217</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>145</v>
@@ -8900,14 +8896,14 @@
       <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="E4" s="29"/>
+      <c r="E4" s="30"/>
       <c r="F4" s="2" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>94</v>
@@ -8918,12 +8914,12 @@
       <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
       <c r="D5" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="E5" s="29"/>
+      <c r="E5" s="30"/>
       <c r="F5" s="2" t="s">
         <v>158</v>
       </c>
@@ -8936,14 +8932,14 @@
       <c r="A6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E6" s="29"/>
+      <c r="E6" s="30"/>
       <c r="F6" s="2" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>92</v>
@@ -8954,14 +8950,14 @@
       <c r="A7" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="E7" s="30"/>
+      <c r="E7" s="31"/>
       <c r="F7" s="11" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>162</v>
@@ -8974,13 +8970,13 @@
       <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="E8" s="28" t="s">
-        <v>258</v>
+      <c r="E8" s="29" t="s">
+        <v>250</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>147</v>
@@ -8994,14 +8990,14 @@
       <c r="A9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="E9" s="29"/>
+      <c r="E9" s="30"/>
       <c r="F9" s="2" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>76</v>
@@ -9012,12 +9008,12 @@
       <c r="A10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="E10" s="29"/>
+      <c r="E10" s="30"/>
       <c r="F10" s="2" t="s">
         <v>159</v>
       </c>
@@ -9030,14 +9026,14 @@
       <c r="A11" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="E11" s="29"/>
+      <c r="E11" s="30"/>
       <c r="F11" s="2" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>76</v>
@@ -9048,14 +9044,14 @@
       <c r="A12" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
       <c r="D12" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="31"/>
       <c r="F12" s="11" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>162</v>
@@ -9066,21 +9062,21 @@
     </row>
     <row r="13" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A13" s="22" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="B13" s="23"/>
       <c r="C13" s="23"/>
       <c r="D13" s="22" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="H13" s="23"/>
     </row>
@@ -9101,9 +9097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -9148,20 +9142,20 @@
       <c r="A3" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="31" t="s">
-        <v>185</v>
+      <c r="C3" s="32" t="s">
+        <v>270</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="28" t="s">
-        <v>261</v>
+      <c r="E3" s="29" t="s">
+        <v>253</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>103</v>
@@ -9175,14 +9169,14 @@
       <c r="A4" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
       <c r="D4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="29"/>
+      <c r="E4" s="30"/>
       <c r="F4" s="2" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>85</v>
@@ -9198,14 +9192,14 @@
       <c r="A5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
       <c r="D5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="29"/>
+      <c r="E5" s="30"/>
       <c r="F5" s="2" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>77</v>
@@ -9217,12 +9211,12 @@
       <c r="A6" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
       <c r="D6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="30"/>
+      <c r="E6" s="31"/>
       <c r="F6" s="2" t="s">
         <v>122</v>
       </c>
@@ -9238,21 +9232,21 @@
     </row>
     <row r="7" spans="1:9" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A7" s="22" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="23"/>
       <c r="D7" s="22" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="H7" s="23"/>
     </row>
@@ -9285,7 +9279,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -9328,20 +9322,20 @@
       <c r="A3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="25" t="s">
-        <v>266</v>
+      <c r="C3" s="26" t="s">
+        <v>271</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="E3" s="28" t="s">
-        <v>272</v>
+        <v>259</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>263</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>76</v>
@@ -9352,12 +9346,12 @@
       <c r="A4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="29"/>
+      <c r="E4" s="30"/>
       <c r="F4" s="2" t="s">
         <v>123</v>
       </c>
@@ -9372,14 +9366,14 @@
       <c r="A5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
       <c r="D5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="30"/>
+      <c r="E5" s="31"/>
       <c r="F5" s="2" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>76</v>
@@ -9388,39 +9382,39 @@
     </row>
     <row r="6" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A6" s="22" t="s">
-        <v>267</v>
-      </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
+        <v>258</v>
+      </c>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
       <c r="D6" s="22" t="s">
-        <v>269</v>
-      </c>
-      <c r="E6" s="33" t="s">
-        <v>273</v>
+        <v>260</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>264</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="G6" s="22"/>
       <c r="H6" s="22"/>
     </row>
     <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A7" s="22" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="23"/>
       <c r="D7" s="22" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="H7" s="23"/>
     </row>
@@ -9446,9 +9440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -9492,20 +9484,20 @@
       <c r="A3" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="25" t="s">
-        <v>190</v>
+      <c r="C3" s="26" t="s">
+        <v>272</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="E3" s="28" t="s">
-        <v>226</v>
+      <c r="E3" s="29" t="s">
+        <v>218</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>80</v>
@@ -9516,12 +9508,12 @@
       <c r="A4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="E4" s="29"/>
+      <c r="E4" s="30"/>
       <c r="F4" s="2" t="s">
         <v>163</v>
       </c>
@@ -9534,14 +9526,14 @@
       <c r="A5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
       <c r="D5" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E5" s="29"/>
+      <c r="E5" s="30"/>
       <c r="F5" s="2" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>79</v>
@@ -9552,12 +9544,12 @@
       <c r="A6" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="E6" s="30"/>
+      <c r="E6" s="31"/>
       <c r="F6" s="11" t="s">
         <v>165</v>
       </c>
@@ -9570,22 +9562,22 @@
       <c r="A7" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
       <c r="D7" s="11" t="s">
         <v>174</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>180</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
@@ -9618,20 +9610,20 @@
       <c r="A11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="25" t="s">
-        <v>191</v>
+      <c r="C11" s="26" t="s">
+        <v>188</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="E11" s="28" t="s">
-        <v>228</v>
+      <c r="E11" s="29" t="s">
+        <v>220</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>76</v>
@@ -9642,12 +9634,12 @@
       <c r="A12" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
       <c r="D12" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E12" s="29"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="2" t="s">
         <v>175</v>
       </c>
@@ -9660,12 +9652,12 @@
       <c r="A13" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E13" s="29"/>
+      <c r="E13" s="30"/>
       <c r="F13" s="2" t="s">
         <v>177</v>
       </c>
@@ -9678,12 +9670,12 @@
       <c r="A14" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
       <c r="D14" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="E14" s="30"/>
+      <c r="E14" s="31"/>
       <c r="F14" s="11" t="s">
         <v>181</v>
       </c>
@@ -9696,41 +9688,41 @@
       <c r="A15" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
       <c r="D15" s="11" t="s">
         <v>169</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>76</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A16" s="22" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="23"/>
       <c r="D16" s="22" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="G16" s="23" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="H16" s="23"/>
     </row>
@@ -9753,9 +9745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -9798,20 +9788,20 @@
       <c r="A3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="31" t="s">
-        <v>192</v>
+      <c r="C3" s="32" t="s">
+        <v>273</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E3" s="28" t="s">
-        <v>264</v>
+      <c r="E3" s="29" t="s">
+        <v>256</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>76</v>
@@ -9822,12 +9812,12 @@
       <c r="A4" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
       <c r="D4" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="29"/>
+      <c r="E4" s="30"/>
       <c r="F4" s="2" t="s">
         <v>125</v>
       </c>
@@ -9842,14 +9832,14 @@
       <c r="A5" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
       <c r="D5" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="30"/>
+      <c r="E5" s="31"/>
       <c r="F5" s="2" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>78</v>
@@ -9858,21 +9848,21 @@
     </row>
     <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A6" s="22" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="23"/>
       <c r="D6" s="22" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="H6" s="23"/>
     </row>
@@ -9945,10 +9935,10 @@
       <c r="A3" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="26" t="s">
         <v>105</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -9957,7 +9947,7 @@
       <c r="E3" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="26" t="s">
         <v>114</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -9969,15 +9959,15 @@
       <c r="A4" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="2" t="s">
         <v>110</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="F4" s="26"/>
+      <c r="F4" s="27"/>
       <c r="G4" s="2" t="s">
         <v>117</v>
       </c>
@@ -9987,15 +9977,15 @@
       <c r="A5" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
       <c r="D5" s="2" t="s">
         <v>111</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F5" s="26"/>
+      <c r="F5" s="27"/>
       <c r="G5" s="2" t="s">
         <v>117</v>
       </c>
@@ -10005,15 +9995,15 @@
       <c r="A6" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="2" t="s">
         <v>113</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F6" s="26"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="5" t="s">
         <v>117</v>
       </c>
@@ -10023,15 +10013,15 @@
       <c r="A7" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
       <c r="D7" s="2" t="s">
         <v>116</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="28"/>
       <c r="G7" s="5" t="s">
         <v>117</v>
       </c>

</xml_diff>

<commit_message>
Update the test case file on the afternoon of 12th,June
</commit_message>
<xml_diff>
--- a/src/MyItems/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="285">
   <si>
     <t>Test Case 001</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1902,70 +1902,6 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>需要被复制文件夹的路径和</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>不存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>目标路径
-2.输入被复制文件夹路径和目标文件夹路径</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t/>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.找到本地计算机中</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>都不存在的</t>
     </r>
     <r>
@@ -5188,94 +5124,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>E:\Program Files</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the source folder or file path</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:" 输入被复制文件的路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\Alonso.txt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the target folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入需要复制到目标文件夹的路径，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E:\Program Files\Test</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -7304,6 +7152,627 @@
   </si>
   <si>
     <t>8. Rename file with specificname</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test Case 066</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.找到本地计算机中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要被复制文件夹的路径和</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>不存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>目标路径
+2.输入被复制文件夹路径和目标文件夹路径</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.找到本地计算机中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要被复制文件夹的路径和</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>空字符串</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.输入被复制文件夹路径和目标文件夹路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入被复制文件夹的路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入需要复制到目标文件夹的路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\Program Files</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入被复制文件夹的路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入空字符串</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test Case 067</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 提示请不要输入空的信息 
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Do not input the empty infos. Please input again!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2. 返回重新输入非空字符的文件夹路径，若仍然是空字符串，则继续提示错误，并重新输入</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.找到本地计算机中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要被复制文件的路径和</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>空字符串</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.输入被复制文件夹路径和目标文件夹路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test Case 068</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test Case 069</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the source folder or file path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:" 输入被复制文件的路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\Alonso.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入需要复制到目标文件夹的路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\Program Files\Test</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入被复制文件夹的路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入空字符串</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入被复制文件夹的路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\Alonso.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入空字符串</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -7936,7 +8405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -7996,16 +8465,16 @@
         <v>57</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>59</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>77</v>
@@ -8023,7 +8492,7 @@
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>78</v>
@@ -8041,7 +8510,7 @@
       </c>
       <c r="E5" s="30"/>
       <c r="F5" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>79</v>
@@ -8059,7 +8528,7 @@
       </c>
       <c r="E6" s="31"/>
       <c r="F6" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>85</v>
@@ -8070,21 +8539,21 @@
     </row>
     <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A7" s="22" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="23"/>
       <c r="D7" s="22" t="s">
+        <v>237</v>
+      </c>
+      <c r="E7" s="22" t="s">
         <v>239</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="F7" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="G7" s="23" t="s">
         <v>241</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>242</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>243</v>
       </c>
       <c r="H7" s="23"/>
     </row>
@@ -8173,16 +8642,16 @@
         <v>2</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>81</v>
@@ -8199,16 +8668,16 @@
         <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
@@ -8221,10 +8690,10 @@
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>81</v>
@@ -8277,16 +8746,16 @@
         <v>8</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>76</v>
@@ -8304,16 +8773,16 @@
         <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I10" s="3"/>
     </row>
@@ -8327,10 +8796,10 @@
         <v>16</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>76</v>
@@ -8340,21 +8809,21 @@
     </row>
     <row r="12" spans="1:9" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A12" s="22" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B12" s="23"/>
       <c r="C12" s="23"/>
       <c r="D12" s="22" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G12" s="23" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H12" s="23"/>
     </row>
@@ -8462,9 +8931,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -8518,19 +8987,19 @@
         <v>68</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>133</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>76</v>
@@ -8550,7 +9019,7 @@
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>88</v>
@@ -8564,11 +9033,11 @@
       <c r="B5" s="32"/>
       <c r="C5" s="32"/>
       <c r="D5" s="2" t="s">
-        <v>135</v>
+        <v>273</v>
       </c>
       <c r="E5" s="30"/>
       <c r="F5" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>76</v>
@@ -8584,11 +9053,11 @@
       <c r="B6" s="32"/>
       <c r="C6" s="32"/>
       <c r="D6" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E6" s="31"/>
       <c r="F6" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>87</v>
@@ -8602,19 +9071,19 @@
       <c r="B7" s="32"/>
       <c r="C7" s="32"/>
       <c r="D7" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>87</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="13" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
@@ -8624,18 +9093,37 @@
       <c r="B8" s="32"/>
       <c r="C8" s="32"/>
       <c r="D8" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>213</v>
+        <v>275</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G8" s="16" t="s">
         <v>97</v>
       </c>
       <c r="H8" s="16"/>
+    </row>
+    <row r="9" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
+      <c r="A9" s="22" t="s">
+        <v>272</v>
+      </c>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="22" t="s">
+        <v>274</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>276</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>278</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A12" s="15" t="s">
@@ -8668,19 +9156,19 @@
         <v>69</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G13" s="15" t="s">
         <v>76</v>
@@ -8694,11 +9182,11 @@
       <c r="B14" s="27"/>
       <c r="C14" s="27"/>
       <c r="D14" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E14" s="30"/>
       <c r="F14" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G14" s="15" t="s">
         <v>76</v>
@@ -8712,11 +9200,11 @@
       <c r="B15" s="27"/>
       <c r="C15" s="27"/>
       <c r="D15" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E15" s="30"/>
       <c r="F15" s="15" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G15" s="15" t="s">
         <v>76</v>
@@ -8730,11 +9218,11 @@
       <c r="B16" s="27"/>
       <c r="C16" s="27"/>
       <c r="D16" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E16" s="31"/>
       <c r="F16" s="15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G16" s="15" t="s">
         <v>76</v>
@@ -8748,19 +9236,19 @@
       <c r="B17" s="27"/>
       <c r="C17" s="27"/>
       <c r="D17" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G17" s="15" t="s">
         <v>76</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="114" x14ac:dyDescent="0.15">
@@ -8770,13 +9258,13 @@
       <c r="B18" s="28"/>
       <c r="C18" s="28"/>
       <c r="D18" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G18" s="16" t="s">
         <v>76</v>
@@ -8787,23 +9275,42 @@
     </row>
     <row r="19" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A19" s="22" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B19" s="23"/>
       <c r="C19" s="23"/>
       <c r="D19" s="22" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F19" s="22" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G19" s="23" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H19" s="23"/>
+    </row>
+    <row r="20" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
+      <c r="A20" s="22" t="s">
+        <v>277</v>
+      </c>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>276</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>278</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>76</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -8827,9 +9334,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H13"/>
+  <dimension ref="A2:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -8876,16 +9383,16 @@
         <v>28</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>217</v>
+        <v>282</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>93</v>
@@ -8899,11 +9406,11 @@
       <c r="B4" s="27"/>
       <c r="C4" s="27"/>
       <c r="D4" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>94</v>
@@ -8917,11 +9424,11 @@
       <c r="B5" s="27"/>
       <c r="C5" s="27"/>
       <c r="D5" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E5" s="30"/>
       <c r="F5" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>92</v>
@@ -8935,11 +9442,11 @@
       <c r="B6" s="27"/>
       <c r="C6" s="27"/>
       <c r="D6" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E6" s="30"/>
       <c r="F6" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>92</v>
@@ -8948,22 +9455,22 @@
     </row>
     <row r="7" spans="1:8" s="13" customFormat="1" ht="156.75" x14ac:dyDescent="0.15">
       <c r="A7" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B7" s="27"/>
       <c r="C7" s="27"/>
       <c r="D7" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E7" s="31"/>
       <c r="F7" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
@@ -8973,13 +9480,13 @@
       <c r="B8" s="27"/>
       <c r="C8" s="27"/>
       <c r="D8" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>76</v>
@@ -8993,11 +9500,11 @@
       <c r="B9" s="27"/>
       <c r="C9" s="27"/>
       <c r="D9" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E9" s="30"/>
       <c r="F9" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>76</v>
@@ -9011,11 +9518,11 @@
       <c r="B10" s="27"/>
       <c r="C10" s="27"/>
       <c r="D10" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E10" s="30"/>
       <c r="F10" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>76</v>
@@ -9029,11 +9536,11 @@
       <c r="B11" s="27"/>
       <c r="C11" s="27"/>
       <c r="D11" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E11" s="30"/>
       <c r="F11" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>76</v>
@@ -9047,38 +9554,76 @@
       <c r="B12" s="28"/>
       <c r="C12" s="28"/>
       <c r="D12" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E12" s="31"/>
       <c r="F12" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A13" s="22" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B13" s="23"/>
       <c r="C13" s="23"/>
       <c r="D13" s="22" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H13" s="23"/>
+    </row>
+    <row r="14" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
+      <c r="A14" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="22" t="s">
+        <v>274</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>283</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>278</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
+      <c r="A15" s="22" t="s">
+        <v>281</v>
+      </c>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>284</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>278</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>76</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -9146,16 +9691,16 @@
         <v>36</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>103</v>
@@ -9176,7 +9721,7 @@
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>85</v>
@@ -9199,7 +9744,7 @@
       </c>
       <c r="E5" s="30"/>
       <c r="F5" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>77</v>
@@ -9232,21 +9777,21 @@
     </row>
     <row r="7" spans="1:9" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A7" s="22" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="23"/>
       <c r="D7" s="22" t="s">
+        <v>237</v>
+      </c>
+      <c r="E7" s="22" t="s">
         <v>239</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="F7" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="G7" s="23" t="s">
         <v>241</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>242</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>243</v>
       </c>
       <c r="H7" s="23"/>
     </row>
@@ -9326,16 +9871,16 @@
         <v>41</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>261</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>263</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>261</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>76</v>
@@ -9373,7 +9918,7 @@
       </c>
       <c r="E5" s="31"/>
       <c r="F5" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>76</v>
@@ -9382,39 +9927,39 @@
     </row>
     <row r="6" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A6" s="22" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B6" s="28"/>
       <c r="C6" s="28"/>
       <c r="D6" s="22" t="s">
+        <v>258</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>262</v>
+      </c>
+      <c r="F6" s="22" t="s">
         <v>260</v>
-      </c>
-      <c r="E6" s="24" t="s">
-        <v>264</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>262</v>
       </c>
       <c r="G6" s="22"/>
       <c r="H6" s="22"/>
     </row>
     <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A7" s="22" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="23"/>
       <c r="D7" s="22" t="s">
+        <v>237</v>
+      </c>
+      <c r="E7" s="22" t="s">
         <v>239</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="F7" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="G7" s="23" t="s">
         <v>241</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>242</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>243</v>
       </c>
       <c r="H7" s="23"/>
     </row>
@@ -9440,7 +9985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -9488,16 +10033,16 @@
         <v>48</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>80</v>
@@ -9511,11 +10056,11 @@
       <c r="B4" s="27"/>
       <c r="C4" s="27"/>
       <c r="D4" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>78</v>
@@ -9529,11 +10074,11 @@
       <c r="B5" s="27"/>
       <c r="C5" s="27"/>
       <c r="D5" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E5" s="30"/>
       <c r="F5" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>79</v>
@@ -9542,19 +10087,19 @@
     </row>
     <row r="6" spans="1:8" s="13" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B6" s="27"/>
       <c r="C6" s="27"/>
       <c r="D6" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E6" s="31"/>
       <c r="F6" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H6" s="11"/>
     </row>
@@ -9565,19 +10110,19 @@
       <c r="B7" s="28"/>
       <c r="C7" s="28"/>
       <c r="D7" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
@@ -9614,16 +10159,16 @@
         <v>49</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>76</v>
@@ -9637,11 +10182,11 @@
       <c r="B12" s="27"/>
       <c r="C12" s="27"/>
       <c r="D12" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E12" s="30"/>
       <c r="F12" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>76</v>
@@ -9655,11 +10200,11 @@
       <c r="B13" s="27"/>
       <c r="C13" s="27"/>
       <c r="D13" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E13" s="30"/>
       <c r="F13" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>76</v>
@@ -9668,16 +10213,16 @@
     </row>
     <row r="14" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A14" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B14" s="27"/>
       <c r="C14" s="27"/>
       <c r="D14" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E14" s="31"/>
       <c r="F14" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>76</v>
@@ -9691,38 +10236,38 @@
       <c r="B15" s="28"/>
       <c r="C15" s="28"/>
       <c r="D15" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>76</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A16" s="22" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="23"/>
       <c r="D16" s="22" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G16" s="23" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H16" s="23"/>
     </row>
@@ -9792,16 +10337,16 @@
         <v>55</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>124</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>76</v>
@@ -9839,7 +10384,7 @@
       </c>
       <c r="E5" s="31"/>
       <c r="F5" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>78</v>
@@ -9848,21 +10393,21 @@
     </row>
     <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A6" s="22" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="23"/>
       <c r="D6" s="22" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H6" s="23"/>
     </row>

</xml_diff>

<commit_message>
Update the test case file again on the afternoon of 12th,June
</commit_message>
<xml_diff>
--- a/src/MyItems/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -7445,6 +7445,307 @@
   </si>
   <si>
     <r>
+      <t>1.找到本地计算机中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要被复制文件的路径和</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>空字符串</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.输入被复制文件夹路径和目标文件夹路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test Case 068</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test Case 069</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the source folder or file path</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:" 输入被复制文件的路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\Alonso.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入需要复制到目标文件夹的路径，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E:\Program Files\Test</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入被复制文件夹的路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入空字符串</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder or file path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入被复制文件夹的路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\Alonso.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input target folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入空字符串</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
       <t>1. 提示请不要输入空的信息 
 （</t>
     </r>
@@ -7470,308 +7771,8 @@
         <scheme val="minor"/>
       </rPr>
       <t>）
-2. 返回重新输入非空字符的文件夹路径，若仍然是空字符串，则继续提示错误，并重新输入</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.找到本地计算机中</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>需要被复制文件的路径和</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>空字符串</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.输入被复制文件夹路径和目标文件夹路径</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test Case 068</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test Case 069</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the source folder or file path</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:" 输入被复制文件的路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\Alonso.txt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the target folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入需要复制到目标文件夹的路径，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E:\Program Files\Test</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入被复制文件夹的路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input target folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入空字符串</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder or file path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入被复制文件夹的路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\Alonso.txt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input target folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入空字符串</t>
+2. 返回重新输入非空字符的文件夹路径，若仍然是空字符串，则继续提示错误，并重新输入
+3. 若输入了正确路径格式，则应被复制成功且能在本地查看到</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -8933,7 +8934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -9106,7 +9107,7 @@
       </c>
       <c r="H8" s="16"/>
     </row>
-    <row r="9" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A9" s="22" t="s">
         <v>272</v>
       </c>
@@ -9119,7 +9120,7 @@
         <v>276</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="G9" s="23" t="s">
         <v>76</v>
@@ -9293,20 +9294,20 @@
       </c>
       <c r="H19" s="23"/>
     </row>
-    <row r="20" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A20" s="22" t="s">
         <v>277</v>
       </c>
       <c r="B20" s="23"/>
       <c r="C20" s="23"/>
       <c r="D20" s="22" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E20" s="22" t="s">
         <v>276</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="G20" s="23" t="s">
         <v>76</v>
@@ -9336,7 +9337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H15"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -9389,7 +9390,7 @@
         <v>147</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>144</v>
@@ -9587,9 +9588,9 @@
       </c>
       <c r="H13" s="23"/>
     </row>
-    <row r="14" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A14" s="22" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B14" s="23"/>
       <c r="C14" s="23"/>
@@ -9597,29 +9598,29 @@
         <v>274</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="G14" s="23" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A15" s="22" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B15" s="23"/>
       <c r="C15" s="23"/>
       <c r="D15" s="22" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E15" s="22" t="s">
+        <v>283</v>
+      </c>
+      <c r="F15" s="22" t="s">
         <v>284</v>
-      </c>
-      <c r="F15" s="22" t="s">
-        <v>278</v>
       </c>
       <c r="G15" s="23" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
Update the test case file on the 16 of 12th,June
</commit_message>
<xml_diff>
--- a/src/MyItems/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -1797,7 +1797,71 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
+      <t>不存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要被复制文件夹的路径和</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>目标路径
+2.输入被复制文件夹路径和目标文件夹路径</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.找到本地计算机中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>都不存在的</t>
     </r>
     <r>
       <rPr>
@@ -1838,111 +1902,6 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>不存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>需要被复制文件夹的路径和</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>目标路径
-2.输入被复制文件夹路径和目标文件夹路径</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t/>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.找到本地计算机中</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>都不存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>需要被复制文件夹的路径和目标路径
-2.输入被复制文件夹路径和目标文件夹路径</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t/>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.找到本地计算机中</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>存在的</t>
     </r>
     <r>
@@ -2018,80 +1977,6 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>需要被复制文件夹的路径和目标路径已经</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.输入被复制文件路径和目标文件夹路径</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t/>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.找到本地计算机中</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>需要被复制文件的路径和目标路径
 2.输入被复制文件路径和目标文件夹路径</t>
     </r>
@@ -2952,7 +2837,181 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>都存在的</t>
+      <t>不存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要被移动的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的路径和</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>目标路径
+2.输入被移动文件路径和目标文件夹路径</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">        </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.找到本地计算机中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要被移动的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的路径和</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>不存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>目标路径
+2.输入被移动文件路径和目标文件夹路径</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.找到本地计算机中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>都不存在的</t>
     </r>
     <r>
       <rPr>
@@ -2992,324 +3051,12 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.找到本地计算机中</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>不存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>需要被移动的</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>的路径和</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>目标路径
-2.输入被移动文件路径和目标文件夹路径</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">        </t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.找到本地计算机中</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>需要被移动的</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>的路径和</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>不存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>目标路径
-2.输入被移动文件路径和目标文件夹路径</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.找到本地计算机中</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>都不存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>需要被移动的</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>的路径和目标路径
-2.输入被移动文件路径和目标文件夹路径</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
         <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">        </t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.找到本地计算机中</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>需要被复制文件夹的路径和目标路径已经</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.输入被复制文件路径和目标文件夹路径</t>
     </r>
     <r>
       <rPr>
@@ -7773,6 +7520,306 @@
       <t>）
 2. 返回重新输入非空字符的文件夹路径，若仍然是空字符串，则继续提示错误，并重新输入
 3. 若输入了正确路径格式，则应被复制成功且能在本地查看到</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.找到本地计算机中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要被复制</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>非空和空</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹的路径和目标路径已经</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.输入被复制文件路径和目标文件夹路径</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.找到本地计算机中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要被复制</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>非空和空</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹的路径和目标路径
+2.输入被复制文件夹路径和目标文件夹路径</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.找到本地计算机中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>都存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要被移动的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>非空和空文件夹</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">的路径和目标路径
+2.输入被移动文件路径和目标文件夹路径       </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.找到本地计算机中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要被复制</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>非空和空</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹的路径和目标路径已经</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.输入被复制文件路径和目标文件夹路径        </t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -8466,16 +8513,16 @@
         <v>57</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>59</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>77</v>
@@ -8493,7 +8540,7 @@
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>78</v>
@@ -8511,7 +8558,7 @@
       </c>
       <c r="E5" s="30"/>
       <c r="F5" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>79</v>
@@ -8529,7 +8576,7 @@
       </c>
       <c r="E6" s="31"/>
       <c r="F6" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>85</v>
@@ -8540,21 +8587,21 @@
     </row>
     <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A7" s="22" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="23"/>
       <c r="D7" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="G7" s="23" t="s">
         <v>237</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>239</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>240</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>241</v>
       </c>
       <c r="H7" s="23"/>
     </row>
@@ -8643,16 +8690,16 @@
         <v>2</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>81</v>
@@ -8669,16 +8716,16 @@
         <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>188</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
@@ -8691,10 +8738,10 @@
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>81</v>
@@ -8747,16 +8794,16 @@
         <v>8</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>76</v>
@@ -8774,16 +8821,16 @@
         <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="I10" s="3"/>
     </row>
@@ -8797,10 +8844,10 @@
         <v>16</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>76</v>
@@ -8810,21 +8857,21 @@
     </row>
     <row r="12" spans="1:9" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A12" s="22" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B12" s="23"/>
       <c r="C12" s="23"/>
       <c r="D12" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="G12" s="23" t="s">
         <v>237</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>244</v>
-      </c>
-      <c r="F12" s="22" t="s">
-        <v>240</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>241</v>
       </c>
       <c r="H12" s="23"/>
     </row>
@@ -8934,7 +8981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -8988,19 +9035,19 @@
         <v>68</v>
       </c>
       <c r="B3" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>262</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="E3" s="29" t="s">
         <v>208</v>
       </c>
-      <c r="C3" s="32" t="s">
-        <v>266</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>212</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>76</v>
@@ -9016,11 +9063,11 @@
       <c r="B4" s="32"/>
       <c r="C4" s="32"/>
       <c r="D4" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>88</v>
@@ -9034,11 +9081,11 @@
       <c r="B5" s="32"/>
       <c r="C5" s="32"/>
       <c r="D5" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="E5" s="30"/>
       <c r="F5" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>76</v>
@@ -9054,11 +9101,11 @@
       <c r="B6" s="32"/>
       <c r="C6" s="32"/>
       <c r="D6" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E6" s="31"/>
       <c r="F6" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>87</v>
@@ -9072,19 +9119,19 @@
       <c r="B7" s="32"/>
       <c r="C7" s="32"/>
       <c r="D7" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>87</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="13" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
@@ -9094,13 +9141,13 @@
       <c r="B8" s="32"/>
       <c r="C8" s="32"/>
       <c r="D8" s="11" t="s">
-        <v>137</v>
+        <v>281</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="G8" s="16" t="s">
         <v>97</v>
@@ -9109,18 +9156,18 @@
     </row>
     <row r="9" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A9" s="22" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
       <c r="D9" s="22" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="G9" s="23" t="s">
         <v>76</v>
@@ -9157,19 +9204,19 @@
         <v>69</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G13" s="15" t="s">
         <v>76</v>
@@ -9183,11 +9230,11 @@
       <c r="B14" s="27"/>
       <c r="C14" s="27"/>
       <c r="D14" s="15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E14" s="30"/>
       <c r="F14" s="15" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="G14" s="15" t="s">
         <v>76</v>
@@ -9201,11 +9248,11 @@
       <c r="B15" s="27"/>
       <c r="C15" s="27"/>
       <c r="D15" s="15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E15" s="30"/>
       <c r="F15" s="15" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="G15" s="15" t="s">
         <v>76</v>
@@ -9219,11 +9266,11 @@
       <c r="B16" s="27"/>
       <c r="C16" s="27"/>
       <c r="D16" s="15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E16" s="31"/>
       <c r="F16" s="15" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="G16" s="15" t="s">
         <v>76</v>
@@ -9237,19 +9284,19 @@
       <c r="B17" s="27"/>
       <c r="C17" s="27"/>
       <c r="D17" s="15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="G17" s="15" t="s">
         <v>76</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="114" x14ac:dyDescent="0.15">
@@ -9259,13 +9306,13 @@
       <c r="B18" s="28"/>
       <c r="C18" s="28"/>
       <c r="D18" s="11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="G18" s="16" t="s">
         <v>76</v>
@@ -9276,38 +9323,38 @@
     </row>
     <row r="19" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A19" s="22" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B19" s="23"/>
       <c r="C19" s="23"/>
       <c r="D19" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="G19" s="23" t="s">
         <v>237</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>244</v>
-      </c>
-      <c r="F19" s="22" t="s">
-        <v>240</v>
-      </c>
-      <c r="G19" s="23" t="s">
-        <v>241</v>
       </c>
       <c r="H19" s="23"/>
     </row>
     <row r="20" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A20" s="22" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B20" s="23"/>
       <c r="C20" s="23"/>
       <c r="D20" s="22" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="G20" s="23" t="s">
         <v>76</v>
@@ -9337,7 +9384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -9384,16 +9431,16 @@
         <v>28</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>93</v>
@@ -9407,11 +9454,11 @@
       <c r="B4" s="27"/>
       <c r="C4" s="27"/>
       <c r="D4" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>94</v>
@@ -9425,11 +9472,11 @@
       <c r="B5" s="27"/>
       <c r="C5" s="27"/>
       <c r="D5" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E5" s="30"/>
       <c r="F5" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>92</v>
@@ -9443,11 +9490,11 @@
       <c r="B6" s="27"/>
       <c r="C6" s="27"/>
       <c r="D6" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E6" s="30"/>
       <c r="F6" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>92</v>
@@ -9456,38 +9503,38 @@
     </row>
     <row r="7" spans="1:8" s="13" customFormat="1" ht="156.75" x14ac:dyDescent="0.15">
       <c r="A7" s="11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B7" s="27"/>
       <c r="C7" s="27"/>
       <c r="D7" s="11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E7" s="31"/>
       <c r="F7" s="11" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B8" s="27"/>
       <c r="C8" s="27"/>
       <c r="D8" s="2" t="s">
-        <v>152</v>
+        <v>283</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>76</v>
@@ -9501,11 +9548,11 @@
       <c r="B9" s="27"/>
       <c r="C9" s="27"/>
       <c r="D9" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E9" s="30"/>
       <c r="F9" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>76</v>
@@ -9519,11 +9566,11 @@
       <c r="B10" s="27"/>
       <c r="C10" s="27"/>
       <c r="D10" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E10" s="30"/>
       <c r="F10" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>76</v>
@@ -9537,11 +9584,11 @@
       <c r="B11" s="27"/>
       <c r="C11" s="27"/>
       <c r="D11" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E11" s="30"/>
       <c r="F11" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>76</v>
@@ -9555,53 +9602,53 @@
       <c r="B12" s="28"/>
       <c r="C12" s="28"/>
       <c r="D12" s="11" t="s">
-        <v>156</v>
+        <v>284</v>
       </c>
       <c r="E12" s="31"/>
       <c r="F12" s="11" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A13" s="22" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B13" s="23"/>
       <c r="C13" s="23"/>
       <c r="D13" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="G13" s="23" t="s">
         <v>237</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>249</v>
-      </c>
-      <c r="F13" s="22" t="s">
-        <v>240</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>241</v>
       </c>
       <c r="H13" s="23"/>
     </row>
     <row r="14" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A14" s="22" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B14" s="23"/>
       <c r="C14" s="23"/>
       <c r="D14" s="22" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="G14" s="23" t="s">
         <v>76</v>
@@ -9609,18 +9656,18 @@
     </row>
     <row r="15" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A15" s="22" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B15" s="23"/>
       <c r="C15" s="23"/>
       <c r="D15" s="22" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="G15" s="23" t="s">
         <v>76</v>
@@ -9692,16 +9739,16 @@
         <v>36</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>103</v>
@@ -9722,7 +9769,7 @@
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="2" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>85</v>
@@ -9745,7 +9792,7 @@
       </c>
       <c r="E5" s="30"/>
       <c r="F5" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>77</v>
@@ -9778,21 +9825,21 @@
     </row>
     <row r="7" spans="1:9" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A7" s="22" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="23"/>
       <c r="D7" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="G7" s="23" t="s">
         <v>237</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>239</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>240</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>241</v>
       </c>
       <c r="H7" s="23"/>
     </row>
@@ -9872,16 +9919,16 @@
         <v>41</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E3" s="29" t="s">
         <v>257</v>
       </c>
-      <c r="E3" s="29" t="s">
-        <v>261</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>76</v>
@@ -9919,7 +9966,7 @@
       </c>
       <c r="E5" s="31"/>
       <c r="F5" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>76</v>
@@ -9928,39 +9975,39 @@
     </row>
     <row r="6" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A6" s="22" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B6" s="28"/>
       <c r="C6" s="28"/>
       <c r="D6" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="E6" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="E6" s="24" t="s">
-        <v>262</v>
-      </c>
       <c r="F6" s="22" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="G6" s="22"/>
       <c r="H6" s="22"/>
     </row>
     <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A7" s="22" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="23"/>
       <c r="D7" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="G7" s="23" t="s">
         <v>237</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>239</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>240</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>241</v>
       </c>
       <c r="H7" s="23"/>
     </row>
@@ -10034,16 +10081,16 @@
         <v>48</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>80</v>
@@ -10057,11 +10104,11 @@
       <c r="B4" s="27"/>
       <c r="C4" s="27"/>
       <c r="D4" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>78</v>
@@ -10075,11 +10122,11 @@
       <c r="B5" s="27"/>
       <c r="C5" s="27"/>
       <c r="D5" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E5" s="30"/>
       <c r="F5" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>79</v>
@@ -10088,19 +10135,19 @@
     </row>
     <row r="6" spans="1:8" s="13" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="11" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B6" s="27"/>
       <c r="C6" s="27"/>
       <c r="D6" s="11" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E6" s="31"/>
       <c r="F6" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="H6" s="11"/>
     </row>
@@ -10111,19 +10158,19 @@
       <c r="B7" s="28"/>
       <c r="C7" s="28"/>
       <c r="D7" s="11" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
@@ -10160,16 +10207,16 @@
         <v>49</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>76</v>
@@ -10183,11 +10230,11 @@
       <c r="B12" s="27"/>
       <c r="C12" s="27"/>
       <c r="D12" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E12" s="30"/>
       <c r="F12" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>76</v>
@@ -10201,11 +10248,11 @@
       <c r="B13" s="27"/>
       <c r="C13" s="27"/>
       <c r="D13" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E13" s="30"/>
       <c r="F13" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>76</v>
@@ -10214,16 +10261,16 @@
     </row>
     <row r="14" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A14" s="11" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B14" s="27"/>
       <c r="C14" s="27"/>
       <c r="D14" s="11" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E14" s="31"/>
       <c r="F14" s="11" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>76</v>
@@ -10237,38 +10284,38 @@
       <c r="B15" s="28"/>
       <c r="C15" s="28"/>
       <c r="D15" s="11" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>76</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A16" s="22" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="23"/>
       <c r="D16" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="G16" s="23" t="s">
         <v>237</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>244</v>
-      </c>
-      <c r="F16" s="22" t="s">
-        <v>240</v>
-      </c>
-      <c r="G16" s="23" t="s">
-        <v>241</v>
       </c>
       <c r="H16" s="23"/>
     </row>
@@ -10338,16 +10385,16 @@
         <v>55</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>124</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>76</v>
@@ -10385,7 +10432,7 @@
       </c>
       <c r="E5" s="31"/>
       <c r="F5" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>78</v>
@@ -10394,21 +10441,21 @@
     </row>
     <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A6" s="22" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="23"/>
       <c r="D6" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="G6" s="23" t="s">
         <v>237</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>244</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>240</v>
-      </c>
-      <c r="G6" s="23" t="s">
-        <v>241</v>
       </c>
       <c r="H6" s="23"/>
     </row>

</xml_diff>

<commit_message>
Update the test case file before 17 on 12th,June
</commit_message>
<xml_diff>
--- a/src/MyItems/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Test Cases for FileOperation.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="284">
   <si>
     <t>删除文件夹</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1755,66 +1755,6 @@
   </si>
   <si>
     <r>
-      <t>1.显示指定的文件已经成功的移动到了新路径中（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\Alonso.txt have been moved to E:\Program Files\Test\Alonso.txt succeeded!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.本地计算机中能查到新文件路径</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.显示指定的文件夹已经成功的移动到了新路径中（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test have been moved to E:\Program Files\Test succeeded!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.本地计算机中能查到新文件夹路径</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>1.找到本地计算机中</t>
     </r>
     <r>
@@ -2233,68 +2173,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>1.新建目标文件夹
-2.显示文件被移动到新建文件夹内（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\Alonso.txt have been moved to E:\Program Files8\Alonso.txt succeeded!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-3.本地计算机中能查到新文件路径</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.新建目标文件夹
-2.显示文件被移动到新建文件夹内（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E:\Program Files\Test\Test have been moved to D:\ succeeded!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-3.本地计算机中能查到新文件夹路径</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Pass</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2871,61 +2749,6 @@
       </rPr>
       <t>)
 2.本地计算机上该文件夹确实被删除</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.检查是否会提示“覆盖”信息
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>There is a same file on target file , would you still want to move? (Y/N)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.若选择覆盖后，原有文件应被移动替换为新的文件 （</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\Alonso.txt have been moved to E:\Program Files\Test\Alonso.txt succeeded!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-3.本地计算机中能查到新文件路径</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3994,37 +3817,6 @@
   </si>
   <si>
     <r>
-      <t>1.显示文件成功被复制到指定路径（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\But.txt has been copied to E:\Program Files succeeded!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.本地计算机上存在复制后的新文件
-3.若目标文件路径已存在，则有会提示覆盖与否，并复制到该文件夹中，不删除原有文件</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>1.检查是否会提示“覆盖”信息
 （</t>
     </r>
@@ -4063,67 +3855,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>D:\Test33 have copied succeeded to folder E:\Program Files\Test33</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.显示文件夹成功被复制到指定路径（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test33 have copied succeeded to folder E:\Program Files\Test33</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.本地计算机上存在复制后的新路径
-3.若目标文件夹路径已存在，则会提示是否删除原文件夹，并重新复制到该文件夹中</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.新创建目标文件夹
-2.文件夹复制到新创建的指定路径，且目录下包含原名称的子文件夹（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test33 have copied succeeded to folder E:\Program Files\McL\Test33</t>
     </r>
     <r>
       <rPr>
@@ -7810,6 +7541,359 @@
       </rPr>
       <t>）
 2.文件不应该被移动到指定路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示文件夹成功被复制到指定路径（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test33 has copied succeeded to folder E:\Program Files</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.本地计算机上存在复制后的新路径
+3.若目标文件夹路径已存在，则会提示是否删除原文件夹，并重新复制到该文件夹中</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.新创建目标文件夹
+2.文件夹复制到新创建的指定路径，且目录下包含原名称的子文件夹（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test33 has copied succeeded to folder E:\Program Files\McL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.检查是否会提示“覆盖”信息
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>There is a same folder on target folder , would you still want to copy? (Y/N)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.若选择覆盖，则被复制的文件夹内的内容会被复制到目标文件夹内（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test33 has copied succeeded to folder E:\Program Files</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示文件成功被复制到指定路径（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\But.txt has been copied to E:\Program Files succeeded!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.本地计算机上存在复制后的新文件
+3.若目标文件路径已存在，则有会提示覆盖与否，并复制到该文件夹中，不删除原有文件</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示指定的文件已经成功的移动到了新路径中（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alonso.txt has been moved from D:\Test\ to E:\Program Files\Test succeeded!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.本地计算机中能查到新文件路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.新建目标文件夹
+2.显示文件被移动到新建文件夹内（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alonso.txt has been moved from D:\Test\ to E:\Program Files\Test succeeded!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+3.本地计算机中能查到新文件路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.检查是否会提示“覆盖”信息
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>There is a same file on target file , would you still want to move? (Y/N)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.若选择覆盖后，原有文件应被移动替换为新的文件 （</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alonso.txt has been moved from D:\Test\ to E:\Program Files\Test succeeded!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+3.本地计算机中能查到新文件路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示指定的文件夹已经成功的移动到了新路径中（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test has been moved from D: to E:\Program Files succeeded!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.本地计算机中能查到新文件夹路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示指定的文件夹已经成功的移动到了新路径中（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test has been moved from D: to E:\Program Files succeeded!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.本地计算机中能查到新文件夹路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.新建目标文件夹
+2.显示文件被移动到新建文件夹内（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test has been moved from D: to E:\Program Files succeeded!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+3.本地计算机中能查到新文件夹路径</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -8133,6 +8217,30 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -8160,15 +8268,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -8181,32 +8280,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8532,14 +8616,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="36"/>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
+      <c r="A1" s="44"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -8571,20 +8655,20 @@
       <c r="A3" s="22">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="40" t="s">
-        <v>158</v>
+      <c r="C3" s="48" t="s">
+        <v>150</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="37" t="s">
-        <v>142</v>
+      <c r="E3" s="45" t="s">
+        <v>134</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>33</v>
@@ -8595,14 +8679,14 @@
       <c r="A4" s="22">
         <v>1.2</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
       <c r="D4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="38"/>
+      <c r="E4" s="46"/>
       <c r="F4" s="2" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>34</v>
@@ -8613,14 +8697,14 @@
       <c r="A5" s="22">
         <v>1.3</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
       <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="38"/>
+      <c r="E5" s="46"/>
       <c r="F5" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>35</v>
@@ -8631,14 +8715,14 @@
       <c r="A6" s="22">
         <v>1.4</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
       <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="39"/>
+      <c r="E6" s="47"/>
       <c r="F6" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>38</v>
@@ -8649,19 +8733,19 @@
       <c r="A7" s="27">
         <v>1.5</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
       <c r="D7" s="20" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="H7" s="21"/>
     </row>
@@ -8703,14 +8787,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="48"/>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
+      <c r="A1" s="53"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -8742,23 +8826,23 @@
       <c r="A3" s="22">
         <v>10.1</v>
       </c>
-      <c r="B3" s="52" t="s">
-        <v>215</v>
-      </c>
-      <c r="C3" s="52" t="s">
-        <v>216</v>
-      </c>
-      <c r="D3" s="52" t="s">
-        <v>217</v>
+      <c r="B3" s="60" t="s">
+        <v>207</v>
+      </c>
+      <c r="C3" s="60" t="s">
+        <v>208</v>
+      </c>
+      <c r="D3" s="60" t="s">
+        <v>209</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -8766,17 +8850,17 @@
       <c r="A4" s="22">
         <v>10.199999999999999</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
       <c r="E4" s="2" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -8784,17 +8868,17 @@
       <c r="A5" s="22">
         <v>10.3</v>
       </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
       <c r="E5" s="2" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -8802,17 +8886,17 @@
       <c r="A6" s="22">
         <v>10.4</v>
       </c>
-      <c r="B6" s="52"/>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
       <c r="E6" s="2" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="H6" s="5"/>
     </row>
@@ -8820,17 +8904,17 @@
       <c r="A7" s="22">
         <v>10.5</v>
       </c>
-      <c r="B7" s="52"/>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
       <c r="E7" s="2" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="H7" s="5"/>
     </row>
@@ -8838,17 +8922,17 @@
       <c r="A8" s="22">
         <v>10.6</v>
       </c>
-      <c r="B8" s="52"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
       <c r="E8" s="2" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="H8" s="5"/>
     </row>
@@ -8856,17 +8940,17 @@
       <c r="A9" s="22">
         <v>10.7</v>
       </c>
-      <c r="B9" s="52"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
       <c r="E9" s="2" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="H9" s="5"/>
     </row>
@@ -8874,17 +8958,17 @@
       <c r="A10" s="22">
         <v>10.8</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
       <c r="E10" s="2" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="H10" s="5"/>
     </row>
@@ -8892,35 +8976,35 @@
       <c r="A11" s="22">
         <v>10.9</v>
       </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
       <c r="E11" s="2" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A12" s="29" t="s">
-        <v>228</v>
-      </c>
-      <c r="B12" s="52"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
+        <v>220</v>
+      </c>
+      <c r="B12" s="60"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
       <c r="E12" s="2" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="H12" s="5"/>
     </row>
@@ -8958,14 +9042,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="36"/>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
+      <c r="A1" s="44"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -8995,22 +9079,22 @@
     </row>
     <row r="3" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B3" s="40" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="40" t="s">
-        <v>159</v>
+      <c r="C3" s="48" t="s">
+        <v>151</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>37</v>
@@ -9019,18 +9103,18 @@
     </row>
     <row r="4" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
+        <v>166</v>
+      </c>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
       <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>32</v>
@@ -9039,18 +9123,18 @@
     </row>
     <row r="5" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
+        <v>167</v>
+      </c>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
       <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>37</v>
@@ -9059,18 +9143,18 @@
     </row>
     <row r="6" spans="1:9" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A6" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
+        <v>172</v>
+      </c>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="20" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="G6" s="21" t="s">
         <v>32</v>
@@ -9117,22 +9201,22 @@
     </row>
     <row r="9" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="B9" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="B9" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="40" t="s">
-        <v>159</v>
+      <c r="C9" s="48" t="s">
+        <v>151</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>32</v>
@@ -9142,41 +9226,41 @@
     </row>
     <row r="10" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
+        <v>169</v>
+      </c>
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
       <c r="D10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
+        <v>170</v>
+      </c>
+      <c r="B11" s="49"/>
+      <c r="C11" s="49"/>
       <c r="D11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>32</v>
@@ -9186,27 +9270,27 @@
     </row>
     <row r="12" spans="1:9" s="23" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A12" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
+        <v>171</v>
+      </c>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
       <c r="D12" s="20" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="G12" s="21" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="H12" s="21"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
-      <c r="B13" s="43"/>
+      <c r="B13" s="51"/>
       <c r="C13" s="4"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -9217,7 +9301,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
-      <c r="B14" s="43"/>
+      <c r="B14" s="51"/>
       <c r="C14" s="4"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -9228,7 +9312,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
-      <c r="B15" s="43"/>
+      <c r="B15" s="51"/>
       <c r="C15" s="4"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -9239,7 +9323,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
-      <c r="B16" s="43"/>
+      <c r="B16" s="51"/>
       <c r="C16" s="4"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -9250,7 +9334,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
-      <c r="B17" s="43"/>
+      <c r="B17" s="51"/>
       <c r="C17" s="4"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -9326,14 +9410,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A1" s="44"/>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
+      <c r="A1" s="52"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -9363,22 +9447,22 @@
     </row>
     <row r="3" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="B3" s="40" t="s">
-        <v>119</v>
-      </c>
-      <c r="C3" s="40" t="s">
-        <v>161</v>
+        <v>176</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>153</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E3" s="37" t="s">
-        <v>123</v>
+        <v>173</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>118</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>132</v>
+        <v>274</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>32</v>
@@ -9387,16 +9471,16 @@
     </row>
     <row r="4" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
+        <v>177</v>
+      </c>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
       <c r="D4" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="E4" s="38"/>
+        <v>174</v>
+      </c>
+      <c r="E4" s="46"/>
       <c r="F4" s="2" t="s">
-        <v>132</v>
+        <v>274</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>32</v>
@@ -9405,16 +9489,16 @@
     </row>
     <row r="5" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
+        <v>178</v>
+      </c>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
       <c r="D5" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E5" s="38"/>
+      <c r="E5" s="46"/>
       <c r="F5" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>40</v>
@@ -9423,16 +9507,16 @@
     </row>
     <row r="6" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
+        <v>179</v>
+      </c>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
       <c r="D6" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E6" s="38"/>
+        <v>159</v>
+      </c>
+      <c r="E6" s="46"/>
       <c r="F6" s="2" t="s">
-        <v>133</v>
+        <v>275</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>32</v>
@@ -9441,16 +9525,16 @@
     </row>
     <row r="7" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
+        <v>180</v>
+      </c>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
       <c r="D7" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="38"/>
+      <c r="E7" s="46"/>
       <c r="F7" s="2" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>39</v>
@@ -9459,16 +9543,16 @@
     </row>
     <row r="8" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A8" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
+        <v>181</v>
+      </c>
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
       <c r="D8" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="E8" s="38"/>
+        <v>175</v>
+      </c>
+      <c r="E8" s="46"/>
       <c r="F8" s="19" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>44</v>
@@ -9477,16 +9561,16 @@
     </row>
     <row r="9" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
+        <v>182</v>
+      </c>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
       <c r="D9" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="E9" s="38"/>
+        <v>254</v>
+      </c>
+      <c r="E9" s="46"/>
       <c r="F9" s="19" t="s">
-        <v>131</v>
+        <v>276</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>32</v>
@@ -9494,37 +9578,37 @@
       <c r="H9" s="15"/>
     </row>
     <row r="10" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
-      <c r="A10" s="53" t="s">
-        <v>266</v>
-      </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="53" t="s">
-        <v>270</v>
-      </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="54" t="s">
-        <v>264</v>
-      </c>
-      <c r="G10" s="55" t="s">
-        <v>265</v>
-      </c>
-      <c r="H10" s="55"/>
+      <c r="A10" s="36" t="s">
+        <v>258</v>
+      </c>
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="36" t="s">
+        <v>262</v>
+      </c>
+      <c r="E10" s="47"/>
+      <c r="F10" s="37" t="s">
+        <v>256</v>
+      </c>
+      <c r="G10" s="38" t="s">
+        <v>257</v>
+      </c>
+      <c r="H10" s="38"/>
     </row>
     <row r="11" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A11" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
+        <v>259</v>
+      </c>
+      <c r="B11" s="49"/>
+      <c r="C11" s="49"/>
       <c r="D11" s="20" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="G11" s="21" t="s">
         <v>32</v>
@@ -9533,18 +9617,18 @@
     </row>
     <row r="12" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A12" s="20" t="s">
-        <v>268</v>
-      </c>
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
+        <v>260</v>
+      </c>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
       <c r="D12" s="20" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="G12" s="21" t="s">
         <v>32</v>
@@ -9579,22 +9663,22 @@
     </row>
     <row r="16" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A16" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="B16" s="40" t="s">
-        <v>120</v>
-      </c>
-      <c r="C16" s="40" t="s">
-        <v>160</v>
+        <v>185</v>
+      </c>
+      <c r="B16" s="48" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" s="48" t="s">
+        <v>152</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E16" s="37" t="s">
-        <v>124</v>
+        <v>183</v>
+      </c>
+      <c r="E16" s="45" t="s">
+        <v>119</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>130</v>
+        <v>277</v>
       </c>
       <c r="G16" s="14" t="s">
         <v>32</v>
@@ -9603,16 +9687,16 @@
     </row>
     <row r="17" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A17" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
+        <v>186</v>
+      </c>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
       <c r="D17" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="38"/>
+      <c r="E17" s="46"/>
       <c r="F17" s="14" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="G17" s="14" t="s">
         <v>32</v>
@@ -9621,16 +9705,16 @@
     </row>
     <row r="18" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A18" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
+        <v>187</v>
+      </c>
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
       <c r="D18" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="E18" s="38"/>
+      <c r="E18" s="46"/>
       <c r="F18" s="14" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="G18" s="14" t="s">
         <v>32</v>
@@ -9639,16 +9723,16 @@
     </row>
     <row r="19" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A19" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
+        <v>188</v>
+      </c>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
       <c r="D19" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="E19" s="38"/>
+      <c r="E19" s="46"/>
       <c r="F19" s="14" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G19" s="14" t="s">
         <v>32</v>
@@ -9657,16 +9741,16 @@
     </row>
     <row r="20" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A20" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
+        <v>189</v>
+      </c>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
       <c r="D20" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="E20" s="38"/>
+        <v>184</v>
+      </c>
+      <c r="E20" s="46"/>
       <c r="F20" s="11" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G20" s="15" t="s">
         <v>32</v>
@@ -9674,57 +9758,57 @@
       <c r="H20" s="16"/>
     </row>
     <row r="21" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
-      <c r="A21" s="53" t="s">
-        <v>271</v>
-      </c>
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="53" t="s">
-        <v>269</v>
-      </c>
-      <c r="E21" s="39"/>
-      <c r="F21" s="54" t="s">
-        <v>273</v>
-      </c>
-      <c r="G21" s="55" t="s">
+      <c r="A21" s="36" t="s">
+        <v>263</v>
+      </c>
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="36" t="s">
+        <v>261</v>
+      </c>
+      <c r="E21" s="47"/>
+      <c r="F21" s="37" t="s">
         <v>265</v>
       </c>
-      <c r="H21" s="55"/>
+      <c r="G21" s="38" t="s">
+        <v>257</v>
+      </c>
+      <c r="H21" s="38"/>
     </row>
     <row r="22" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A22" s="20" t="s">
-        <v>198</v>
-      </c>
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
+        <v>190</v>
+      </c>
+      <c r="B22" s="49"/>
+      <c r="C22" s="49"/>
       <c r="D22" s="20" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="H22" s="21"/>
     </row>
     <row r="23" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A23" s="20" t="s">
-        <v>272</v>
-      </c>
-      <c r="B23" s="42"/>
-      <c r="C23" s="42"/>
+        <v>264</v>
+      </c>
+      <c r="B23" s="50"/>
+      <c r="C23" s="50"/>
       <c r="D23" s="20" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="G23" s="21" t="s">
         <v>32</v>
@@ -9768,14 +9852,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="48"/>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
+      <c r="A1" s="53"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -9805,22 +9889,22 @@
     </row>
     <row r="3" spans="1:8" s="23" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="B3" s="49" t="s">
-        <v>239</v>
-      </c>
-      <c r="C3" s="49" t="s">
-        <v>162</v>
+        <v>240</v>
+      </c>
+      <c r="B3" s="54" t="s">
+        <v>231</v>
+      </c>
+      <c r="C3" s="54" t="s">
+        <v>154</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="E3" s="45" t="s">
-        <v>169</v>
+        <v>236</v>
+      </c>
+      <c r="E3" s="57" t="s">
+        <v>161</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>72</v>
+        <v>278</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>42</v>
@@ -9829,16 +9913,16 @@
     </row>
     <row r="4" spans="1:8" s="23" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
+        <v>241</v>
+      </c>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
       <c r="D4" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="E4" s="46"/>
+        <v>233</v>
+      </c>
+      <c r="E4" s="58"/>
       <c r="F4" s="6" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>43</v>
@@ -9847,16 +9931,16 @@
     </row>
     <row r="5" spans="1:8" s="23" customFormat="1" ht="114" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
+        <v>242</v>
+      </c>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
       <c r="D5" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E5" s="46"/>
+        <v>72</v>
+      </c>
+      <c r="E5" s="58"/>
       <c r="F5" s="6" t="s">
-        <v>79</v>
+        <v>279</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>41</v>
@@ -9865,16 +9949,16 @@
     </row>
     <row r="6" spans="1:8" s="23" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
+        <v>243</v>
+      </c>
+      <c r="B6" s="55"/>
+      <c r="C6" s="55"/>
       <c r="D6" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="E6" s="46"/>
+        <v>73</v>
+      </c>
+      <c r="E6" s="58"/>
       <c r="F6" s="6" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G6" s="25" t="s">
         <v>41</v>
@@ -9883,54 +9967,54 @@
     </row>
     <row r="7" spans="1:8" s="23" customFormat="1" ht="156.75" x14ac:dyDescent="0.15">
       <c r="A7" s="30" t="s">
-        <v>252</v>
-      </c>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
+        <v>244</v>
+      </c>
+      <c r="B7" s="55"/>
+      <c r="C7" s="55"/>
       <c r="D7" s="30" t="s">
-        <v>245</v>
-      </c>
-      <c r="E7" s="46"/>
+        <v>237</v>
+      </c>
+      <c r="E7" s="58"/>
       <c r="F7" s="30" t="s">
-        <v>102</v>
+        <v>280</v>
       </c>
       <c r="G7" s="31" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H7" s="32"/>
     </row>
     <row r="8" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
-      <c r="A8" s="56" t="s">
-        <v>276</v>
-      </c>
-      <c r="B8" s="50"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="53" t="s">
-        <v>279</v>
-      </c>
-      <c r="E8" s="47"/>
-      <c r="F8" s="54" t="s">
-        <v>281</v>
-      </c>
-      <c r="G8" s="57" t="s">
-        <v>265</v>
-      </c>
-      <c r="H8" s="58"/>
+      <c r="A8" s="39" t="s">
+        <v>268</v>
+      </c>
+      <c r="B8" s="55"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="36" t="s">
+        <v>271</v>
+      </c>
+      <c r="E8" s="59"/>
+      <c r="F8" s="37" t="s">
+        <v>273</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="H8" s="41"/>
     </row>
     <row r="9" spans="1:8" s="23" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A9" s="20" t="s">
-        <v>253</v>
-      </c>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
+        <v>245</v>
+      </c>
+      <c r="B9" s="55"/>
+      <c r="C9" s="55"/>
       <c r="D9" s="20" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="G9" s="21" t="s">
         <v>32</v>
@@ -9939,18 +10023,18 @@
     </row>
     <row r="10" spans="1:8" s="34" customFormat="1" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A10" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="B10" s="51"/>
-      <c r="C10" s="51"/>
+        <v>267</v>
+      </c>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
       <c r="D10" s="20" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="G10" s="21" t="s">
         <v>32</v>
@@ -9994,22 +10078,22 @@
     </row>
     <row r="13" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="B13" s="40" t="s">
-        <v>240</v>
-      </c>
-      <c r="C13" s="49" t="s">
-        <v>162</v>
+        <v>246</v>
+      </c>
+      <c r="B13" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="C13" s="54" t="s">
+        <v>154</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="E13" s="37" t="s">
-        <v>148</v>
+        <v>234</v>
+      </c>
+      <c r="E13" s="45" t="s">
+        <v>140</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>73</v>
+        <v>281</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>32</v>
@@ -10018,16 +10102,16 @@
     </row>
     <row r="14" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="50"/>
+        <v>247</v>
+      </c>
+      <c r="B14" s="49"/>
+      <c r="C14" s="55"/>
       <c r="D14" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="E14" s="38"/>
+        <v>235</v>
+      </c>
+      <c r="E14" s="46"/>
       <c r="F14" s="2" t="s">
-        <v>73</v>
+        <v>282</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>32</v>
@@ -10036,16 +10120,16 @@
     </row>
     <row r="15" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="B15" s="41"/>
-      <c r="C15" s="50"/>
+        <v>248</v>
+      </c>
+      <c r="B15" s="49"/>
+      <c r="C15" s="55"/>
       <c r="D15" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E15" s="38"/>
+        <v>74</v>
+      </c>
+      <c r="E15" s="46"/>
       <c r="F15" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>32</v>
@@ -10054,16 +10138,16 @@
     </row>
     <row r="16" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="50"/>
+        <v>249</v>
+      </c>
+      <c r="B16" s="49"/>
+      <c r="C16" s="55"/>
       <c r="D16" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E16" s="38"/>
+        <v>75</v>
+      </c>
+      <c r="E16" s="46"/>
       <c r="F16" s="2" t="s">
-        <v>80</v>
+        <v>283</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>32</v>
@@ -10072,16 +10156,16 @@
     </row>
     <row r="17" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="50"/>
+        <v>250</v>
+      </c>
+      <c r="B17" s="49"/>
+      <c r="C17" s="55"/>
       <c r="D17" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E17" s="38"/>
+        <v>76</v>
+      </c>
+      <c r="E17" s="46"/>
       <c r="F17" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>32</v>
@@ -10090,34 +10174,34 @@
     </row>
     <row r="18" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A18" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="50"/>
+        <v>251</v>
+      </c>
+      <c r="B18" s="49"/>
+      <c r="C18" s="55"/>
       <c r="D18" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="E18" s="38"/>
+        <v>239</v>
+      </c>
+      <c r="E18" s="46"/>
       <c r="F18" s="11" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H18" s="16"/>
     </row>
     <row r="19" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A19" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="50"/>
+        <v>252</v>
+      </c>
+      <c r="B19" s="49"/>
+      <c r="C19" s="55"/>
       <c r="D19" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="E19" s="38"/>
+        <v>238</v>
+      </c>
+      <c r="E19" s="46"/>
       <c r="F19" s="11" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G19" s="12" t="s">
         <v>32</v>
@@ -10125,57 +10209,57 @@
       <c r="H19" s="16"/>
     </row>
     <row r="20" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
-      <c r="A20" s="53" t="s">
-        <v>278</v>
-      </c>
-      <c r="B20" s="41"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="53" t="s">
-        <v>280</v>
-      </c>
-      <c r="E20" s="39"/>
-      <c r="F20" s="54" t="s">
-        <v>277</v>
-      </c>
-      <c r="G20" s="59" t="s">
-        <v>265</v>
-      </c>
-      <c r="H20" s="60"/>
+      <c r="A20" s="36" t="s">
+        <v>270</v>
+      </c>
+      <c r="B20" s="49"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="36" t="s">
+        <v>272</v>
+      </c>
+      <c r="E20" s="47"/>
+      <c r="F20" s="37" t="s">
+        <v>269</v>
+      </c>
+      <c r="G20" s="42" t="s">
+        <v>257</v>
+      </c>
+      <c r="H20" s="43"/>
     </row>
     <row r="21" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A21" s="20" t="s">
-        <v>261</v>
-      </c>
-      <c r="B21" s="41"/>
-      <c r="C21" s="50"/>
+        <v>253</v>
+      </c>
+      <c r="B21" s="49"/>
+      <c r="C21" s="55"/>
       <c r="D21" s="20" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="G21" s="21" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="H21" s="21"/>
     </row>
     <row r="22" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A22" s="20" t="s">
-        <v>274</v>
-      </c>
-      <c r="B22" s="42"/>
-      <c r="C22" s="51"/>
+        <v>266</v>
+      </c>
+      <c r="B22" s="50"/>
+      <c r="C22" s="56"/>
       <c r="D22" s="20" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="G22" s="21" t="s">
         <v>32</v>
@@ -10219,14 +10303,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="48"/>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
+      <c r="A1" s="53"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -10258,20 +10342,20 @@
       <c r="A3" s="22">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="40" t="s">
-        <v>163</v>
+      <c r="C3" s="48" t="s">
+        <v>155</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="37" t="s">
-        <v>150</v>
+      <c r="E3" s="45" t="s">
+        <v>142</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>45</v>
@@ -10282,14 +10366,14 @@
       <c r="A4" s="22">
         <v>5.2</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
       <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="38"/>
+      <c r="E4" s="46"/>
       <c r="F4" s="2" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>38</v>
@@ -10300,14 +10384,14 @@
       <c r="A5" s="22">
         <v>5.3</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
       <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="38"/>
+      <c r="E5" s="46"/>
       <c r="F5" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>33</v>
@@ -10318,12 +10402,12 @@
       <c r="A6" s="22">
         <v>5.4</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
       <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="39"/>
+      <c r="E6" s="47"/>
       <c r="F6" s="2" t="s">
         <v>59</v>
       </c>
@@ -10336,19 +10420,19 @@
       <c r="A7" s="27">
         <v>5.5</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
       <c r="D7" s="20" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="H7" s="21"/>
     </row>
@@ -10391,14 +10475,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="48"/>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
+      <c r="A1" s="53"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -10430,20 +10514,20 @@
       <c r="A3" s="22">
         <v>6.1</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="40" t="s">
-        <v>164</v>
+      <c r="C3" s="48" t="s">
+        <v>156</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E3" s="37" t="s">
-        <v>156</v>
+        <v>144</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>148</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>32</v>
@@ -10454,12 +10538,12 @@
       <c r="A4" s="22">
         <v>6.2</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
       <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="38"/>
+      <c r="E4" s="46"/>
       <c r="F4" s="2" t="s">
         <v>60</v>
       </c>
@@ -10472,14 +10556,14 @@
       <c r="A5" s="22">
         <v>6.3</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
       <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="39"/>
+      <c r="E5" s="47"/>
       <c r="F5" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>32</v>
@@ -10490,19 +10574,19 @@
       <c r="A6" s="24">
         <v>6.4</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
       <c r="D6" s="6" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="H6" s="6"/>
     </row>
@@ -10510,19 +10594,19 @@
       <c r="A7" s="27">
         <v>6.5</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
       <c r="D7" s="20" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="H7" s="21"/>
     </row>
@@ -10563,14 +10647,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="48"/>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
+      <c r="A1" s="53"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -10600,22 +10684,22 @@
     </row>
     <row r="3" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="B3" s="40" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="40" t="s">
-        <v>165</v>
+      <c r="C3" s="48" t="s">
+        <v>157</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E3" s="37" t="s">
-        <v>125</v>
+        <v>82</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>120</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>36</v>
@@ -10624,16 +10708,16 @@
     </row>
     <row r="4" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
+        <v>196</v>
+      </c>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
       <c r="D4" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E4" s="38"/>
+        <v>83</v>
+      </c>
+      <c r="E4" s="46"/>
       <c r="F4" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>34</v>
@@ -10642,16 +10726,16 @@
     </row>
     <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
+        <v>197</v>
+      </c>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
       <c r="D5" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E5" s="38"/>
+        <v>84</v>
+      </c>
+      <c r="E5" s="46"/>
       <c r="F5" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>35</v>
@@ -10660,36 +10744,36 @@
     </row>
     <row r="6" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
+        <v>198</v>
+      </c>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
       <c r="D6" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" s="47"/>
+      <c r="F6" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>89</v>
-      </c>
-      <c r="E6" s="39"/>
-      <c r="F6" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>93</v>
       </c>
       <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A7" s="20" t="s">
-        <v>207</v>
-      </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
+        <v>199</v>
+      </c>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
       <c r="D7" s="20" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="G7" s="21" t="s">
         <v>32</v>
@@ -10724,22 +10808,22 @@
     </row>
     <row r="10" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="B10" s="40" t="s">
+        <v>200</v>
+      </c>
+      <c r="B10" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="40" t="s">
-        <v>99</v>
+      <c r="C10" s="48" t="s">
+        <v>95</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E10" s="37" t="s">
-        <v>126</v>
+        <v>80</v>
+      </c>
+      <c r="E10" s="45" t="s">
+        <v>121</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>32</v>
@@ -10748,16 +10832,16 @@
     </row>
     <row r="11" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
+        <v>201</v>
+      </c>
+      <c r="B11" s="49"/>
+      <c r="C11" s="49"/>
       <c r="D11" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" s="38"/>
+        <v>81</v>
+      </c>
+      <c r="E11" s="46"/>
       <c r="F11" s="2" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>32</v>
@@ -10766,16 +10850,16 @@
     </row>
     <row r="12" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
+        <v>202</v>
+      </c>
+      <c r="B12" s="49"/>
+      <c r="C12" s="49"/>
       <c r="D12" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E12" s="38"/>
+        <v>86</v>
+      </c>
+      <c r="E12" s="46"/>
       <c r="F12" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>32</v>
@@ -10784,16 +10868,16 @@
     </row>
     <row r="13" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
+        <v>203</v>
+      </c>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
       <c r="D13" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E13" s="39"/>
+        <v>88</v>
+      </c>
+      <c r="E13" s="47"/>
       <c r="F13" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>32</v>
@@ -10802,21 +10886,21 @@
     </row>
     <row r="14" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A14" s="20" t="s">
-        <v>212</v>
-      </c>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
+        <v>204</v>
+      </c>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
       <c r="D14" s="20" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="H14" s="21"/>
     </row>
@@ -10856,14 +10940,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="48"/>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
+      <c r="A1" s="53"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -10895,38 +10979,38 @@
       <c r="A3" s="22">
         <v>8.1</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="40" t="s">
-        <v>166</v>
+      <c r="C3" s="48" t="s">
+        <v>158</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="E3" s="37" t="s">
-        <v>151</v>
+        <v>205</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>143</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>32</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A4" s="22">
         <v>8.1999999999999993</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
       <c r="D4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="38"/>
+      <c r="E4" s="46"/>
       <c r="F4" s="2" t="s">
         <v>61</v>
       </c>
@@ -10939,14 +11023,14 @@
       <c r="A5" s="22">
         <v>8.3000000000000007</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
       <c r="D5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="39"/>
+      <c r="E5" s="47"/>
       <c r="F5" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>34</v>
@@ -10957,19 +11041,19 @@
       <c r="A6" s="27">
         <v>8.4</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="20" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="H6" s="21"/>
     </row>
@@ -11011,14 +11095,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="48"/>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
+      <c r="A1" s="53"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -11050,10 +11134,10 @@
       <c r="A3" s="22">
         <v>9.1</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="48" t="s">
         <v>47</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -11062,7 +11146,7 @@
       <c r="E3" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="48" t="s">
         <v>52</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -11074,15 +11158,15 @@
       <c r="A4" s="22">
         <v>9.1999999999999993</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
       <c r="D4" s="2" t="s">
         <v>49</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="41"/>
+      <c r="F4" s="49"/>
       <c r="G4" s="2" t="s">
         <v>54</v>
       </c>
@@ -11092,15 +11176,15 @@
       <c r="A5" s="22">
         <v>9.3000000000000007</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
       <c r="D5" s="2" t="s">
         <v>50</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="49"/>
       <c r="G5" s="2" t="s">
         <v>54</v>
       </c>
@@ -11110,15 +11194,15 @@
       <c r="A6" s="22">
         <v>9.4</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
       <c r="D6" s="2" t="s">
         <v>51</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="49"/>
       <c r="G6" s="5" t="s">
         <v>54</v>
       </c>
@@ -11128,15 +11212,15 @@
       <c r="A7" s="22">
         <v>9.5</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
       <c r="D7" s="2" t="s">
         <v>53</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="42"/>
+      <c r="F7" s="50"/>
       <c r="G7" s="5" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
Update the test case file on the morning of 15th,Jun
</commit_message>
<xml_diff>
--- a/src/MyItems/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -9394,7 +9394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -9835,7 +9835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update the test case file on the 9am of 15th,June
</commit_message>
<xml_diff>
--- a/src/MyItems/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -4722,346 +4722,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>1.输入</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹路径
-2.输入文件夹下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件名</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.输入</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹路径
-2.输入文件夹下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹名</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.能够出现提示输入的信息
-2.显示指定文件被找到的信息（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>File: 456.txt has found on D:\Test1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.能够出现提示输入的信息
-2.显示指定文件被找到的信息（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Folder: McLaren has found on D:\Test9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What file or folder you want to find on this folder?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入文件名，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>456.txt</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder path</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What file or folder you want to find on this folder?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入文件夹名，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>McLaren</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1. Replace content on txt files</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -7894,6 +7554,350 @@
       </rPr>
       <t>）
 3.本地计算机中能查到新文件夹路径</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹路径
+2.输入文件夹下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件名或扩展名</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹路径
+2.输入文件夹下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹名</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What file or folder you want to find on this folder?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入文件名或扩展名，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.txt，456.txt,20170614</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What file or folder you want to find on this folder?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入文件夹名，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>McLaren</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.能够出现提示输入的信息
+2.显示指定文件被找到的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>File: txt has found on D:\Test Folder\Test9\寝室宽带账号.txt
+File: txt has found on D:\Test Folder\Test9\CCC\Honda.txt
+File: txt has found on D:\Test Folder\Test9\McLaren\Button.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.能够出现提示输入的信息
+2.显示指定文件被找到的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Folder: McLAREN has found on D:\Test Folder\Test9\McLaren</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -7902,7 +7906,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8000,6 +8004,15 @@
       <color theme="1"/>
       <name val="宋体"/>
       <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -8108,7 +8121,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -8291,6 +8304,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8659,7 +8678,7 @@
         <v>28</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>30</v>
@@ -8736,7 +8755,7 @@
       <c r="B7" s="50"/>
       <c r="C7" s="50"/>
       <c r="D7" s="20" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="E7" s="20" t="s">
         <v>135</v>
@@ -8827,22 +8846,22 @@
         <v>10.1</v>
       </c>
       <c r="B3" s="60" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C3" s="60" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="D3" s="60" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -8854,13 +8873,13 @@
       <c r="C4" s="60"/>
       <c r="D4" s="60"/>
       <c r="E4" s="2" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -8872,13 +8891,13 @@
       <c r="C5" s="60"/>
       <c r="D5" s="60"/>
       <c r="E5" s="2" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -8890,13 +8909,13 @@
       <c r="C6" s="60"/>
       <c r="D6" s="60"/>
       <c r="E6" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="H6" s="5"/>
     </row>
@@ -8908,13 +8927,13 @@
       <c r="C7" s="60"/>
       <c r="D7" s="60"/>
       <c r="E7" s="2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="H7" s="5"/>
     </row>
@@ -8926,13 +8945,13 @@
       <c r="C8" s="60"/>
       <c r="D8" s="60"/>
       <c r="E8" s="2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="H8" s="5"/>
     </row>
@@ -8944,13 +8963,13 @@
       <c r="C9" s="60"/>
       <c r="D9" s="60"/>
       <c r="E9" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="H9" s="5"/>
     </row>
@@ -8962,13 +8981,13 @@
       <c r="C10" s="60"/>
       <c r="D10" s="60"/>
       <c r="E10" s="2" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="H10" s="5"/>
     </row>
@@ -8980,31 +8999,31 @@
       <c r="C11" s="60"/>
       <c r="D11" s="60"/>
       <c r="E11" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A12" s="29" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B12" s="60"/>
       <c r="C12" s="60"/>
       <c r="D12" s="60"/>
       <c r="E12" s="2" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="H12" s="5"/>
     </row>
@@ -9079,13 +9098,13 @@
     </row>
     <row r="3" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B3" s="48" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -9103,7 +9122,7 @@
     </row>
     <row r="4" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B4" s="49"/>
       <c r="C4" s="49"/>
@@ -9123,7 +9142,7 @@
     </row>
     <row r="5" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B5" s="49"/>
       <c r="C5" s="49"/>
@@ -9143,12 +9162,12 @@
     </row>
     <row r="6" spans="1:9" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A6" s="20" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B6" s="50"/>
       <c r="C6" s="50"/>
       <c r="D6" s="20" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="E6" s="20" t="s">
         <v>139</v>
@@ -9201,13 +9220,13 @@
     </row>
     <row r="9" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B9" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>10</v>
@@ -9226,7 +9245,7 @@
     </row>
     <row r="10" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B10" s="49"/>
       <c r="C10" s="49"/>
@@ -9249,7 +9268,7 @@
     </row>
     <row r="11" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B11" s="49"/>
       <c r="C11" s="49"/>
@@ -9270,12 +9289,12 @@
     </row>
     <row r="12" spans="1:9" s="23" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A12" s="20" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B12" s="50"/>
       <c r="C12" s="50"/>
       <c r="D12" s="20" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>139</v>
@@ -9447,22 +9466,22 @@
     </row>
     <row r="3" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B3" s="48" t="s">
         <v>114</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="E3" s="45" t="s">
         <v>118</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>32</v>
@@ -9471,16 +9490,16 @@
     </row>
     <row r="4" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B4" s="49"/>
       <c r="C4" s="49"/>
       <c r="D4" s="2" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="E4" s="46"/>
       <c r="F4" s="2" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>32</v>
@@ -9489,7 +9508,7 @@
     </row>
     <row r="5" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="B5" s="49"/>
       <c r="C5" s="49"/>
@@ -9507,16 +9526,16 @@
     </row>
     <row r="6" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B6" s="49"/>
       <c r="C6" s="49"/>
       <c r="D6" s="2" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="E6" s="46"/>
       <c r="F6" s="2" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>32</v>
@@ -9525,7 +9544,7 @@
     </row>
     <row r="7" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B7" s="49"/>
       <c r="C7" s="49"/>
@@ -9534,7 +9553,7 @@
       </c>
       <c r="E7" s="46"/>
       <c r="F7" s="2" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>39</v>
@@ -9543,12 +9562,12 @@
     </row>
     <row r="8" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A8" s="11" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B8" s="49"/>
       <c r="C8" s="49"/>
       <c r="D8" s="11" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="E8" s="46"/>
       <c r="F8" s="19" t="s">
@@ -9561,16 +9580,16 @@
     </row>
     <row r="9" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B9" s="49"/>
       <c r="C9" s="49"/>
       <c r="D9" s="11" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="E9" s="46"/>
       <c r="F9" s="19" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>32</v>
@@ -9579,30 +9598,30 @@
     </row>
     <row r="10" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A10" s="36" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="B10" s="49"/>
       <c r="C10" s="49"/>
       <c r="D10" s="36" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="E10" s="47"/>
       <c r="F10" s="37" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="G10" s="38" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="H10" s="38"/>
     </row>
     <row r="11" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A11" s="20" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B11" s="49"/>
       <c r="C11" s="49"/>
       <c r="D11" s="20" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>139</v>
@@ -9617,18 +9636,18 @@
     </row>
     <row r="12" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A12" s="20" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B12" s="50"/>
       <c r="C12" s="50"/>
       <c r="D12" s="20" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="G12" s="21" t="s">
         <v>32</v>
@@ -9663,22 +9682,22 @@
     </row>
     <row r="16" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A16" s="14" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B16" s="48" t="s">
         <v>115</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E16" s="45" t="s">
         <v>119</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="G16" s="14" t="s">
         <v>32</v>
@@ -9687,7 +9706,7 @@
     </row>
     <row r="17" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A17" s="14" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B17" s="49"/>
       <c r="C17" s="49"/>
@@ -9705,7 +9724,7 @@
     </row>
     <row r="18" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A18" s="14" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B18" s="49"/>
       <c r="C18" s="49"/>
@@ -9723,7 +9742,7 @@
     </row>
     <row r="19" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A19" s="14" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B19" s="49"/>
       <c r="C19" s="49"/>
@@ -9741,12 +9760,12 @@
     </row>
     <row r="20" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A20" s="11" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B20" s="49"/>
       <c r="C20" s="49"/>
       <c r="D20" s="11" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="E20" s="46"/>
       <c r="F20" s="11" t="s">
@@ -9759,25 +9778,25 @@
     </row>
     <row r="21" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A21" s="36" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="B21" s="49"/>
       <c r="C21" s="49"/>
       <c r="D21" s="36" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="E21" s="47"/>
       <c r="F21" s="37" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="G21" s="38" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="H21" s="38"/>
     </row>
     <row r="22" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A22" s="20" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B22" s="49"/>
       <c r="C22" s="49"/>
@@ -9797,18 +9816,18 @@
     </row>
     <row r="23" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A23" s="20" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="B23" s="50"/>
       <c r="C23" s="50"/>
       <c r="D23" s="20" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="G23" s="21" t="s">
         <v>32</v>
@@ -9835,7 +9854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -9889,22 +9908,22 @@
     </row>
     <row r="3" spans="1:8" s="23" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B3" s="54" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="C3" s="54" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="E3" s="57" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>42</v>
@@ -9913,12 +9932,12 @@
     </row>
     <row r="4" spans="1:8" s="23" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="B4" s="55"/>
       <c r="C4" s="55"/>
       <c r="D4" s="6" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E4" s="58"/>
       <c r="F4" s="6" t="s">
@@ -9931,7 +9950,7 @@
     </row>
     <row r="5" spans="1:8" s="23" customFormat="1" ht="114" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="B5" s="55"/>
       <c r="C5" s="55"/>
@@ -9940,7 +9959,7 @@
       </c>
       <c r="E5" s="58"/>
       <c r="F5" s="6" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>41</v>
@@ -9949,7 +9968,7 @@
     </row>
     <row r="6" spans="1:8" s="23" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="B6" s="55"/>
       <c r="C6" s="55"/>
@@ -9967,16 +9986,16 @@
     </row>
     <row r="7" spans="1:8" s="23" customFormat="1" ht="156.75" x14ac:dyDescent="0.15">
       <c r="A7" s="30" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B7" s="55"/>
       <c r="C7" s="55"/>
       <c r="D7" s="30" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="E7" s="58"/>
       <c r="F7" s="30" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="G7" s="31" t="s">
         <v>77</v>
@@ -9985,30 +10004,30 @@
     </row>
     <row r="8" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A8" s="39" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="B8" s="55"/>
       <c r="C8" s="55"/>
       <c r="D8" s="36" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="E8" s="59"/>
       <c r="F8" s="37" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="G8" s="40" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="H8" s="41"/>
     </row>
     <row r="9" spans="1:8" s="23" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A9" s="20" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B9" s="55"/>
       <c r="C9" s="55"/>
       <c r="D9" s="20" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="E9" s="20" t="s">
         <v>141</v>
@@ -10023,18 +10042,18 @@
     </row>
     <row r="10" spans="1:8" s="34" customFormat="1" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A10" s="20" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B10" s="56"/>
       <c r="C10" s="56"/>
       <c r="D10" s="20" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="G10" s="21" t="s">
         <v>32</v>
@@ -10078,22 +10097,22 @@
     </row>
     <row r="13" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B13" s="48" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C13" s="54" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E13" s="45" t="s">
         <v>140</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>32</v>
@@ -10102,16 +10121,16 @@
     </row>
     <row r="14" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="B14" s="49"/>
       <c r="C14" s="55"/>
       <c r="D14" s="2" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E14" s="46"/>
       <c r="F14" s="2" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>32</v>
@@ -10120,7 +10139,7 @@
     </row>
     <row r="15" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B15" s="49"/>
       <c r="C15" s="55"/>
@@ -10138,7 +10157,7 @@
     </row>
     <row r="16" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B16" s="49"/>
       <c r="C16" s="55"/>
@@ -10147,7 +10166,7 @@
       </c>
       <c r="E16" s="46"/>
       <c r="F16" s="2" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>32</v>
@@ -10156,7 +10175,7 @@
     </row>
     <row r="17" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="B17" s="49"/>
       <c r="C17" s="55"/>
@@ -10174,12 +10193,12 @@
     </row>
     <row r="18" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A18" s="11" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="B18" s="49"/>
       <c r="C18" s="55"/>
       <c r="D18" s="11" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="E18" s="46"/>
       <c r="F18" s="11" t="s">
@@ -10192,12 +10211,12 @@
     </row>
     <row r="19" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A19" s="11" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B19" s="49"/>
       <c r="C19" s="55"/>
       <c r="D19" s="11" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="E19" s="46"/>
       <c r="F19" s="11" t="s">
@@ -10210,30 +10229,30 @@
     </row>
     <row r="20" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A20" s="36" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="B20" s="49"/>
       <c r="C20" s="55"/>
       <c r="D20" s="36" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="E20" s="47"/>
       <c r="F20" s="37" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="G20" s="42" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="H20" s="43"/>
     </row>
     <row r="21" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A21" s="20" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="B21" s="49"/>
       <c r="C21" s="55"/>
       <c r="D21" s="20" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="E21" s="20" t="s">
         <v>141</v>
@@ -10248,18 +10267,18 @@
     </row>
     <row r="22" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A22" s="20" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="B22" s="50"/>
       <c r="C22" s="56"/>
       <c r="D22" s="20" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="G22" s="21" t="s">
         <v>32</v>
@@ -10346,7 +10365,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>17</v>
@@ -10423,7 +10442,7 @@
       <c r="B7" s="50"/>
       <c r="C7" s="50"/>
       <c r="D7" s="20" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="E7" s="20" t="s">
         <v>135</v>
@@ -10459,7 +10478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -10510,24 +10529,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" ht="228" x14ac:dyDescent="0.15">
       <c r="A3" s="22">
         <v>6.1</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="48" t="s">
-        <v>156</v>
+      <c r="C3" s="17" t="s">
+        <v>150</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>144</v>
+        <v>278</v>
       </c>
       <c r="E3" s="45" t="s">
-        <v>148</v>
+        <v>280</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>146</v>
+        <v>282</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>32</v>
@@ -10538,8 +10557,8 @@
       <c r="A4" s="22">
         <v>6.2</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
       <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
@@ -10556,8 +10575,8 @@
       <c r="A5" s="22">
         <v>6.3</v>
       </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
       <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
@@ -10574,19 +10593,19 @@
       <c r="A6" s="24">
         <v>6.4</v>
       </c>
-      <c r="B6" s="49"/>
-      <c r="C6" s="49"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
       <c r="D6" s="6" t="s">
-        <v>145</v>
+        <v>279</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>149</v>
+        <v>281</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>147</v>
+        <v>283</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="H6" s="6"/>
     </row>
@@ -10594,10 +10613,10 @@
       <c r="A7" s="27">
         <v>6.5</v>
       </c>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
       <c r="D7" s="20" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="E7" s="20" t="s">
         <v>135</v>
@@ -10614,11 +10633,9 @@
       <c r="B10" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="2">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="E3:E5"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C3:C7"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10684,13 +10701,13 @@
     </row>
     <row r="3" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B3" s="48" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>82</v>
@@ -10708,7 +10725,7 @@
     </row>
     <row r="4" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B4" s="49"/>
       <c r="C4" s="49"/>
@@ -10726,7 +10743,7 @@
     </row>
     <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B5" s="49"/>
       <c r="C5" s="49"/>
@@ -10744,7 +10761,7 @@
     </row>
     <row r="6" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B6" s="49"/>
       <c r="C6" s="49"/>
@@ -10762,12 +10779,12 @@
     </row>
     <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A7" s="20" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="B7" s="50"/>
       <c r="C7" s="50"/>
       <c r="D7" s="20" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="E7" s="20" t="s">
         <v>139</v>
@@ -10808,7 +10825,7 @@
     </row>
     <row r="10" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B10" s="48" t="s">
         <v>24</v>
@@ -10832,7 +10849,7 @@
     </row>
     <row r="11" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B11" s="49"/>
       <c r="C11" s="49"/>
@@ -10841,7 +10858,7 @@
       </c>
       <c r="E11" s="46"/>
       <c r="F11" s="2" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>32</v>
@@ -10850,7 +10867,7 @@
     </row>
     <row r="12" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B12" s="49"/>
       <c r="C12" s="49"/>
@@ -10868,7 +10885,7 @@
     </row>
     <row r="13" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B13" s="49"/>
       <c r="C13" s="49"/>
@@ -10886,12 +10903,12 @@
     </row>
     <row r="14" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A14" s="20" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B14" s="50"/>
       <c r="C14" s="50"/>
       <c r="D14" s="20" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="E14" s="20" t="s">
         <v>139</v>
@@ -10983,10 +11000,10 @@
         <v>26</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="E3" s="45" t="s">
         <v>143</v>
@@ -10998,7 +11015,7 @@
         <v>32</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
@@ -11044,7 +11061,7 @@
       <c r="B6" s="50"/>
       <c r="C6" s="50"/>
       <c r="D6" s="20" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="E6" s="20" t="s">
         <v>139</v>

</xml_diff>

<commit_message>
Update the test case file on the 10am of 15th,June
</commit_message>
<xml_diff>
--- a/src/MyItems/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Test Cases for FileOperation.xlsx
@@ -1118,36 +1118,6 @@
   </si>
   <si>
     <r>
-      <t>1.能够出现提示输入的信息
-2.显示指定文件未被找到的信息（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>File: 9888.png didn't found on D:\Test1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>1. 显示查找的文件不包含指定字段 （</t>
     </r>
     <r>
@@ -7887,6 +7857,36 @@
         <scheme val="minor"/>
       </rPr>
       <t>Folder: McLAREN has found on D:\Test Folder\Test9\McLaren</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.能够出现提示输入的信息
+2.显示指定文件未被找到的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>9888.png didn't found on D:\Test1</t>
     </r>
     <r>
       <rPr>
@@ -8254,6 +8254,12 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -8304,12 +8310,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8635,14 +8635,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="44"/>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
+      <c r="A1" s="46"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -8674,20 +8674,20 @@
       <c r="A3" s="22">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="48" t="s">
-        <v>144</v>
+      <c r="C3" s="50" t="s">
+        <v>143</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="45" t="s">
-        <v>134</v>
+      <c r="E3" s="47" t="s">
+        <v>133</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>33</v>
@@ -8698,14 +8698,14 @@
       <c r="A4" s="22">
         <v>1.2</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
       <c r="D4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="46"/>
+      <c r="E4" s="48"/>
       <c r="F4" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>34</v>
@@ -8716,14 +8716,14 @@
       <c r="A5" s="22">
         <v>1.3</v>
       </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="51"/>
       <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="46"/>
+      <c r="E5" s="48"/>
       <c r="F5" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>35</v>
@@ -8734,14 +8734,14 @@
       <c r="A6" s="22">
         <v>1.4</v>
       </c>
-      <c r="B6" s="49"/>
-      <c r="C6" s="49"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="51"/>
       <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="47"/>
+      <c r="E6" s="49"/>
       <c r="F6" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>38</v>
@@ -8752,19 +8752,19 @@
       <c r="A7" s="27">
         <v>1.5</v>
       </c>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
       <c r="D7" s="20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E7" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="F7" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="G7" s="21" t="s">
         <v>136</v>
-      </c>
-      <c r="G7" s="21" t="s">
-        <v>137</v>
       </c>
       <c r="H7" s="21"/>
     </row>
@@ -8806,14 +8806,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="53"/>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
+      <c r="A1" s="55"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -8845,23 +8845,23 @@
       <c r="A3" s="22">
         <v>10.1</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="62" t="s">
+        <v>200</v>
+      </c>
+      <c r="C3" s="62" t="s">
         <v>201</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="D3" s="62" t="s">
         <v>202</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="E3" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>204</v>
-      </c>
       <c r="F3" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>217</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -8869,17 +8869,17 @@
       <c r="A4" s="22">
         <v>10.199999999999999</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
       <c r="E4" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -8887,17 +8887,17 @@
       <c r="A5" s="22">
         <v>10.3</v>
       </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
       <c r="E5" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -8905,17 +8905,17 @@
       <c r="A6" s="22">
         <v>10.4</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
       <c r="E6" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H6" s="5"/>
     </row>
@@ -8923,17 +8923,17 @@
       <c r="A7" s="22">
         <v>10.5</v>
       </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
       <c r="E7" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H7" s="5"/>
     </row>
@@ -8941,17 +8941,17 @@
       <c r="A8" s="22">
         <v>10.6</v>
       </c>
-      <c r="B8" s="60"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="62"/>
       <c r="E8" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H8" s="5"/>
     </row>
@@ -8959,17 +8959,17 @@
       <c r="A9" s="22">
         <v>10.7</v>
       </c>
-      <c r="B9" s="60"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
       <c r="E9" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H9" s="5"/>
     </row>
@@ -8977,17 +8977,17 @@
       <c r="A10" s="22">
         <v>10.8</v>
       </c>
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
       <c r="E10" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H10" s="5"/>
     </row>
@@ -8995,35 +8995,35 @@
       <c r="A11" s="22">
         <v>10.9</v>
       </c>
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
       <c r="E11" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A12" s="29" t="s">
+        <v>213</v>
+      </c>
+      <c r="B12" s="62"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B12" s="60"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>215</v>
-      </c>
       <c r="G12" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H12" s="5"/>
     </row>
@@ -9061,14 +9061,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="44"/>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
+      <c r="A1" s="46"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -9098,22 +9098,22 @@
     </row>
     <row r="3" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B3" s="48" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="48" t="s">
-        <v>145</v>
+      <c r="C3" s="50" t="s">
+        <v>144</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>37</v>
@@ -9122,18 +9122,18 @@
     </row>
     <row r="4" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
+        <v>159</v>
+      </c>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
       <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>32</v>
@@ -9142,18 +9142,18 @@
     </row>
     <row r="5" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
+        <v>160</v>
+      </c>
+      <c r="B5" s="51"/>
+      <c r="C5" s="51"/>
       <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>37</v>
@@ -9162,18 +9162,18 @@
     </row>
     <row r="6" spans="1:9" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A6" s="20" t="s">
-        <v>166</v>
-      </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
+        <v>165</v>
+      </c>
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
       <c r="D6" s="20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G6" s="21" t="s">
         <v>32</v>
@@ -9220,22 +9220,22 @@
     </row>
     <row r="9" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B9" s="48" t="s">
+        <v>161</v>
+      </c>
+      <c r="B9" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="48" t="s">
-        <v>145</v>
+      <c r="C9" s="50" t="s">
+        <v>144</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>32</v>
@@ -9245,41 +9245,41 @@
     </row>
     <row r="10" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
+        <v>162</v>
+      </c>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
       <c r="D10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B11" s="49"/>
-      <c r="C11" s="49"/>
+        <v>163</v>
+      </c>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
       <c r="D11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>32</v>
@@ -9289,27 +9289,27 @@
     </row>
     <row r="12" spans="1:9" s="23" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A12" s="20" t="s">
-        <v>165</v>
-      </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
+        <v>164</v>
+      </c>
+      <c r="B12" s="52"/>
+      <c r="C12" s="52"/>
       <c r="D12" s="20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F12" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="G12" s="21" t="s">
         <v>136</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>137</v>
       </c>
       <c r="H12" s="21"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
-      <c r="B13" s="51"/>
+      <c r="B13" s="53"/>
       <c r="C13" s="4"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -9320,7 +9320,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
-      <c r="B14" s="51"/>
+      <c r="B14" s="53"/>
       <c r="C14" s="4"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -9331,7 +9331,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
-      <c r="B15" s="51"/>
+      <c r="B15" s="53"/>
       <c r="C15" s="4"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -9342,7 +9342,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
-      <c r="B16" s="51"/>
+      <c r="B16" s="53"/>
       <c r="C16" s="4"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -9353,7 +9353,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
-      <c r="B17" s="51"/>
+      <c r="B17" s="53"/>
       <c r="C17" s="4"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -9429,14 +9429,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A1" s="52"/>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
+      <c r="A1" s="54"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -9466,22 +9466,22 @@
     </row>
     <row r="3" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B3" s="48" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="48" t="s">
-        <v>147</v>
+        <v>169</v>
+      </c>
+      <c r="B3" s="50" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="50" t="s">
+        <v>146</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E3" s="45" t="s">
-        <v>118</v>
+        <v>166</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>117</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>32</v>
@@ -9490,16 +9490,16 @@
     </row>
     <row r="4" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
+        <v>170</v>
+      </c>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
       <c r="D4" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E4" s="46"/>
+        <v>167</v>
+      </c>
+      <c r="E4" s="48"/>
       <c r="F4" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>32</v>
@@ -9508,16 +9508,16 @@
     </row>
     <row r="5" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
+        <v>171</v>
+      </c>
+      <c r="B5" s="51"/>
+      <c r="C5" s="51"/>
       <c r="D5" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" s="46"/>
+        <v>66</v>
+      </c>
+      <c r="E5" s="48"/>
       <c r="F5" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>40</v>
@@ -9526,16 +9526,16 @@
     </row>
     <row r="6" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B6" s="49"/>
-      <c r="C6" s="49"/>
+        <v>172</v>
+      </c>
+      <c r="B6" s="51"/>
+      <c r="C6" s="51"/>
       <c r="D6" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E6" s="46"/>
+        <v>152</v>
+      </c>
+      <c r="E6" s="48"/>
       <c r="F6" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>32</v>
@@ -9544,16 +9544,16 @@
     </row>
     <row r="7" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B7" s="49"/>
-      <c r="C7" s="49"/>
+        <v>173</v>
+      </c>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
       <c r="D7" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E7" s="46"/>
+        <v>67</v>
+      </c>
+      <c r="E7" s="48"/>
       <c r="F7" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>39</v>
@@ -9562,16 +9562,16 @@
     </row>
     <row r="8" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A8" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
+        <v>174</v>
+      </c>
+      <c r="B8" s="51"/>
+      <c r="C8" s="51"/>
       <c r="D8" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="E8" s="46"/>
+        <v>168</v>
+      </c>
+      <c r="E8" s="48"/>
       <c r="F8" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>44</v>
@@ -9580,16 +9580,16 @@
     </row>
     <row r="9" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="B9" s="49"/>
-      <c r="C9" s="49"/>
+        <v>175</v>
+      </c>
+      <c r="B9" s="51"/>
+      <c r="C9" s="51"/>
       <c r="D9" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="E9" s="46"/>
+        <v>247</v>
+      </c>
+      <c r="E9" s="48"/>
       <c r="F9" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>32</v>
@@ -9598,36 +9598,36 @@
     </row>
     <row r="10" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A10" s="36" t="s">
-        <v>252</v>
-      </c>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
+        <v>251</v>
+      </c>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
       <c r="D10" s="36" t="s">
-        <v>256</v>
-      </c>
-      <c r="E10" s="47"/>
+        <v>255</v>
+      </c>
+      <c r="E10" s="49"/>
       <c r="F10" s="37" t="s">
+        <v>249</v>
+      </c>
+      <c r="G10" s="38" t="s">
         <v>250</v>
-      </c>
-      <c r="G10" s="38" t="s">
-        <v>251</v>
       </c>
       <c r="H10" s="38"/>
     </row>
     <row r="11" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A11" s="20" t="s">
-        <v>253</v>
-      </c>
-      <c r="B11" s="49"/>
-      <c r="C11" s="49"/>
+        <v>252</v>
+      </c>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
       <c r="D11" s="20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G11" s="21" t="s">
         <v>32</v>
@@ -9636,18 +9636,18 @@
     </row>
     <row r="12" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A12" s="20" t="s">
-        <v>254</v>
-      </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
+        <v>253</v>
+      </c>
+      <c r="B12" s="52"/>
+      <c r="C12" s="52"/>
       <c r="D12" s="20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G12" s="21" t="s">
         <v>32</v>
@@ -9682,22 +9682,22 @@
     </row>
     <row r="16" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A16" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="B16" s="48" t="s">
-        <v>115</v>
-      </c>
-      <c r="C16" s="48" t="s">
-        <v>146</v>
+        <v>178</v>
+      </c>
+      <c r="B16" s="50" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" s="50" t="s">
+        <v>145</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="E16" s="45" t="s">
-        <v>119</v>
+        <v>176</v>
+      </c>
+      <c r="E16" s="47" t="s">
+        <v>118</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G16" s="14" t="s">
         <v>32</v>
@@ -9706,16 +9706,16 @@
     </row>
     <row r="17" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A17" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
+        <v>179</v>
+      </c>
+      <c r="B17" s="51"/>
+      <c r="C17" s="51"/>
       <c r="D17" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E17" s="46"/>
+        <v>68</v>
+      </c>
+      <c r="E17" s="48"/>
       <c r="F17" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G17" s="14" t="s">
         <v>32</v>
@@ -9724,16 +9724,16 @@
     </row>
     <row r="18" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A18" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="B18" s="49"/>
-      <c r="C18" s="49"/>
+        <v>180</v>
+      </c>
+      <c r="B18" s="51"/>
+      <c r="C18" s="51"/>
       <c r="D18" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="E18" s="46"/>
+        <v>69</v>
+      </c>
+      <c r="E18" s="48"/>
       <c r="F18" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G18" s="14" t="s">
         <v>32</v>
@@ -9742,16 +9742,16 @@
     </row>
     <row r="19" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A19" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="B19" s="49"/>
-      <c r="C19" s="49"/>
+        <v>181</v>
+      </c>
+      <c r="B19" s="51"/>
+      <c r="C19" s="51"/>
       <c r="D19" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="E19" s="46"/>
+        <v>70</v>
+      </c>
+      <c r="E19" s="48"/>
       <c r="F19" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G19" s="14" t="s">
         <v>32</v>
@@ -9760,16 +9760,16 @@
     </row>
     <row r="20" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A20" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="B20" s="49"/>
-      <c r="C20" s="49"/>
+        <v>182</v>
+      </c>
+      <c r="B20" s="51"/>
+      <c r="C20" s="51"/>
       <c r="D20" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="E20" s="46"/>
+        <v>177</v>
+      </c>
+      <c r="E20" s="48"/>
       <c r="F20" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G20" s="15" t="s">
         <v>32</v>
@@ -9778,56 +9778,56 @@
     </row>
     <row r="21" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A21" s="36" t="s">
-        <v>257</v>
-      </c>
-      <c r="B21" s="49"/>
-      <c r="C21" s="49"/>
+        <v>256</v>
+      </c>
+      <c r="B21" s="51"/>
+      <c r="C21" s="51"/>
       <c r="D21" s="36" t="s">
-        <v>255</v>
-      </c>
-      <c r="E21" s="47"/>
+        <v>254</v>
+      </c>
+      <c r="E21" s="49"/>
       <c r="F21" s="37" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G21" s="38" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H21" s="38"/>
     </row>
     <row r="22" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A22" s="20" t="s">
-        <v>184</v>
-      </c>
-      <c r="B22" s="49"/>
-      <c r="C22" s="49"/>
+        <v>183</v>
+      </c>
+      <c r="B22" s="51"/>
+      <c r="C22" s="51"/>
       <c r="D22" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F22" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="G22" s="21" t="s">
         <v>136</v>
-      </c>
-      <c r="G22" s="21" t="s">
-        <v>137</v>
       </c>
       <c r="H22" s="21"/>
     </row>
     <row r="23" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A23" s="20" t="s">
-        <v>258</v>
-      </c>
-      <c r="B23" s="50"/>
-      <c r="C23" s="50"/>
+        <v>257</v>
+      </c>
+      <c r="B23" s="52"/>
+      <c r="C23" s="52"/>
       <c r="D23" s="20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G23" s="21" t="s">
         <v>32</v>
@@ -9871,14 +9871,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="53"/>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
+      <c r="A1" s="55"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -9908,22 +9908,22 @@
     </row>
     <row r="3" spans="1:8" s="23" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B3" s="54" t="s">
-        <v>225</v>
-      </c>
-      <c r="C3" s="54" t="s">
-        <v>148</v>
+        <v>233</v>
+      </c>
+      <c r="B3" s="56" t="s">
+        <v>224</v>
+      </c>
+      <c r="C3" s="56" t="s">
+        <v>147</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="E3" s="57" t="s">
-        <v>155</v>
+        <v>229</v>
+      </c>
+      <c r="E3" s="59" t="s">
+        <v>154</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>42</v>
@@ -9932,16 +9932,16 @@
     </row>
     <row r="4" spans="1:8" s="23" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
+        <v>234</v>
+      </c>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
       <c r="D4" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="E4" s="58"/>
+        <v>226</v>
+      </c>
+      <c r="E4" s="60"/>
       <c r="F4" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>43</v>
@@ -9950,16 +9950,16 @@
     </row>
     <row r="5" spans="1:8" s="23" customFormat="1" ht="114" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
+        <v>235</v>
+      </c>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
       <c r="D5" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5" s="58"/>
+        <v>71</v>
+      </c>
+      <c r="E5" s="60"/>
       <c r="F5" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>41</v>
@@ -9968,16 +9968,16 @@
     </row>
     <row r="6" spans="1:8" s="23" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
+        <v>236</v>
+      </c>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
       <c r="D6" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E6" s="58"/>
+        <v>72</v>
+      </c>
+      <c r="E6" s="60"/>
       <c r="F6" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G6" s="25" t="s">
         <v>41</v>
@@ -9986,54 +9986,54 @@
     </row>
     <row r="7" spans="1:8" s="23" customFormat="1" ht="156.75" x14ac:dyDescent="0.15">
       <c r="A7" s="30" t="s">
-        <v>238</v>
-      </c>
-      <c r="B7" s="55"/>
-      <c r="C7" s="55"/>
+        <v>237</v>
+      </c>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
       <c r="D7" s="30" t="s">
-        <v>231</v>
-      </c>
-      <c r="E7" s="58"/>
+        <v>230</v>
+      </c>
+      <c r="E7" s="60"/>
       <c r="F7" s="30" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G7" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H7" s="32"/>
     </row>
     <row r="8" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A8" s="39" t="s">
-        <v>262</v>
-      </c>
-      <c r="B8" s="55"/>
-      <c r="C8" s="55"/>
+        <v>261</v>
+      </c>
+      <c r="B8" s="57"/>
+      <c r="C8" s="57"/>
       <c r="D8" s="36" t="s">
-        <v>265</v>
-      </c>
-      <c r="E8" s="59"/>
+        <v>264</v>
+      </c>
+      <c r="E8" s="61"/>
       <c r="F8" s="37" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G8" s="40" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H8" s="41"/>
     </row>
     <row r="9" spans="1:8" s="23" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A9" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="B9" s="55"/>
-      <c r="C9" s="55"/>
+        <v>238</v>
+      </c>
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
       <c r="D9" s="20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G9" s="21" t="s">
         <v>32</v>
@@ -10042,18 +10042,18 @@
     </row>
     <row r="10" spans="1:8" s="34" customFormat="1" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A10" s="20" t="s">
-        <v>261</v>
-      </c>
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
+        <v>260</v>
+      </c>
+      <c r="B10" s="58"/>
+      <c r="C10" s="58"/>
       <c r="D10" s="20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G10" s="21" t="s">
         <v>32</v>
@@ -10097,22 +10097,22 @@
     </row>
     <row r="13" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="B13" s="48" t="s">
-        <v>226</v>
-      </c>
-      <c r="C13" s="54" t="s">
-        <v>148</v>
+        <v>239</v>
+      </c>
+      <c r="B13" s="50" t="s">
+        <v>225</v>
+      </c>
+      <c r="C13" s="56" t="s">
+        <v>147</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="E13" s="45" t="s">
-        <v>140</v>
+        <v>227</v>
+      </c>
+      <c r="E13" s="47" t="s">
+        <v>139</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>32</v>
@@ -10121,16 +10121,16 @@
     </row>
     <row r="14" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="B14" s="49"/>
-      <c r="C14" s="55"/>
+        <v>240</v>
+      </c>
+      <c r="B14" s="51"/>
+      <c r="C14" s="57"/>
       <c r="D14" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="E14" s="46"/>
+        <v>228</v>
+      </c>
+      <c r="E14" s="48"/>
       <c r="F14" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>32</v>
@@ -10139,16 +10139,16 @@
     </row>
     <row r="15" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="B15" s="49"/>
-      <c r="C15" s="55"/>
+        <v>241</v>
+      </c>
+      <c r="B15" s="51"/>
+      <c r="C15" s="57"/>
       <c r="D15" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E15" s="46"/>
+        <v>73</v>
+      </c>
+      <c r="E15" s="48"/>
       <c r="F15" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>32</v>
@@ -10157,16 +10157,16 @@
     </row>
     <row r="16" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="B16" s="49"/>
-      <c r="C16" s="55"/>
+        <v>242</v>
+      </c>
+      <c r="B16" s="51"/>
+      <c r="C16" s="57"/>
       <c r="D16" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E16" s="46"/>
+        <v>74</v>
+      </c>
+      <c r="E16" s="48"/>
       <c r="F16" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>32</v>
@@ -10175,16 +10175,16 @@
     </row>
     <row r="17" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="B17" s="49"/>
-      <c r="C17" s="55"/>
+        <v>243</v>
+      </c>
+      <c r="B17" s="51"/>
+      <c r="C17" s="57"/>
       <c r="D17" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E17" s="46"/>
+        <v>75</v>
+      </c>
+      <c r="E17" s="48"/>
       <c r="F17" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>32</v>
@@ -10193,34 +10193,34 @@
     </row>
     <row r="18" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A18" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="B18" s="49"/>
-      <c r="C18" s="55"/>
+        <v>244</v>
+      </c>
+      <c r="B18" s="51"/>
+      <c r="C18" s="57"/>
       <c r="D18" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="E18" s="46"/>
+        <v>232</v>
+      </c>
+      <c r="E18" s="48"/>
       <c r="F18" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H18" s="16"/>
     </row>
     <row r="19" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A19" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="B19" s="49"/>
-      <c r="C19" s="55"/>
+        <v>245</v>
+      </c>
+      <c r="B19" s="51"/>
+      <c r="C19" s="57"/>
       <c r="D19" s="11" t="s">
-        <v>232</v>
-      </c>
-      <c r="E19" s="46"/>
+        <v>231</v>
+      </c>
+      <c r="E19" s="48"/>
       <c r="F19" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G19" s="12" t="s">
         <v>32</v>
@@ -10229,56 +10229,56 @@
     </row>
     <row r="20" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A20" s="36" t="s">
-        <v>264</v>
-      </c>
-      <c r="B20" s="49"/>
-      <c r="C20" s="55"/>
+        <v>263</v>
+      </c>
+      <c r="B20" s="51"/>
+      <c r="C20" s="57"/>
       <c r="D20" s="36" t="s">
-        <v>266</v>
-      </c>
-      <c r="E20" s="47"/>
+        <v>265</v>
+      </c>
+      <c r="E20" s="49"/>
       <c r="F20" s="37" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G20" s="42" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H20" s="43"/>
     </row>
     <row r="21" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A21" s="20" t="s">
-        <v>247</v>
-      </c>
-      <c r="B21" s="49"/>
-      <c r="C21" s="55"/>
+        <v>246</v>
+      </c>
+      <c r="B21" s="51"/>
+      <c r="C21" s="57"/>
       <c r="D21" s="20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F21" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="G21" s="21" t="s">
         <v>136</v>
-      </c>
-      <c r="G21" s="21" t="s">
-        <v>137</v>
       </c>
       <c r="H21" s="21"/>
     </row>
     <row r="22" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A22" s="20" t="s">
-        <v>260</v>
-      </c>
-      <c r="B22" s="50"/>
-      <c r="C22" s="56"/>
+        <v>259</v>
+      </c>
+      <c r="B22" s="52"/>
+      <c r="C22" s="58"/>
       <c r="D22" s="20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E22" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="F22" s="20" t="s">
         <v>157</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>158</v>
       </c>
       <c r="G22" s="21" t="s">
         <v>32</v>
@@ -10322,14 +10322,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="53"/>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
+      <c r="A1" s="55"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -10361,20 +10361,20 @@
       <c r="A3" s="22">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="48" t="s">
-        <v>149</v>
+      <c r="C3" s="50" t="s">
+        <v>148</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="45" t="s">
-        <v>142</v>
+      <c r="E3" s="47" t="s">
+        <v>141</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>45</v>
@@ -10385,14 +10385,14 @@
       <c r="A4" s="22">
         <v>5.2</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
       <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="46"/>
+      <c r="E4" s="48"/>
       <c r="F4" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>38</v>
@@ -10403,14 +10403,14 @@
       <c r="A5" s="22">
         <v>5.3</v>
       </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="51"/>
       <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="46"/>
+      <c r="E5" s="48"/>
       <c r="F5" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>33</v>
@@ -10421,12 +10421,12 @@
       <c r="A6" s="22">
         <v>5.4</v>
       </c>
-      <c r="B6" s="49"/>
-      <c r="C6" s="49"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="51"/>
       <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="47"/>
+      <c r="E6" s="49"/>
       <c r="F6" s="2" t="s">
         <v>59</v>
       </c>
@@ -10439,19 +10439,19 @@
       <c r="A7" s="27">
         <v>5.5</v>
       </c>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
       <c r="D7" s="20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E7" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="F7" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="G7" s="21" t="s">
         <v>136</v>
-      </c>
-      <c r="G7" s="21" t="s">
-        <v>137</v>
       </c>
       <c r="H7" s="21"/>
     </row>
@@ -10494,14 +10494,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="53"/>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
+      <c r="A1" s="55"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -10537,16 +10537,16 @@
         <v>20</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="E3" s="45" t="s">
-        <v>280</v>
+        <v>277</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>279</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>32</v>
@@ -10557,14 +10557,14 @@
       <c r="A4" s="22">
         <v>6.2</v>
       </c>
-      <c r="B4" s="61"/>
-      <c r="C4" s="61"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
       <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="46"/>
+      <c r="E4" s="48"/>
       <c r="F4" s="2" t="s">
-        <v>60</v>
+        <v>283</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>38</v>
@@ -10575,14 +10575,14 @@
       <c r="A5" s="22">
         <v>6.3</v>
       </c>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
       <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="47"/>
+      <c r="E5" s="49"/>
       <c r="F5" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>32</v>
@@ -10593,19 +10593,19 @@
       <c r="A6" s="24">
         <v>6.4</v>
       </c>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
       <c r="D6" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H6" s="6"/>
     </row>
@@ -10613,19 +10613,19 @@
       <c r="A7" s="27">
         <v>6.5</v>
       </c>
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
       <c r="D7" s="20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E7" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="F7" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="G7" s="21" t="s">
         <v>136</v>
-      </c>
-      <c r="G7" s="21" t="s">
-        <v>137</v>
       </c>
       <c r="H7" s="21"/>
     </row>
@@ -10664,14 +10664,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="53"/>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
+      <c r="A1" s="55"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -10701,22 +10701,22 @@
     </row>
     <row r="3" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B3" s="48" t="s">
+        <v>188</v>
+      </c>
+      <c r="B3" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="48" t="s">
-        <v>151</v>
+      <c r="C3" s="50" t="s">
+        <v>150</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E3" s="45" t="s">
-        <v>120</v>
+        <v>81</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>119</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>36</v>
@@ -10725,16 +10725,16 @@
     </row>
     <row r="4" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
+        <v>189</v>
+      </c>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
       <c r="D4" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E4" s="46"/>
+        <v>82</v>
+      </c>
+      <c r="E4" s="48"/>
       <c r="F4" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>34</v>
@@ -10743,16 +10743,16 @@
     </row>
     <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
+        <v>190</v>
+      </c>
+      <c r="B5" s="51"/>
+      <c r="C5" s="51"/>
       <c r="D5" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E5" s="46"/>
+        <v>83</v>
+      </c>
+      <c r="E5" s="48"/>
       <c r="F5" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>35</v>
@@ -10761,36 +10761,36 @@
     </row>
     <row r="6" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="B6" s="49"/>
-      <c r="C6" s="49"/>
+        <v>191</v>
+      </c>
+      <c r="B6" s="51"/>
+      <c r="C6" s="51"/>
       <c r="D6" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="E6" s="47"/>
+        <v>84</v>
+      </c>
+      <c r="E6" s="49"/>
       <c r="F6" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A7" s="20" t="s">
-        <v>193</v>
-      </c>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
+        <v>192</v>
+      </c>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
       <c r="D7" s="20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G7" s="21" t="s">
         <v>32</v>
@@ -10825,22 +10825,22 @@
     </row>
     <row r="10" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B10" s="48" t="s">
+        <v>193</v>
+      </c>
+      <c r="B10" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="48" t="s">
-        <v>95</v>
+      <c r="C10" s="50" t="s">
+        <v>94</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" s="45" t="s">
-        <v>121</v>
+        <v>79</v>
+      </c>
+      <c r="E10" s="47" t="s">
+        <v>120</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>32</v>
@@ -10849,16 +10849,16 @@
     </row>
     <row r="11" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B11" s="49"/>
-      <c r="C11" s="49"/>
+        <v>194</v>
+      </c>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
       <c r="D11" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E11" s="46"/>
+        <v>80</v>
+      </c>
+      <c r="E11" s="48"/>
       <c r="F11" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>32</v>
@@ -10867,16 +10867,16 @@
     </row>
     <row r="12" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B12" s="49"/>
-      <c r="C12" s="49"/>
+        <v>195</v>
+      </c>
+      <c r="B12" s="51"/>
+      <c r="C12" s="51"/>
       <c r="D12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" s="48"/>
+      <c r="F12" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="E12" s="46"/>
-      <c r="F12" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>32</v>
@@ -10885,16 +10885,16 @@
     </row>
     <row r="13" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="B13" s="49"/>
-      <c r="C13" s="49"/>
+        <v>196</v>
+      </c>
+      <c r="B13" s="51"/>
+      <c r="C13" s="51"/>
       <c r="D13" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E13" s="47"/>
+        <v>87</v>
+      </c>
+      <c r="E13" s="49"/>
       <c r="F13" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>32</v>
@@ -10903,21 +10903,21 @@
     </row>
     <row r="14" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A14" s="20" t="s">
-        <v>198</v>
-      </c>
-      <c r="B14" s="50"/>
-      <c r="C14" s="50"/>
+        <v>197</v>
+      </c>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
       <c r="D14" s="20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F14" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="G14" s="21" t="s">
         <v>136</v>
-      </c>
-      <c r="G14" s="21" t="s">
-        <v>137</v>
       </c>
       <c r="H14" s="21"/>
     </row>
@@ -10957,14 +10957,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="53"/>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
+      <c r="A1" s="55"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -10996,40 +10996,40 @@
       <c r="A3" s="22">
         <v>8.1</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="48" t="s">
-        <v>152</v>
+      <c r="C3" s="50" t="s">
+        <v>151</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E3" s="45" t="s">
-        <v>143</v>
+        <v>198</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>142</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>32</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A4" s="22">
         <v>8.1999999999999993</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
       <c r="D4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="46"/>
+      <c r="E4" s="48"/>
       <c r="F4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>38</v>
@@ -11040,14 +11040,14 @@
       <c r="A5" s="22">
         <v>8.3000000000000007</v>
       </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="51"/>
       <c r="D5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="47"/>
+      <c r="E5" s="49"/>
       <c r="F5" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>34</v>
@@ -11058,19 +11058,19 @@
       <c r="A6" s="27">
         <v>8.4</v>
       </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
       <c r="D6" s="20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F6" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="G6" s="21" t="s">
         <v>136</v>
-      </c>
-      <c r="G6" s="21" t="s">
-        <v>137</v>
       </c>
       <c r="H6" s="21"/>
     </row>
@@ -11112,14 +11112,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="53"/>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
+      <c r="A1" s="55"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -11151,19 +11151,19 @@
       <c r="A3" s="22">
         <v>9.1</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="50" t="s">
         <v>47</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="50" t="s">
         <v>52</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -11175,15 +11175,15 @@
       <c r="A4" s="22">
         <v>9.1999999999999993</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
       <c r="D4" s="2" t="s">
         <v>49</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="49"/>
+        <v>62</v>
+      </c>
+      <c r="F4" s="51"/>
       <c r="G4" s="2" t="s">
         <v>54</v>
       </c>
@@ -11193,15 +11193,15 @@
       <c r="A5" s="22">
         <v>9.3000000000000007</v>
       </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="51"/>
       <c r="D5" s="2" t="s">
         <v>50</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="49"/>
+        <v>63</v>
+      </c>
+      <c r="F5" s="51"/>
       <c r="G5" s="2" t="s">
         <v>54</v>
       </c>
@@ -11211,15 +11211,15 @@
       <c r="A6" s="22">
         <v>9.4</v>
       </c>
-      <c r="B6" s="49"/>
-      <c r="C6" s="49"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="51"/>
       <c r="D6" s="2" t="s">
         <v>51</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F6" s="49"/>
+        <v>65</v>
+      </c>
+      <c r="F6" s="51"/>
       <c r="G6" s="5" t="s">
         <v>54</v>
       </c>
@@ -11229,15 +11229,15 @@
       <c r="A7" s="22">
         <v>9.5</v>
       </c>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
       <c r="D7" s="2" t="s">
         <v>53</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7" s="50"/>
+        <v>64</v>
+      </c>
+      <c r="F7" s="52"/>
       <c r="G7" s="5" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
Update the test case file after updated on function 5
</commit_message>
<xml_diff>
--- a/src/MyItems/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="285">
   <si>
     <t>删除文件夹</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1084,36 +1084,6 @@
   </si>
   <si>
     <t>测试数据</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1. 能够出现提示输入的信息
-2.显示该文件夹下不存在txt文件（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>There is no txt files under folder D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -4517,106 +4487,6 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>What content you want to find on txt file?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入txt文件内存在的内容，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Alonso
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t/>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>What word do you want find?</t>
     </r>
     <r>
@@ -7887,6 +7757,189 @@
         <scheme val="minor"/>
       </rPr>
       <t>9888.png didn't found on D:\Test1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹路径且</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>不包含</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">txt文件
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What content you want to find on txt file?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入txt文件内存在的内容，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Alonso
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 不出现需要查找内容的输入框
+2. 显示该文件夹下不存在txt文件（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>There is no txt files under folder D:\Test</t>
     </r>
     <r>
       <rPr>
@@ -8678,16 +8731,16 @@
         <v>28</v>
       </c>
       <c r="C3" s="50" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E3" s="47" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>33</v>
@@ -8705,7 +8758,7 @@
       </c>
       <c r="E4" s="48"/>
       <c r="F4" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>34</v>
@@ -8723,7 +8776,7 @@
       </c>
       <c r="E5" s="48"/>
       <c r="F5" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>35</v>
@@ -8741,7 +8794,7 @@
       </c>
       <c r="E6" s="49"/>
       <c r="F6" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>38</v>
@@ -8755,16 +8808,16 @@
       <c r="B7" s="52"/>
       <c r="C7" s="52"/>
       <c r="D7" s="20" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E7" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="F7" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="G7" s="21" t="s">
         <v>135</v>
-      </c>
-      <c r="G7" s="21" t="s">
-        <v>136</v>
       </c>
       <c r="H7" s="21"/>
     </row>
@@ -8846,22 +8899,22 @@
         <v>10.1</v>
       </c>
       <c r="B3" s="62" t="s">
+        <v>198</v>
+      </c>
+      <c r="C3" s="62" t="s">
+        <v>199</v>
+      </c>
+      <c r="D3" s="62" t="s">
         <v>200</v>
       </c>
-      <c r="C3" s="62" t="s">
+      <c r="E3" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="D3" s="62" t="s">
-        <v>202</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>203</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H3" s="2"/>
     </row>
@@ -8873,13 +8926,13 @@
       <c r="C4" s="62"/>
       <c r="D4" s="62"/>
       <c r="E4" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H4" s="2"/>
     </row>
@@ -8891,13 +8944,13 @@
       <c r="C5" s="62"/>
       <c r="D5" s="62"/>
       <c r="E5" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H5" s="2"/>
     </row>
@@ -8909,13 +8962,13 @@
       <c r="C6" s="62"/>
       <c r="D6" s="62"/>
       <c r="E6" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H6" s="5"/>
     </row>
@@ -8927,13 +8980,13 @@
       <c r="C7" s="62"/>
       <c r="D7" s="62"/>
       <c r="E7" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H7" s="5"/>
     </row>
@@ -8945,13 +8998,13 @@
       <c r="C8" s="62"/>
       <c r="D8" s="62"/>
       <c r="E8" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H8" s="5"/>
     </row>
@@ -8963,13 +9016,13 @@
       <c r="C9" s="62"/>
       <c r="D9" s="62"/>
       <c r="E9" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H9" s="5"/>
     </row>
@@ -8981,13 +9034,13 @@
       <c r="C10" s="62"/>
       <c r="D10" s="62"/>
       <c r="E10" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H10" s="5"/>
     </row>
@@ -8999,31 +9052,31 @@
       <c r="C11" s="62"/>
       <c r="D11" s="62"/>
       <c r="E11" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A12" s="29" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B12" s="62"/>
       <c r="C12" s="62"/>
       <c r="D12" s="62"/>
       <c r="E12" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>214</v>
-      </c>
       <c r="G12" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H12" s="5"/>
     </row>
@@ -9098,22 +9151,22 @@
     </row>
     <row r="3" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B3" s="50" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="50" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>37</v>
@@ -9122,7 +9175,7 @@
     </row>
     <row r="4" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B4" s="51"/>
       <c r="C4" s="51"/>
@@ -9130,10 +9183,10 @@
         <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>32</v>
@@ -9142,7 +9195,7 @@
     </row>
     <row r="5" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B5" s="51"/>
       <c r="C5" s="51"/>
@@ -9150,10 +9203,10 @@
         <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>37</v>
@@ -9162,18 +9215,18 @@
     </row>
     <row r="6" spans="1:9" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A6" s="20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B6" s="52"/>
       <c r="C6" s="52"/>
       <c r="D6" s="20" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G6" s="21" t="s">
         <v>32</v>
@@ -9220,22 +9273,22 @@
     </row>
     <row r="9" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B9" s="50" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>32</v>
@@ -9245,7 +9298,7 @@
     </row>
     <row r="10" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B10" s="51"/>
       <c r="C10" s="51"/>
@@ -9253,22 +9306,22 @@
         <v>11</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
@@ -9276,10 +9329,10 @@
         <v>12</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>32</v>
@@ -9289,21 +9342,21 @@
     </row>
     <row r="12" spans="1:9" s="23" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A12" s="20" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B12" s="52"/>
       <c r="C12" s="52"/>
       <c r="D12" s="20" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F12" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="G12" s="21" t="s">
         <v>135</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>136</v>
       </c>
       <c r="H12" s="21"/>
     </row>
@@ -9466,22 +9519,22 @@
     </row>
     <row r="3" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C3" s="50" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E3" s="47" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>32</v>
@@ -9490,16 +9543,16 @@
     </row>
     <row r="4" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B4" s="51"/>
       <c r="C4" s="51"/>
       <c r="D4" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E4" s="48"/>
       <c r="F4" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>32</v>
@@ -9508,16 +9561,16 @@
     </row>
     <row r="5" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B5" s="51"/>
       <c r="C5" s="51"/>
       <c r="D5" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E5" s="48"/>
       <c r="F5" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>40</v>
@@ -9526,16 +9579,16 @@
     </row>
     <row r="6" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B6" s="51"/>
       <c r="C6" s="51"/>
       <c r="D6" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E6" s="48"/>
       <c r="F6" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>32</v>
@@ -9544,16 +9597,16 @@
     </row>
     <row r="7" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B7" s="51"/>
       <c r="C7" s="51"/>
       <c r="D7" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E7" s="48"/>
       <c r="F7" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>39</v>
@@ -9562,16 +9615,16 @@
     </row>
     <row r="8" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A8" s="11" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B8" s="51"/>
       <c r="C8" s="51"/>
       <c r="D8" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E8" s="48"/>
       <c r="F8" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>44</v>
@@ -9580,16 +9633,16 @@
     </row>
     <row r="9" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B9" s="51"/>
       <c r="C9" s="51"/>
       <c r="D9" s="11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E9" s="48"/>
       <c r="F9" s="19" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>32</v>
@@ -9598,36 +9651,36 @@
     </row>
     <row r="10" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A10" s="36" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B10" s="51"/>
       <c r="C10" s="51"/>
       <c r="D10" s="36" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E10" s="49"/>
       <c r="F10" s="37" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G10" s="38" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="H10" s="38"/>
     </row>
     <row r="11" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A11" s="20" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
       <c r="D11" s="20" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G11" s="21" t="s">
         <v>32</v>
@@ -9636,18 +9689,18 @@
     </row>
     <row r="12" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A12" s="20" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B12" s="52"/>
       <c r="C12" s="52"/>
       <c r="D12" s="20" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G12" s="21" t="s">
         <v>32</v>
@@ -9682,22 +9735,22 @@
     </row>
     <row r="16" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A16" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B16" s="50" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C16" s="50" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E16" s="47" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G16" s="14" t="s">
         <v>32</v>
@@ -9706,16 +9759,16 @@
     </row>
     <row r="17" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A17" s="14" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B17" s="51"/>
       <c r="C17" s="51"/>
       <c r="D17" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E17" s="48"/>
       <c r="F17" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G17" s="14" t="s">
         <v>32</v>
@@ -9724,16 +9777,16 @@
     </row>
     <row r="18" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A18" s="14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B18" s="51"/>
       <c r="C18" s="51"/>
       <c r="D18" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E18" s="48"/>
       <c r="F18" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G18" s="14" t="s">
         <v>32</v>
@@ -9742,16 +9795,16 @@
     </row>
     <row r="19" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A19" s="14" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B19" s="51"/>
       <c r="C19" s="51"/>
       <c r="D19" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E19" s="48"/>
       <c r="F19" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G19" s="14" t="s">
         <v>32</v>
@@ -9760,16 +9813,16 @@
     </row>
     <row r="20" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A20" s="11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B20" s="51"/>
       <c r="C20" s="51"/>
       <c r="D20" s="11" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E20" s="48"/>
       <c r="F20" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G20" s="15" t="s">
         <v>32</v>
@@ -9778,56 +9831,56 @@
     </row>
     <row r="21" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A21" s="36" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B21" s="51"/>
       <c r="C21" s="51"/>
       <c r="D21" s="36" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="37" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G21" s="38" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="H21" s="38"/>
     </row>
     <row r="22" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A22" s="20" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B22" s="51"/>
       <c r="C22" s="51"/>
       <c r="D22" s="20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F22" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="G22" s="21" t="s">
         <v>135</v>
-      </c>
-      <c r="G22" s="21" t="s">
-        <v>136</v>
       </c>
       <c r="H22" s="21"/>
     </row>
     <row r="23" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A23" s="20" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B23" s="52"/>
       <c r="C23" s="52"/>
       <c r="D23" s="20" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G23" s="21" t="s">
         <v>32</v>
@@ -9908,22 +9961,22 @@
     </row>
     <row r="3" spans="1:8" s="23" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B3" s="56" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C3" s="56" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E3" s="59" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>42</v>
@@ -9932,16 +9985,16 @@
     </row>
     <row r="4" spans="1:8" s="23" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B4" s="57"/>
       <c r="C4" s="57"/>
       <c r="D4" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E4" s="60"/>
       <c r="F4" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>43</v>
@@ -9950,16 +10003,16 @@
     </row>
     <row r="5" spans="1:8" s="23" customFormat="1" ht="114" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B5" s="57"/>
       <c r="C5" s="57"/>
       <c r="D5" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E5" s="60"/>
       <c r="F5" s="6" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>41</v>
@@ -9968,16 +10021,16 @@
     </row>
     <row r="6" spans="1:8" s="23" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B6" s="57"/>
       <c r="C6" s="57"/>
       <c r="D6" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E6" s="60"/>
       <c r="F6" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G6" s="25" t="s">
         <v>41</v>
@@ -9986,54 +10039,54 @@
     </row>
     <row r="7" spans="1:8" s="23" customFormat="1" ht="156.75" x14ac:dyDescent="0.15">
       <c r="A7" s="30" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B7" s="57"/>
       <c r="C7" s="57"/>
       <c r="D7" s="30" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E7" s="60"/>
       <c r="F7" s="30" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G7" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H7" s="32"/>
     </row>
     <row r="8" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A8" s="39" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B8" s="57"/>
       <c r="C8" s="57"/>
       <c r="D8" s="36" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E8" s="61"/>
       <c r="F8" s="37" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G8" s="40" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="H8" s="41"/>
     </row>
     <row r="9" spans="1:8" s="23" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A9" s="20" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B9" s="57"/>
       <c r="C9" s="57"/>
       <c r="D9" s="20" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G9" s="21" t="s">
         <v>32</v>
@@ -10042,18 +10095,18 @@
     </row>
     <row r="10" spans="1:8" s="34" customFormat="1" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A10" s="20" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B10" s="58"/>
       <c r="C10" s="58"/>
       <c r="D10" s="20" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E10" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="F10" s="20" t="s">
         <v>155</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>157</v>
       </c>
       <c r="G10" s="21" t="s">
         <v>32</v>
@@ -10097,22 +10150,22 @@
     </row>
     <row r="13" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B13" s="50" t="s">
+        <v>223</v>
+      </c>
+      <c r="C13" s="56" t="s">
+        <v>145</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="C13" s="56" t="s">
-        <v>147</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>227</v>
-      </c>
       <c r="E13" s="47" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>32</v>
@@ -10121,16 +10174,16 @@
     </row>
     <row r="14" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B14" s="51"/>
       <c r="C14" s="57"/>
       <c r="D14" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E14" s="48"/>
       <c r="F14" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>32</v>
@@ -10139,16 +10192,16 @@
     </row>
     <row r="15" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B15" s="51"/>
       <c r="C15" s="57"/>
       <c r="D15" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E15" s="48"/>
       <c r="F15" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>32</v>
@@ -10157,16 +10210,16 @@
     </row>
     <row r="16" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B16" s="51"/>
       <c r="C16" s="57"/>
       <c r="D16" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E16" s="48"/>
       <c r="F16" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>32</v>
@@ -10175,16 +10228,16 @@
     </row>
     <row r="17" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B17" s="51"/>
       <c r="C17" s="57"/>
       <c r="D17" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E17" s="48"/>
       <c r="F17" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>32</v>
@@ -10193,34 +10246,34 @@
     </row>
     <row r="18" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A18" s="11" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B18" s="51"/>
       <c r="C18" s="57"/>
       <c r="D18" s="11" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E18" s="48"/>
       <c r="F18" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H18" s="16"/>
     </row>
     <row r="19" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A19" s="11" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B19" s="51"/>
       <c r="C19" s="57"/>
       <c r="D19" s="11" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E19" s="48"/>
       <c r="F19" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G19" s="12" t="s">
         <v>32</v>
@@ -10229,56 +10282,56 @@
     </row>
     <row r="20" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A20" s="36" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B20" s="51"/>
       <c r="C20" s="57"/>
       <c r="D20" s="36" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E20" s="49"/>
       <c r="F20" s="37" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G20" s="42" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="H20" s="43"/>
     </row>
     <row r="21" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A21" s="20" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B21" s="51"/>
       <c r="C21" s="57"/>
       <c r="D21" s="20" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F21" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="G21" s="21" t="s">
         <v>135</v>
-      </c>
-      <c r="G21" s="21" t="s">
-        <v>136</v>
       </c>
       <c r="H21" s="21"/>
     </row>
     <row r="22" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A22" s="20" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B22" s="52"/>
       <c r="C22" s="58"/>
       <c r="D22" s="20" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G22" s="21" t="s">
         <v>32</v>
@@ -10305,7 +10358,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -10365,16 +10418,16 @@
         <v>15</v>
       </c>
       <c r="C3" s="50" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="47" t="s">
-        <v>141</v>
+        <v>283</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>45</v>
@@ -10392,7 +10445,7 @@
       </c>
       <c r="E4" s="48"/>
       <c r="F4" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>38</v>
@@ -10410,7 +10463,7 @@
       </c>
       <c r="E5" s="48"/>
       <c r="F5" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>33</v>
@@ -10424,11 +10477,11 @@
       <c r="B6" s="51"/>
       <c r="C6" s="51"/>
       <c r="D6" s="2" t="s">
-        <v>19</v>
+        <v>282</v>
       </c>
       <c r="E6" s="49"/>
       <c r="F6" s="2" t="s">
-        <v>59</v>
+        <v>284</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>38</v>
@@ -10442,16 +10495,16 @@
       <c r="B7" s="52"/>
       <c r="C7" s="52"/>
       <c r="D7" s="20" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E7" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="F7" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="G7" s="21" t="s">
         <v>135</v>
-      </c>
-      <c r="G7" s="21" t="s">
-        <v>136</v>
       </c>
       <c r="H7" s="21"/>
     </row>
@@ -10478,7 +10531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -10537,16 +10590,16 @@
         <v>20</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="E3" s="47" t="s">
         <v>277</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="F3" s="2" t="s">
         <v>279</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>281</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>32</v>
@@ -10564,7 +10617,7 @@
       </c>
       <c r="E4" s="48"/>
       <c r="F4" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>38</v>
@@ -10582,7 +10635,7 @@
       </c>
       <c r="E5" s="49"/>
       <c r="F5" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>32</v>
@@ -10596,16 +10649,16 @@
       <c r="B6" s="44"/>
       <c r="C6" s="44"/>
       <c r="D6" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="E6" s="28" t="s">
         <v>278</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="F6" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>282</v>
-      </c>
       <c r="G6" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H6" s="6"/>
     </row>
@@ -10616,16 +10669,16 @@
       <c r="B7" s="45"/>
       <c r="C7" s="45"/>
       <c r="D7" s="20" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E7" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="F7" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="G7" s="21" t="s">
         <v>135</v>
-      </c>
-      <c r="G7" s="21" t="s">
-        <v>136</v>
       </c>
       <c r="H7" s="21"/>
     </row>
@@ -10701,22 +10754,22 @@
     </row>
     <row r="3" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B3" s="50" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="50" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E3" s="47" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>36</v>
@@ -10725,16 +10778,16 @@
     </row>
     <row r="4" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B4" s="51"/>
       <c r="C4" s="51"/>
       <c r="D4" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E4" s="48"/>
       <c r="F4" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>34</v>
@@ -10743,16 +10796,16 @@
     </row>
     <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B5" s="51"/>
       <c r="C5" s="51"/>
       <c r="D5" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5" s="48"/>
       <c r="F5" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>35</v>
@@ -10761,36 +10814,36 @@
     </row>
     <row r="6" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B6" s="51"/>
       <c r="C6" s="51"/>
       <c r="D6" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E6" s="49"/>
       <c r="F6" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A7" s="20" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B7" s="52"/>
       <c r="C7" s="52"/>
       <c r="D7" s="20" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G7" s="21" t="s">
         <v>32</v>
@@ -10825,22 +10878,22 @@
     </row>
     <row r="10" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B10" s="50" t="s">
         <v>24</v>
       </c>
       <c r="C10" s="50" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E10" s="47" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>32</v>
@@ -10849,16 +10902,16 @@
     </row>
     <row r="11" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B11" s="51"/>
       <c r="C11" s="51"/>
       <c r="D11" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E11" s="48"/>
       <c r="F11" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>32</v>
@@ -10867,16 +10920,16 @@
     </row>
     <row r="12" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B12" s="51"/>
       <c r="C12" s="51"/>
       <c r="D12" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E12" s="48"/>
       <c r="F12" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>32</v>
@@ -10885,16 +10938,16 @@
     </row>
     <row r="13" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B13" s="51"/>
       <c r="C13" s="51"/>
       <c r="D13" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E13" s="49"/>
       <c r="F13" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>32</v>
@@ -10903,21 +10956,21 @@
     </row>
     <row r="14" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A14" s="20" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B14" s="52"/>
       <c r="C14" s="52"/>
       <c r="D14" s="20" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F14" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="G14" s="21" t="s">
         <v>135</v>
-      </c>
-      <c r="G14" s="21" t="s">
-        <v>136</v>
       </c>
       <c r="H14" s="21"/>
     </row>
@@ -11000,22 +11053,22 @@
         <v>26</v>
       </c>
       <c r="C3" s="50" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E3" s="47" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>32</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
@@ -11029,7 +11082,7 @@
       </c>
       <c r="E4" s="48"/>
       <c r="F4" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>38</v>
@@ -11047,7 +11100,7 @@
       </c>
       <c r="E5" s="49"/>
       <c r="F5" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>34</v>
@@ -11061,16 +11114,16 @@
       <c r="B6" s="52"/>
       <c r="C6" s="52"/>
       <c r="D6" s="20" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F6" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="G6" s="21" t="s">
         <v>135</v>
-      </c>
-      <c r="G6" s="21" t="s">
-        <v>136</v>
       </c>
       <c r="H6" s="21"/>
     </row>
@@ -11161,7 +11214,7 @@
         <v>48</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F3" s="50" t="s">
         <v>52</v>
@@ -11181,7 +11234,7 @@
         <v>49</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F4" s="51"/>
       <c r="G4" s="2" t="s">
@@ -11199,7 +11252,7 @@
         <v>50</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F5" s="51"/>
       <c r="G5" s="2" t="s">
@@ -11217,7 +11270,7 @@
         <v>51</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F6" s="51"/>
       <c r="G6" s="5" t="s">
@@ -11235,7 +11288,7 @@
         <v>53</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F7" s="52"/>
       <c r="G7" s="5" t="s">

</xml_diff>

<commit_message>
Update the test case file on the afternoon of 22th,June
</commit_message>
<xml_diff>
--- a/src/MyItems/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Test Cases for FileOperation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="5355" windowHeight="7605" tabRatio="914"/>
   </bookViews>
   <sheets>
     <sheet name="1.替换txt文件内的指定内容" sheetId="14" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="287">
   <si>
     <t>删除文件夹</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -5708,10 +5708,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>10.10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>退出程序，并输出Bye</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -7951,6 +7947,43 @@
         <scheme val="minor"/>
       </rPr>
       <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在"Please choose :"中输入9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>进入"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>查看PC信息</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"模块，并输出本机系统，用户，IP地址等信息</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -7959,6 +7992,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="179" formatCode="0.00_ "/>
+  </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -8174,7 +8210,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -8260,9 +8296,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8363,6 +8396,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8671,7 +8716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -8688,14 +8733,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="46"/>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
+      <c r="A1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -8727,16 +8772,16 @@
       <c r="A3" s="22">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="49" t="s">
         <v>141</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="46" t="s">
         <v>132</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -8751,12 +8796,12 @@
       <c r="A4" s="22">
         <v>1.2</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="48"/>
+      <c r="E4" s="47"/>
       <c r="F4" s="2" t="s">
         <v>129</v>
       </c>
@@ -8769,12 +8814,12 @@
       <c r="A5" s="22">
         <v>1.3</v>
       </c>
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
       <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="48"/>
+      <c r="E5" s="47"/>
       <c r="F5" s="2" t="s">
         <v>101</v>
       </c>
@@ -8787,12 +8832,12 @@
       <c r="A6" s="22">
         <v>1.4</v>
       </c>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="49"/>
+      <c r="E6" s="48"/>
       <c r="F6" s="2" t="s">
         <v>100</v>
       </c>
@@ -8805,8 +8850,8 @@
       <c r="A7" s="27">
         <v>1.5</v>
       </c>
-      <c r="B7" s="52"/>
-      <c r="C7" s="52"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
       <c r="D7" s="20" t="s">
         <v>182</v>
       </c>
@@ -8840,7 +8885,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
@@ -8848,7 +8893,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.875" style="64" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.875" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="28.375" customWidth="1"/>
@@ -8859,17 +8904,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="55"/>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
+      <c r="A1" s="54"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="62" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -8895,41 +8940,41 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A3" s="22">
+      <c r="A3" s="63">
         <v>10.1</v>
       </c>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="61" t="s">
         <v>198</v>
       </c>
-      <c r="C3" s="62" t="s">
+      <c r="C3" s="61" t="s">
         <v>199</v>
       </c>
-      <c r="D3" s="62" t="s">
+      <c r="D3" s="61" t="s">
         <v>200</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>201</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>214</v>
-      </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A4" s="22">
+      <c r="A4" s="63">
         <v>10.199999999999999</v>
       </c>
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
       <c r="E4" s="2" t="s">
         <v>202</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>184</v>
@@ -8937,17 +8982,17 @@
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A5" s="22">
+      <c r="A5" s="63">
         <v>10.3</v>
       </c>
-      <c r="B5" s="62"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
       <c r="E5" s="2" t="s">
         <v>203</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>184</v>
@@ -8955,17 +9000,17 @@
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A6" s="22">
+      <c r="A6" s="63">
         <v>10.4</v>
       </c>
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
       <c r="E6" s="2" t="s">
         <v>204</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>184</v>
@@ -8973,17 +9018,17 @@
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A7" s="22">
+      <c r="A7" s="63">
         <v>10.5</v>
       </c>
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
       <c r="E7" s="2" t="s">
         <v>205</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>184</v>
@@ -8991,17 +9036,17 @@
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A8" s="22">
+      <c r="A8" s="63">
         <v>10.6</v>
       </c>
-      <c r="B8" s="62"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
       <c r="E8" s="2" t="s">
         <v>206</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>184</v>
@@ -9009,17 +9054,17 @@
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A9" s="22">
+      <c r="A9" s="63">
         <v>10.7</v>
       </c>
-      <c r="B9" s="62"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
       <c r="E9" s="2" t="s">
         <v>207</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>184</v>
@@ -9027,17 +9072,17 @@
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A10" s="22">
+      <c r="A10" s="63">
         <v>10.8</v>
       </c>
-      <c r="B10" s="62"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
       <c r="E10" s="2" t="s">
         <v>208</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>184</v>
@@ -9045,50 +9090,69 @@
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A11" s="22">
+      <c r="A11" s="63">
         <v>10.9</v>
       </c>
-      <c r="B11" s="62"/>
-      <c r="C11" s="62"/>
-      <c r="D11" s="62"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="61"/>
       <c r="E11" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A12" s="65">
+        <v>10.1</v>
+      </c>
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A12" s="29" t="s">
+      <c r="F12" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="B12" s="62"/>
-      <c r="C12" s="62"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>212</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>184</v>
       </c>
       <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
+      <c r="A13" s="63" t="s">
+        <v>284</v>
+      </c>
+      <c r="B13" s="61"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="H13" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B3:B12"/>
-    <mergeCell ref="C3:C12"/>
-    <mergeCell ref="D3:D12"/>
+    <mergeCell ref="B3:B13"/>
+    <mergeCell ref="C3:C13"/>
+    <mergeCell ref="D3:D13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9114,14 +9178,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="46"/>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
+      <c r="A1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -9153,10 +9217,10 @@
       <c r="A3" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="49" t="s">
         <v>142</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -9177,8 +9241,8 @@
       <c r="A4" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
@@ -9197,8 +9261,8 @@
       <c r="A5" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
       <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
@@ -9217,8 +9281,8 @@
       <c r="A6" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="B6" s="52"/>
-      <c r="C6" s="52"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="51"/>
       <c r="D6" s="20" t="s">
         <v>182</v>
       </c>
@@ -9275,10 +9339,10 @@
       <c r="A9" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="49" t="s">
         <v>142</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -9300,8 +9364,8 @@
       <c r="A10" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B10" s="51"/>
-      <c r="C10" s="51"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
       <c r="D10" s="2" t="s">
         <v>11</v>
       </c>
@@ -9323,8 +9387,8 @@
       <c r="A11" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B11" s="51"/>
-      <c r="C11" s="51"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
       <c r="D11" s="2" t="s">
         <v>12</v>
       </c>
@@ -9344,8 +9408,8 @@
       <c r="A12" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="B12" s="52"/>
-      <c r="C12" s="52"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="51"/>
       <c r="D12" s="20" t="s">
         <v>182</v>
       </c>
@@ -9362,7 +9426,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
-      <c r="B13" s="53"/>
+      <c r="B13" s="52"/>
       <c r="C13" s="4"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -9373,7 +9437,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
-      <c r="B14" s="53"/>
+      <c r="B14" s="52"/>
       <c r="C14" s="4"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -9384,7 +9448,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
-      <c r="B15" s="53"/>
+      <c r="B15" s="52"/>
       <c r="C15" s="4"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -9395,7 +9459,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
-      <c r="B16" s="53"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="4"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -9406,7 +9470,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
-      <c r="B17" s="53"/>
+      <c r="B17" s="52"/>
       <c r="C17" s="4"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -9482,14 +9546,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A1" s="54"/>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
+      <c r="A1" s="53"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -9521,20 +9585,20 @@
       <c r="A3" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="49" t="s">
         <v>144</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="46" t="s">
         <v>116</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>32</v>
@@ -9545,14 +9609,14 @@
       <c r="A4" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="E4" s="48"/>
+      <c r="E4" s="47"/>
       <c r="F4" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>32</v>
@@ -9563,12 +9627,12 @@
       <c r="A5" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
       <c r="D5" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="48"/>
+      <c r="E5" s="47"/>
       <c r="F5" s="2" t="s">
         <v>104</v>
       </c>
@@ -9581,14 +9645,14 @@
       <c r="A6" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="E6" s="48"/>
+      <c r="E6" s="47"/>
       <c r="F6" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>32</v>
@@ -9599,14 +9663,14 @@
       <c r="A7" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B7" s="51"/>
-      <c r="C7" s="51"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
       <c r="D7" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="48"/>
+      <c r="E7" s="47"/>
       <c r="F7" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>39</v>
@@ -9617,12 +9681,12 @@
       <c r="A8" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="B8" s="51"/>
-      <c r="C8" s="51"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
       <c r="D8" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="E8" s="48"/>
+      <c r="E8" s="47"/>
       <c r="F8" s="19" t="s">
         <v>123</v>
       </c>
@@ -9635,14 +9699,14 @@
       <c r="A9" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="B9" s="51"/>
-      <c r="C9" s="51"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
       <c r="D9" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="E9" s="48"/>
+        <v>244</v>
+      </c>
+      <c r="E9" s="47"/>
       <c r="F9" s="19" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>32</v>
@@ -9650,29 +9714,29 @@
       <c r="H9" s="15"/>
     </row>
     <row r="10" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
-      <c r="A10" s="36" t="s">
-        <v>249</v>
-      </c>
-      <c r="B10" s="51"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="36" t="s">
-        <v>253</v>
-      </c>
-      <c r="E10" s="49"/>
-      <c r="F10" s="37" t="s">
+      <c r="A10" s="35" t="s">
+        <v>248</v>
+      </c>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="35" t="s">
+        <v>252</v>
+      </c>
+      <c r="E10" s="48"/>
+      <c r="F10" s="36" t="s">
+        <v>246</v>
+      </c>
+      <c r="G10" s="37" t="s">
         <v>247</v>
       </c>
-      <c r="G10" s="38" t="s">
-        <v>248</v>
-      </c>
-      <c r="H10" s="38"/>
+      <c r="H10" s="37"/>
     </row>
     <row r="11" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A11" s="20" t="s">
-        <v>250</v>
-      </c>
-      <c r="B11" s="51"/>
-      <c r="C11" s="51"/>
+        <v>249</v>
+      </c>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
       <c r="D11" s="20" t="s">
         <v>182</v>
       </c>
@@ -9689,10 +9753,10 @@
     </row>
     <row r="12" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A12" s="20" t="s">
-        <v>251</v>
-      </c>
-      <c r="B12" s="52"/>
-      <c r="C12" s="52"/>
+        <v>250</v>
+      </c>
+      <c r="B12" s="51"/>
+      <c r="C12" s="51"/>
       <c r="D12" s="20" t="s">
         <v>183</v>
       </c>
@@ -9737,20 +9801,20 @@
       <c r="A16" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="50" t="s">
+      <c r="B16" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="C16" s="50" t="s">
+      <c r="C16" s="49" t="s">
         <v>143</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="E16" s="47" t="s">
+      <c r="E16" s="46" t="s">
         <v>117</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G16" s="14" t="s">
         <v>32</v>
@@ -9761,12 +9825,12 @@
       <c r="A17" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="B17" s="51"/>
-      <c r="C17" s="51"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
       <c r="D17" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="48"/>
+      <c r="E17" s="47"/>
       <c r="F17" s="14" t="s">
         <v>103</v>
       </c>
@@ -9779,12 +9843,12 @@
       <c r="A18" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="B18" s="51"/>
-      <c r="C18" s="51"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="50"/>
       <c r="D18" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="E18" s="48"/>
+      <c r="E18" s="47"/>
       <c r="F18" s="14" t="s">
         <v>121</v>
       </c>
@@ -9797,12 +9861,12 @@
       <c r="A19" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="B19" s="51"/>
-      <c r="C19" s="51"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="50"/>
       <c r="D19" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E19" s="48"/>
+      <c r="E19" s="47"/>
       <c r="F19" s="14" t="s">
         <v>102</v>
       </c>
@@ -9815,12 +9879,12 @@
       <c r="A20" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="B20" s="51"/>
-      <c r="C20" s="51"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
       <c r="D20" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="E20" s="48"/>
+      <c r="E20" s="47"/>
       <c r="F20" s="11" t="s">
         <v>122</v>
       </c>
@@ -9830,29 +9894,29 @@
       <c r="H20" s="16"/>
     </row>
     <row r="21" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
-      <c r="A21" s="36" t="s">
-        <v>254</v>
-      </c>
-      <c r="B21" s="51"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="36" t="s">
-        <v>252</v>
-      </c>
-      <c r="E21" s="49"/>
-      <c r="F21" s="37" t="s">
-        <v>256</v>
-      </c>
-      <c r="G21" s="38" t="s">
-        <v>248</v>
-      </c>
-      <c r="H21" s="38"/>
+      <c r="A21" s="35" t="s">
+        <v>253</v>
+      </c>
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="35" t="s">
+        <v>251</v>
+      </c>
+      <c r="E21" s="48"/>
+      <c r="F21" s="36" t="s">
+        <v>255</v>
+      </c>
+      <c r="G21" s="37" t="s">
+        <v>247</v>
+      </c>
+      <c r="H21" s="37"/>
     </row>
     <row r="22" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A22" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
       <c r="D22" s="20" t="s">
         <v>131</v>
       </c>
@@ -9869,10 +9933,10 @@
     </row>
     <row r="23" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A23" s="20" t="s">
-        <v>255</v>
-      </c>
-      <c r="B23" s="52"/>
-      <c r="C23" s="52"/>
+        <v>254</v>
+      </c>
+      <c r="B23" s="51"/>
+      <c r="C23" s="51"/>
       <c r="D23" s="20" t="s">
         <v>183</v>
       </c>
@@ -9924,14 +9988,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="55"/>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
+      <c r="A1" s="54"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -9961,22 +10025,22 @@
     </row>
     <row r="3" spans="1:8" s="23" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="B3" s="56" t="s">
-        <v>222</v>
-      </c>
-      <c r="C3" s="56" t="s">
+        <v>230</v>
+      </c>
+      <c r="B3" s="55" t="s">
+        <v>221</v>
+      </c>
+      <c r="C3" s="55" t="s">
         <v>145</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="E3" s="59" t="s">
+        <v>226</v>
+      </c>
+      <c r="E3" s="58" t="s">
         <v>152</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>42</v>
@@ -9985,14 +10049,14 @@
     </row>
     <row r="4" spans="1:8" s="23" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
+        <v>231</v>
+      </c>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
       <c r="D4" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="E4" s="60"/>
+        <v>223</v>
+      </c>
+      <c r="E4" s="59"/>
       <c r="F4" s="6" t="s">
         <v>105</v>
       </c>
@@ -10003,16 +10067,16 @@
     </row>
     <row r="5" spans="1:8" s="23" customFormat="1" ht="114" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
+        <v>232</v>
+      </c>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
       <c r="D5" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="60"/>
+      <c r="E5" s="59"/>
       <c r="F5" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>41</v>
@@ -10021,14 +10085,14 @@
     </row>
     <row r="6" spans="1:8" s="23" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
+        <v>233</v>
+      </c>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
       <c r="D6" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="60"/>
+      <c r="E6" s="59"/>
       <c r="F6" s="6" t="s">
         <v>105</v>
       </c>
@@ -10038,47 +10102,47 @@
       <c r="H6" s="25"/>
     </row>
     <row r="7" spans="1:8" s="23" customFormat="1" ht="156.75" x14ac:dyDescent="0.15">
-      <c r="A7" s="30" t="s">
-        <v>235</v>
-      </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="30" t="s">
-        <v>228</v>
-      </c>
-      <c r="E7" s="60"/>
-      <c r="F7" s="30" t="s">
-        <v>271</v>
-      </c>
-      <c r="G7" s="31" t="s">
+      <c r="A7" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="B7" s="56"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="29" t="s">
+        <v>227</v>
+      </c>
+      <c r="E7" s="59"/>
+      <c r="F7" s="29" t="s">
+        <v>270</v>
+      </c>
+      <c r="G7" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="H7" s="32"/>
+      <c r="H7" s="31"/>
     </row>
     <row r="8" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
-      <c r="A8" s="39" t="s">
-        <v>259</v>
-      </c>
-      <c r="B8" s="57"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="36" t="s">
-        <v>262</v>
-      </c>
-      <c r="E8" s="61"/>
-      <c r="F8" s="37" t="s">
-        <v>264</v>
-      </c>
-      <c r="G8" s="40" t="s">
-        <v>248</v>
-      </c>
-      <c r="H8" s="41"/>
+      <c r="A8" s="38" t="s">
+        <v>258</v>
+      </c>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="35" t="s">
+        <v>261</v>
+      </c>
+      <c r="E8" s="60"/>
+      <c r="F8" s="36" t="s">
+        <v>263</v>
+      </c>
+      <c r="G8" s="39" t="s">
+        <v>247</v>
+      </c>
+      <c r="H8" s="40"/>
     </row>
     <row r="9" spans="1:8" s="23" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A9" s="20" t="s">
-        <v>236</v>
-      </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="57"/>
+        <v>235</v>
+      </c>
+      <c r="B9" s="56"/>
+      <c r="C9" s="56"/>
       <c r="D9" s="20" t="s">
         <v>182</v>
       </c>
@@ -10093,12 +10157,12 @@
       </c>
       <c r="H9" s="21"/>
     </row>
-    <row r="10" spans="1:8" s="34" customFormat="1" ht="142.5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" s="33" customFormat="1" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A10" s="20" t="s">
-        <v>258</v>
-      </c>
-      <c r="B10" s="58"/>
-      <c r="C10" s="58"/>
+        <v>257</v>
+      </c>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
       <c r="D10" s="20" t="s">
         <v>183</v>
       </c>
@@ -10113,16 +10177,16 @@
       </c>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" spans="1:8" s="34" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" s="33" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
-      <c r="E11" s="33"/>
+      <c r="E11" s="32"/>
       <c r="F11" s="9"/>
-      <c r="H11" s="35"/>
-    </row>
-    <row r="12" spans="1:8" s="34" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="H11" s="34"/>
+    </row>
+    <row r="12" spans="1:8" s="33" customFormat="1" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
@@ -10150,22 +10214,22 @@
     </row>
     <row r="13" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="B13" s="50" t="s">
-        <v>223</v>
-      </c>
-      <c r="C13" s="56" t="s">
+        <v>236</v>
+      </c>
+      <c r="B13" s="49" t="s">
+        <v>222</v>
+      </c>
+      <c r="C13" s="55" t="s">
         <v>145</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="E13" s="47" t="s">
+        <v>224</v>
+      </c>
+      <c r="E13" s="46" t="s">
         <v>138</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>32</v>
@@ -10174,16 +10238,16 @@
     </row>
     <row r="14" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="B14" s="51"/>
-      <c r="C14" s="57"/>
+        <v>237</v>
+      </c>
+      <c r="B14" s="50"/>
+      <c r="C14" s="56"/>
       <c r="D14" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="E14" s="48"/>
+        <v>225</v>
+      </c>
+      <c r="E14" s="47"/>
       <c r="F14" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>32</v>
@@ -10192,14 +10256,14 @@
     </row>
     <row r="15" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="B15" s="51"/>
-      <c r="C15" s="57"/>
+        <v>238</v>
+      </c>
+      <c r="B15" s="50"/>
+      <c r="C15" s="56"/>
       <c r="D15" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E15" s="48"/>
+      <c r="E15" s="47"/>
       <c r="F15" s="2" t="s">
         <v>107</v>
       </c>
@@ -10210,16 +10274,16 @@
     </row>
     <row r="16" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="B16" s="51"/>
-      <c r="C16" s="57"/>
+        <v>239</v>
+      </c>
+      <c r="B16" s="50"/>
+      <c r="C16" s="56"/>
       <c r="D16" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E16" s="48"/>
+      <c r="E16" s="47"/>
       <c r="F16" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>32</v>
@@ -10228,14 +10292,14 @@
     </row>
     <row r="17" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="B17" s="51"/>
-      <c r="C17" s="57"/>
+        <v>240</v>
+      </c>
+      <c r="B17" s="50"/>
+      <c r="C17" s="56"/>
       <c r="D17" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E17" s="48"/>
+      <c r="E17" s="47"/>
       <c r="F17" s="2" t="s">
         <v>106</v>
       </c>
@@ -10246,14 +10310,14 @@
     </row>
     <row r="18" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A18" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="B18" s="51"/>
-      <c r="C18" s="57"/>
+        <v>241</v>
+      </c>
+      <c r="B18" s="50"/>
+      <c r="C18" s="56"/>
       <c r="D18" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="E18" s="48"/>
+        <v>229</v>
+      </c>
+      <c r="E18" s="47"/>
       <c r="F18" s="11" t="s">
         <v>96</v>
       </c>
@@ -10264,14 +10328,14 @@
     </row>
     <row r="19" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A19" s="11" t="s">
-        <v>243</v>
-      </c>
-      <c r="B19" s="51"/>
-      <c r="C19" s="57"/>
+        <v>242</v>
+      </c>
+      <c r="B19" s="50"/>
+      <c r="C19" s="56"/>
       <c r="D19" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="E19" s="48"/>
+        <v>228</v>
+      </c>
+      <c r="E19" s="47"/>
       <c r="F19" s="11" t="s">
         <v>96</v>
       </c>
@@ -10281,29 +10345,29 @@
       <c r="H19" s="16"/>
     </row>
     <row r="20" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
-      <c r="A20" s="36" t="s">
-        <v>261</v>
-      </c>
-      <c r="B20" s="51"/>
-      <c r="C20" s="57"/>
-      <c r="D20" s="36" t="s">
-        <v>263</v>
-      </c>
-      <c r="E20" s="49"/>
-      <c r="F20" s="37" t="s">
+      <c r="A20" s="35" t="s">
         <v>260</v>
       </c>
-      <c r="G20" s="42" t="s">
-        <v>248</v>
-      </c>
-      <c r="H20" s="43"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="35" t="s">
+        <v>262</v>
+      </c>
+      <c r="E20" s="48"/>
+      <c r="F20" s="36" t="s">
+        <v>259</v>
+      </c>
+      <c r="G20" s="41" t="s">
+        <v>247</v>
+      </c>
+      <c r="H20" s="42"/>
     </row>
     <row r="21" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A21" s="20" t="s">
-        <v>244</v>
-      </c>
-      <c r="B21" s="51"/>
-      <c r="C21" s="57"/>
+        <v>243</v>
+      </c>
+      <c r="B21" s="50"/>
+      <c r="C21" s="56"/>
       <c r="D21" s="20" t="s">
         <v>182</v>
       </c>
@@ -10320,10 +10384,10 @@
     </row>
     <row r="22" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A22" s="20" t="s">
-        <v>257</v>
-      </c>
-      <c r="B22" s="52"/>
-      <c r="C22" s="58"/>
+        <v>256</v>
+      </c>
+      <c r="B22" s="51"/>
+      <c r="C22" s="57"/>
       <c r="D22" s="20" t="s">
         <v>183</v>
       </c>
@@ -10358,7 +10422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -10375,14 +10439,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="55"/>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
+      <c r="A1" s="54"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -10414,17 +10478,17 @@
       <c r="A3" s="22">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="49" t="s">
         <v>146</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="47" t="s">
-        <v>283</v>
+      <c r="E3" s="46" t="s">
+        <v>282</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>128</v>
@@ -10438,12 +10502,12 @@
       <c r="A4" s="22">
         <v>5.2</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="48"/>
+      <c r="E4" s="47"/>
       <c r="F4" s="2" t="s">
         <v>127</v>
       </c>
@@ -10456,12 +10520,12 @@
       <c r="A5" s="22">
         <v>5.3</v>
       </c>
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
       <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="48"/>
+      <c r="E5" s="47"/>
       <c r="F5" s="2" t="s">
         <v>108</v>
       </c>
@@ -10474,14 +10538,14 @@
       <c r="A6" s="22">
         <v>5.4</v>
       </c>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="E6" s="49"/>
+        <v>281</v>
+      </c>
+      <c r="E6" s="48"/>
       <c r="F6" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>38</v>
@@ -10492,8 +10556,8 @@
       <c r="A7" s="27">
         <v>5.5</v>
       </c>
-      <c r="B7" s="52"/>
-      <c r="C7" s="52"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
       <c r="D7" s="20" t="s">
         <v>182</v>
       </c>
@@ -10547,14 +10611,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="55"/>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
+      <c r="A1" s="54"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -10593,13 +10657,13 @@
         <v>147</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="E3" s="47" t="s">
-        <v>277</v>
+        <v>274</v>
+      </c>
+      <c r="E3" s="46" t="s">
+        <v>276</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>32</v>
@@ -10610,14 +10674,14 @@
       <c r="A4" s="22">
         <v>6.2</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
       <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="48"/>
+      <c r="E4" s="47"/>
       <c r="F4" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>38</v>
@@ -10628,12 +10692,12 @@
       <c r="A5" s="22">
         <v>6.3</v>
       </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
       <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="49"/>
+      <c r="E5" s="48"/>
       <c r="F5" s="2" t="s">
         <v>109</v>
       </c>
@@ -10646,16 +10710,16 @@
       <c r="A6" s="24">
         <v>6.4</v>
       </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>184</v>
@@ -10666,8 +10730,8 @@
       <c r="A7" s="27">
         <v>6.5</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
       <c r="D7" s="20" t="s">
         <v>182</v>
       </c>
@@ -10717,14 +10781,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="55"/>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
+      <c r="A1" s="54"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -10756,16 +10820,16 @@
       <c r="A3" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="49" t="s">
         <v>148</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="46" t="s">
         <v>118</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -10780,12 +10844,12 @@
       <c r="A4" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E4" s="48"/>
+      <c r="E4" s="47"/>
       <c r="F4" s="2" t="s">
         <v>76</v>
       </c>
@@ -10798,12 +10862,12 @@
       <c r="A5" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
       <c r="D5" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E5" s="48"/>
+      <c r="E5" s="47"/>
       <c r="F5" s="2" t="s">
         <v>110</v>
       </c>
@@ -10816,12 +10880,12 @@
       <c r="A6" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E6" s="49"/>
+      <c r="E6" s="48"/>
       <c r="F6" s="6" t="s">
         <v>77</v>
       </c>
@@ -10834,8 +10898,8 @@
       <c r="A7" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="B7" s="52"/>
-      <c r="C7" s="52"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
       <c r="D7" s="20" t="s">
         <v>182</v>
       </c>
@@ -10880,16 +10944,16 @@
       <c r="A10" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="50" t="s">
+      <c r="C10" s="49" t="s">
         <v>93</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E10" s="47" t="s">
+      <c r="E10" s="46" t="s">
         <v>119</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -10904,12 +10968,12 @@
       <c r="A11" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B11" s="51"/>
-      <c r="C11" s="51"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
       <c r="D11" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E11" s="48"/>
+      <c r="E11" s="47"/>
       <c r="F11" s="2" t="s">
         <v>185</v>
       </c>
@@ -10922,12 +10986,12 @@
       <c r="A12" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B12" s="51"/>
-      <c r="C12" s="51"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
       <c r="D12" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E12" s="48"/>
+      <c r="E12" s="47"/>
       <c r="F12" s="2" t="s">
         <v>85</v>
       </c>
@@ -10940,12 +11004,12 @@
       <c r="A13" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="B13" s="51"/>
-      <c r="C13" s="51"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
       <c r="D13" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="E13" s="49"/>
+      <c r="E13" s="48"/>
       <c r="F13" s="6" t="s">
         <v>88</v>
       </c>
@@ -10958,8 +11022,8 @@
       <c r="A14" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="B14" s="52"/>
-      <c r="C14" s="52"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="51"/>
       <c r="D14" s="20" t="s">
         <v>182</v>
       </c>
@@ -11010,14 +11074,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="55"/>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
+      <c r="A1" s="54"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -11049,16 +11113,16 @@
       <c r="A3" s="22">
         <v>8.1</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="49" t="s">
         <v>149</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="46" t="s">
         <v>140</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -11075,12 +11139,12 @@
       <c r="A4" s="22">
         <v>8.1999999999999993</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="48"/>
+      <c r="E4" s="47"/>
       <c r="F4" s="2" t="s">
         <v>59</v>
       </c>
@@ -11093,12 +11157,12 @@
       <c r="A5" s="22">
         <v>8.3000000000000007</v>
       </c>
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
       <c r="D5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="49"/>
+      <c r="E5" s="48"/>
       <c r="F5" s="2" t="s">
         <v>111</v>
       </c>
@@ -11111,8 +11175,8 @@
       <c r="A6" s="27">
         <v>8.4</v>
       </c>
-      <c r="B6" s="52"/>
-      <c r="C6" s="52"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="51"/>
       <c r="D6" s="20" t="s">
         <v>182</v>
       </c>
@@ -11165,14 +11229,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="55"/>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
+      <c r="A1" s="54"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -11204,10 +11268,10 @@
       <c r="A3" s="22">
         <v>9.1</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="49" t="s">
         <v>47</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -11216,7 +11280,7 @@
       <c r="E3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="50" t="s">
+      <c r="F3" s="49" t="s">
         <v>52</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -11228,15 +11292,15 @@
       <c r="A4" s="22">
         <v>9.1999999999999993</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="2" t="s">
         <v>49</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="51"/>
+      <c r="F4" s="50"/>
       <c r="G4" s="2" t="s">
         <v>54</v>
       </c>
@@ -11246,15 +11310,15 @@
       <c r="A5" s="22">
         <v>9.3000000000000007</v>
       </c>
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
       <c r="D5" s="2" t="s">
         <v>50</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="51"/>
+      <c r="F5" s="50"/>
       <c r="G5" s="2" t="s">
         <v>54</v>
       </c>
@@ -11264,15 +11328,15 @@
       <c r="A6" s="22">
         <v>9.4</v>
       </c>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="2" t="s">
         <v>51</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="51"/>
+      <c r="F6" s="50"/>
       <c r="G6" s="5" t="s">
         <v>54</v>
       </c>
@@ -11282,15 +11346,15 @@
       <c r="A7" s="22">
         <v>9.5</v>
       </c>
-      <c r="B7" s="52"/>
-      <c r="C7" s="52"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
       <c r="D7" s="2" t="s">
         <v>53</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="52"/>
+      <c r="F7" s="51"/>
       <c r="G7" s="5" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
Update the test case file on the afternoon of 27th,June
</commit_message>
<xml_diff>
--- a/src/MyItems/Test Cases for FileOperation.xlsx
+++ b/src/MyItems/Test Cases for FileOperation.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="288">
   <si>
     <t>删除文件夹</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2634,66 +2634,6 @@
   </si>
   <si>
     <r>
-      <t>1.有显示该文件被删除的消息（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test1\456.txt has been deleted succeeded!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）        
-2.本地计算机上该文件确实被删除</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.有显示该文件夹被删除的消息 (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> D:\Test1\cCc has been deleted succeeded!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)
-2.本地计算机上该文件夹确实被删除</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>1.检查是否会提示“覆盖”信息
 （</t>
     </r>
@@ -2726,36 +2666,6 @@
   </si>
   <si>
     <r>
-      <t>1.有显示该文件夹被删除的消息 (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test1\cCc has been deleted succeeded!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)
-2.本地计算机上该文件夹确实被删除</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>1.显示该文件夹路径不存在，有错误提示信息（</t>
     </r>
     <r>
@@ -3643,270 +3553,6 @@
   </si>
   <si>
     <r>
-      <t>1.有显示该文件被删除的消息（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> D:\Test1\456.txt has been deleted succeeded!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）        
-2.本地计算机上该文件确实被删除</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.新建目标文件夹路径
-2.显示文件复制到了新建路径（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\But.txt has been copied to E:\Program Files\Jenson succeeded!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.检查是否会提示“覆盖”信息
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>There is a same file on target file , would you still want to copy? (Y/N)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.若选择覆盖后，原有文件应被复制替换为新的文件 （</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\But.txt has been copied to E:\Program Files\Jenson succeeded!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.检查是否会提示“覆盖”信息
-（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>There is a same folder on target folder , would you still want to copy? (Y/N)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.若选择覆盖，则被复制的文件夹内的内容会被复制到目标文件夹内（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test33 have copied succeeded to folder E:\Program Files\Test33</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.显示指定的文件夹名已被换成新命名的名字（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\TesT39 has been renamed as D:\Test4 succeeded!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.在本地计算机中能够查看到新命名的文件夹</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.显示指定的文件名已被换成新命名的名字（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\ALO.bmp has been renamed as D:\Test\BUT.txt succeeded!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）
-2.在本地计算机中能够查看到新命名的文件</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1. 显示批量成功的将相同字段的文件名被替换为指定的新名称
-(</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\alonso.accdb has been replaced as D:\Test\Button.accdb succeeded!
-========================================
-D:\Test\alonso.bmp has been replaced as D:\Test\Button.bmp succeeded!
-========================================
-D:\Test\alonso.txt has been replaced as D:\Test\Button.txt succeeded!
-=======================================</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>=)
-2.可以在本地计算机中查到新名称文件</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>1. 能够出现提示输入的信息
 2.显示该内容未在指定文件内查询到(</t>
     </r>
@@ -3992,48 +3638,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1. 能够出现提示输入的信息
-2. 显示指定的内容已经被查到，并替换成功，并能够在本地文件中查看到替换之处，如测试数据所示，应将</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>替换成</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alonso (But has been replaced as Button on file D:\Test9\99888.txt succeeded!)</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -7042,6 +6646,750 @@
   </si>
   <si>
     <r>
+      <t>1.输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹路径
+2.输入文件夹下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件名或扩展名</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹路径
+2.输入文件夹下</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹名</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What file or folder you want to find on this folder?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入文件名或扩展名，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.txt，456.txt,20170614</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What file or folder you want to find on this folder?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入文件夹名，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>McLaren</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.能够出现提示输入的信息
+2.显示指定文件被找到的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>File: txt has found on D:\Test Folder\Test9\寝室宽带账号.txt
+File: txt has found on D:\Test Folder\Test9\CCC\Honda.txt
+File: txt has found on D:\Test Folder\Test9\McLaren\Button.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.能够出现提示输入的信息
+2.显示指定文件被找到的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Folder: McLAREN has found on D:\Test Folder\Test9\McLaren</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.能够出现提示输入的信息
+2.显示指定文件未被找到的信息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>9888.png didn't found on D:\Test1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.输入</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>存在的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>文件夹路径且</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>不包含</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">txt文件
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please input the folder path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" 输入路径，如:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.在"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="4"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>What content you want to find on txt file?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>",输入txt文件内存在的内容，如</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Alonso
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 不出现需要查找内容的输入框
+2. 显示该文件夹下不存在txt文件（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>There is no txt files under folder D:\Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在"Please choose :"中输入9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>进入"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>查看PC信息</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"模块，并输出本机系统，用户，IP地址等信息</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 能够出现提示输入的信息
+2. 显示指定的内容已经被查到，并替换成功，并能够在本地文件中查看到替换之处，如测试数据所示，应将Alo替换成Alonso (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>But has been replaced as Button on file D:\Test9\99888.txt successfully!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.有显示该文件夹被删除的消息 (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test1\cCc has been deleted successfully!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)
+2.本地计算机上该文件夹确实被删除</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.有显示该文件被删除的消息（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test1\456.txt has been deleted successfully!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）        
+2.本地计算机上该文件确实被删除</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.有显示该文件被删除的消息（ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test1\456.txt has been deleted successfully!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）        
+2.本地计算机上该文件确实被删除</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.有显示该文件夹被删除的消息 ( </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test1\cCc has been deleted successfully!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)
+2.本地计算机上该文件夹确实被删除</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
       <t>1.显示文件夹成功被复制到指定路径（</t>
     </r>
     <r>
@@ -7054,7 +7402,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>D:\Test33 has copied succeeded to folder E:\Program Files</t>
+      <t>D:\Test33 has copied successfully to folder E:\Program Files</t>
     </r>
     <r>
       <rPr>
@@ -7073,6 +7421,37 @@
   </si>
   <si>
     <r>
+      <t>1.显示文件夹成功被复制到指定路径（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test33 has copied successfully to folder E:\Program Files</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.本地计算机上存在复制后的新路径
+3.若目标文件夹路径已存在，则会提示是否删除原文件夹，并重新复制到该文件夹中</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
       <t>1.新创建目标文件夹
 2.文件夹复制到新创建的指定路径，且目录下包含原名称的子文件夹（</t>
     </r>
@@ -7086,7 +7465,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>D:\Test33 has copied succeeded to folder E:\Program Files\McL</t>
+      <t>D:\Test33 has copied successfully to folder E:\Program Files\McL</t>
     </r>
     <r>
       <rPr>
@@ -7140,7 +7519,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>D:\Test33 has copied succeeded to folder E:\Program Files</t>
+      <t>D:\Test33 have copied successfully to folder E:\Program Files\Test33</t>
     </r>
     <r>
       <rPr>
@@ -7157,6 +7536,60 @@
   </si>
   <si>
     <r>
+      <t>1.检查是否会提示“覆盖”信息
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>There is a same folder on target folder , would you still want to copy? (Y/N)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.若选择覆盖，则被复制的文件夹内的内容会被复制到目标文件夹内（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test33 has copied successfully to folder E:\Program Files</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
       <t>1.显示文件成功被复制到指定路径（</t>
     </r>
     <r>
@@ -7165,11 +7598,11 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test\But.txt has been copied to E:\Program Files succeeded!</t>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\But.txt has been copied to E:\Program Files successfully!</t>
     </r>
     <r>
       <rPr>
@@ -7188,6 +7621,90 @@
   </si>
   <si>
     <r>
+      <t>1.新建目标文件夹路径
+2.显示文件复制到了新建路径（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\But.txt has been copied to E:\Program Files\Jenson successfully!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.检查是否会提示“覆盖”信息
+（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>There is a same file on target file , would you still want to copy? (Y/N)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.若选择覆盖后，原有文件应被复制替换为新的文件 （</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\But.txt has been copied to E:\Program Files\Jenson successfully!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
       <t>1.显示指定的文件已经成功的移动到了新路径中（</t>
     </r>
     <r>
@@ -7200,7 +7717,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Alonso.txt has been moved from D:\Test\ to E:\Program Files\Test succeeded!</t>
+      <t>Alonso.txt has been moved from D:\Test\ to E:\Program Files\Test successfully!</t>
     </r>
     <r>
       <rPr>
@@ -7231,7 +7748,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Alonso.txt has been moved from D:\Test\ to E:\Program Files\Test succeeded!</t>
+      <t>Alonso.txt has been moved from D:\Test\ to E:\Program Files\Test successfully!</t>
     </r>
     <r>
       <rPr>
@@ -7286,7 +7803,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Alonso.txt has been moved from D:\Test\ to E:\Program Files\Test succeeded!</t>
+      <t>Alonso.txt has been moved from D:\Test\ to E:\Program Files\Test successfully!</t>
     </r>
     <r>
       <rPr>
@@ -7316,7 +7833,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Test has been moved from D: to E:\Program Files succeeded!</t>
+      <t>Test has been moved from D: to E:\Program Files successfully!</t>
     </r>
     <r>
       <rPr>
@@ -7346,7 +7863,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Test has been moved from D: to E:\Program Files succeeded!</t>
+      <t>Test has been moved from D: to E:\Program Files successfully!</t>
     </r>
     <r>
       <rPr>
@@ -7377,7 +7894,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Test has been moved from D: to E:\Program Files succeeded!</t>
+      <t>Test has been moved from D: to E:\Program Files successfully!</t>
     </r>
     <r>
       <rPr>
@@ -7395,595 +7912,97 @@
   </si>
   <si>
     <r>
-      <t>1.输入</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹路径
-2.输入文件夹下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件名或扩展名</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.输入</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹路径
-2.输入文件夹下</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹名</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What file or folder you want to find on this folder?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入文件名或扩展名，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.txt，456.txt,20170614</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What file or folder you want to find on this folder?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入文件夹名，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>McLaren</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.能够出现提示输入的信息
-2.显示指定文件被找到的信息（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>File: txt has found on D:\Test Folder\Test9\寝室宽带账号.txt
-File: txt has found on D:\Test Folder\Test9\CCC\Honda.txt
-File: txt has found on D:\Test Folder\Test9\McLaren\Button.txt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.能够出现提示输入的信息
-2.显示指定文件被找到的信息（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Folder: McLAREN has found on D:\Test Folder\Test9\McLaren</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.能够出现提示输入的信息
-2.显示指定文件未被找到的信息（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>9888.png didn't found on D:\Test1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.输入</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>存在的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>文件夹路径且</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>不包含</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">txt文件
-</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Please input the folder path:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" 输入路径，如:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.在"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="4"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>What content you want to find on txt file?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>",输入txt文件内存在的内容，如</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Alonso
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t/>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1. 不出现需要查找内容的输入框
-2. 显示该文件夹下不存在txt文件（</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>There is no txt files under folder D:\Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10.11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在"Please choose :"中输入9</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>进入"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>查看PC信息</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"模块，并输出本机系统，用户，IP地址等信息</t>
+      <t>1.显示指定的文件夹名已被换成新命名的名字（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\TesT39 has been renamed as D:\Test4 successfully!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.在本地计算机中能够查看到新命名的文件夹</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1.显示指定的文件名已被换成新命名的名字（</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\ALO.bmp has been renamed as D:\Test\BUT.txt successfully!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）
+2.在本地计算机中能够查看到新命名的文件</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1. 显示批量成功的将相同字段的文件名被替换为指定的新名称
+(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D:\Test\alonso.accdb has been replaced as D:\Test\Button.accdb successfully!
+========================================
+D:\Test\alonso.bmp has been replaced as D:\Test\Button.bmp successfully!
+========================================
+D:\Test\alonso.txt has been replaced as D:\Test\Button.txt successfully!
+========================================</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)
+2.可以在本地计算机中查到新名称文件</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -7993,7 +8012,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="179" formatCode="0.00_ "/>
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -8346,6 +8365,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -8396,18 +8427,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8716,7 +8735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -8733,14 +8752,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="45"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
+      <c r="A1" s="49"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -8772,20 +8791,20 @@
       <c r="A3" s="22">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="49" t="s">
-        <v>141</v>
+      <c r="C3" s="53" t="s">
+        <v>130</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="46" t="s">
-        <v>132</v>
+      <c r="E3" s="50" t="s">
+        <v>121</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>130</v>
+        <v>266</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>33</v>
@@ -8796,14 +8815,14 @@
       <c r="A4" s="22">
         <v>1.2</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
       <c r="D4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="47"/>
+      <c r="E4" s="51"/>
       <c r="F4" s="2" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>34</v>
@@ -8814,14 +8833,14 @@
       <c r="A5" s="22">
         <v>1.3</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
       <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="47"/>
+      <c r="E5" s="51"/>
       <c r="F5" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>35</v>
@@ -8832,14 +8851,14 @@
       <c r="A6" s="22">
         <v>1.4</v>
       </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
       <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="48"/>
+      <c r="E6" s="52"/>
       <c r="F6" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>38</v>
@@ -8850,19 +8869,19 @@
       <c r="A7" s="27">
         <v>1.5</v>
       </c>
-      <c r="B7" s="51"/>
-      <c r="C7" s="51"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="55"/>
       <c r="D7" s="20" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="H7" s="21"/>
     </row>
@@ -8893,7 +8912,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.875" style="64" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.875" style="47" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.875" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="28.375" customWidth="1"/>
@@ -8904,17 +8923,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="54"/>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
+      <c r="A1" s="58"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="45" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -8940,167 +8959,167 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A3" s="63">
+      <c r="A3" s="46">
         <v>10.1</v>
       </c>
-      <c r="B3" s="61" t="s">
-        <v>198</v>
-      </c>
-      <c r="C3" s="61" t="s">
-        <v>199</v>
-      </c>
-      <c r="D3" s="61" t="s">
-        <v>200</v>
+      <c r="B3" s="65" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" s="65" t="s">
+        <v>188</v>
+      </c>
+      <c r="D3" s="65" t="s">
+        <v>189</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>212</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A4" s="63">
+      <c r="A4" s="46">
         <v>10.199999999999999</v>
       </c>
-      <c r="B4" s="61"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
       <c r="E4" s="2" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A5" s="63">
+      <c r="A5" s="46">
         <v>10.3</v>
       </c>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
       <c r="E5" s="2" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A6" s="63">
+      <c r="A6" s="46">
         <v>10.4</v>
       </c>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
       <c r="E6" s="2" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A7" s="63">
+      <c r="A7" s="46">
         <v>10.5</v>
       </c>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
       <c r="E7" s="2" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A8" s="63">
+      <c r="A8" s="46">
         <v>10.6</v>
       </c>
-      <c r="B8" s="61"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
       <c r="E8" s="2" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A9" s="63">
+      <c r="A9" s="46">
         <v>10.7</v>
       </c>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
       <c r="E9" s="2" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
-      <c r="A10" s="63">
+      <c r="A10" s="46">
         <v>10.8</v>
       </c>
-      <c r="B10" s="61"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
       <c r="E10" s="2" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A11" s="63">
+      <c r="A11" s="46">
         <v>10.9</v>
       </c>
-      <c r="B11" s="61"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
       <c r="E11" s="2" t="s">
-        <v>285</v>
+        <v>264</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>286</v>
+        <v>265</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>32</v>
@@ -9108,38 +9127,38 @@
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A12" s="65">
+      <c r="A12" s="48">
         <v>10.1</v>
       </c>
-      <c r="B12" s="61"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
+      <c r="B12" s="65"/>
+      <c r="C12" s="65"/>
+      <c r="D12" s="65"/>
       <c r="E12" s="2" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A13" s="63" t="s">
-        <v>284</v>
-      </c>
-      <c r="B13" s="61"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
+      <c r="A13" s="46" t="s">
+        <v>263</v>
+      </c>
+      <c r="B13" s="65"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
       <c r="E13" s="2" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="H13" s="5"/>
     </row>
@@ -9178,14 +9197,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="A1" s="45"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
+      <c r="A1" s="49"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -9215,13 +9234,13 @@
     </row>
     <row r="3" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B3" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="49" t="s">
-        <v>142</v>
+      <c r="C3" s="53" t="s">
+        <v>131</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -9230,7 +9249,7 @@
         <v>91</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>97</v>
+        <v>267</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>37</v>
@@ -9239,10 +9258,10 @@
     </row>
     <row r="4" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
+        <v>146</v>
+      </c>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
       <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
@@ -9250,7 +9269,7 @@
         <v>92</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>94</v>
+        <v>268</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>32</v>
@@ -9259,10 +9278,10 @@
     </row>
     <row r="5" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
+        <v>147</v>
+      </c>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
       <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
@@ -9270,7 +9289,7 @@
         <v>91</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>37</v>
@@ -9279,18 +9298,18 @@
     </row>
     <row r="6" spans="1:9" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A6" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
+        <v>152</v>
+      </c>
+      <c r="B6" s="55"/>
+      <c r="C6" s="55"/>
       <c r="D6" s="20" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="G6" s="21" t="s">
         <v>32</v>
@@ -9337,22 +9356,22 @@
     </row>
     <row r="9" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B9" s="49" t="s">
+        <v>148</v>
+      </c>
+      <c r="B9" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="49" t="s">
-        <v>142</v>
+      <c r="C9" s="53" t="s">
+        <v>131</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>120</v>
+        <v>269</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>32</v>
@@ -9362,18 +9381,18 @@
     </row>
     <row r="10" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B10" s="50"/>
-      <c r="C10" s="50"/>
+        <v>149</v>
+      </c>
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
       <c r="D10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>95</v>
+        <v>270</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>90</v>
@@ -9385,18 +9404,18 @@
     </row>
     <row r="11" spans="1:9" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
+        <v>150</v>
+      </c>
+      <c r="B11" s="54"/>
+      <c r="C11" s="54"/>
       <c r="D11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>32</v>
@@ -9406,27 +9425,27 @@
     </row>
     <row r="12" spans="1:9" s="23" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A12" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="B12" s="51"/>
-      <c r="C12" s="51"/>
+        <v>151</v>
+      </c>
+      <c r="B12" s="55"/>
+      <c r="C12" s="55"/>
       <c r="D12" s="20" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="G12" s="21" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="H12" s="21"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
-      <c r="B13" s="52"/>
+      <c r="B13" s="56"/>
       <c r="C13" s="4"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -9437,7 +9456,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
-      <c r="B14" s="52"/>
+      <c r="B14" s="56"/>
       <c r="C14" s="4"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -9448,7 +9467,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
-      <c r="B15" s="52"/>
+      <c r="B15" s="56"/>
       <c r="C15" s="4"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -9459,7 +9478,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
-      <c r="B16" s="52"/>
+      <c r="B16" s="56"/>
       <c r="C16" s="4"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -9470,7 +9489,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
-      <c r="B17" s="52"/>
+      <c r="B17" s="56"/>
       <c r="C17" s="4"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -9546,14 +9565,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A1" s="53"/>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
+      <c r="A1" s="57"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -9583,22 +9602,22 @@
     </row>
     <row r="3" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="B3" s="49" t="s">
-        <v>112</v>
-      </c>
-      <c r="C3" s="49" t="s">
-        <v>144</v>
+        <v>156</v>
+      </c>
+      <c r="B3" s="53" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>133</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="E3" s="46" t="s">
-        <v>116</v>
+        <v>153</v>
+      </c>
+      <c r="E3" s="50" t="s">
+        <v>113</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>32</v>
@@ -9607,16 +9626,16 @@
     </row>
     <row r="4" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
+        <v>157</v>
+      </c>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
       <c r="D4" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E4" s="47"/>
+        <v>154</v>
+      </c>
+      <c r="E4" s="51"/>
       <c r="F4" s="2" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>32</v>
@@ -9625,16 +9644,16 @@
     </row>
     <row r="5" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
+        <v>158</v>
+      </c>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
       <c r="D5" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="47"/>
+      <c r="E5" s="51"/>
       <c r="F5" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>40</v>
@@ -9643,16 +9662,16 @@
     </row>
     <row r="6" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
+        <v>159</v>
+      </c>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
       <c r="D6" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E6" s="47"/>
+        <v>139</v>
+      </c>
+      <c r="E6" s="51"/>
       <c r="F6" s="2" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>32</v>
@@ -9661,16 +9680,16 @@
     </row>
     <row r="7" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
+        <v>160</v>
+      </c>
+      <c r="B7" s="54"/>
+      <c r="C7" s="54"/>
       <c r="D7" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="47"/>
+      <c r="E7" s="51"/>
       <c r="F7" s="2" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>39</v>
@@ -9679,16 +9698,16 @@
     </row>
     <row r="8" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A8" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="B8" s="50"/>
-      <c r="C8" s="50"/>
+        <v>161</v>
+      </c>
+      <c r="B8" s="54"/>
+      <c r="C8" s="54"/>
       <c r="D8" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="E8" s="47"/>
+        <v>155</v>
+      </c>
+      <c r="E8" s="51"/>
       <c r="F8" s="19" t="s">
-        <v>123</v>
+        <v>274</v>
       </c>
       <c r="G8" s="15" t="s">
         <v>44</v>
@@ -9697,16 +9716,16 @@
     </row>
     <row r="9" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
+        <v>162</v>
+      </c>
+      <c r="B9" s="54"/>
+      <c r="C9" s="54"/>
       <c r="D9" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="E9" s="47"/>
+        <v>233</v>
+      </c>
+      <c r="E9" s="51"/>
       <c r="F9" s="19" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>32</v>
@@ -9715,36 +9734,36 @@
     </row>
     <row r="10" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A10" s="35" t="s">
-        <v>248</v>
-      </c>
-      <c r="B10" s="50"/>
-      <c r="C10" s="50"/>
+        <v>237</v>
+      </c>
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
       <c r="D10" s="35" t="s">
-        <v>252</v>
-      </c>
-      <c r="E10" s="48"/>
+        <v>241</v>
+      </c>
+      <c r="E10" s="52"/>
       <c r="F10" s="36" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="G10" s="37" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="H10" s="37"/>
     </row>
     <row r="11" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A11" s="20" t="s">
-        <v>249</v>
-      </c>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
+        <v>238</v>
+      </c>
+      <c r="B11" s="54"/>
+      <c r="C11" s="54"/>
       <c r="D11" s="20" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="G11" s="21" t="s">
         <v>32</v>
@@ -9753,18 +9772,18 @@
     </row>
     <row r="12" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A12" s="20" t="s">
-        <v>250</v>
-      </c>
-      <c r="B12" s="51"/>
-      <c r="C12" s="51"/>
+        <v>239</v>
+      </c>
+      <c r="B12" s="55"/>
+      <c r="C12" s="55"/>
       <c r="D12" s="20" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="G12" s="21" t="s">
         <v>32</v>
@@ -9799,22 +9818,22 @@
     </row>
     <row r="16" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A16" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="B16" s="49" t="s">
-        <v>113</v>
-      </c>
-      <c r="C16" s="49" t="s">
-        <v>143</v>
+        <v>165</v>
+      </c>
+      <c r="B16" s="53" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" s="53" t="s">
+        <v>132</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="E16" s="46" t="s">
-        <v>117</v>
+        <v>163</v>
+      </c>
+      <c r="E16" s="50" t="s">
+        <v>114</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="G16" s="14" t="s">
         <v>32</v>
@@ -9823,34 +9842,34 @@
     </row>
     <row r="17" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A17" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
+        <v>166</v>
+      </c>
+      <c r="B17" s="54"/>
+      <c r="C17" s="54"/>
       <c r="D17" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="47"/>
+      <c r="E17" s="51"/>
       <c r="F17" s="14" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G17" s="14" t="s">
         <v>32</v>
       </c>
       <c r="H17" s="14"/>
     </row>
-    <row r="18" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A18" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="B18" s="50"/>
-      <c r="C18" s="50"/>
+        <v>167</v>
+      </c>
+      <c r="B18" s="54"/>
+      <c r="C18" s="54"/>
       <c r="D18" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="E18" s="47"/>
+      <c r="E18" s="51"/>
       <c r="F18" s="14" t="s">
-        <v>121</v>
+        <v>277</v>
       </c>
       <c r="G18" s="14" t="s">
         <v>32</v>
@@ -9859,16 +9878,16 @@
     </row>
     <row r="19" spans="1:8" ht="57" x14ac:dyDescent="0.15">
       <c r="A19" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="B19" s="50"/>
-      <c r="C19" s="50"/>
+        <v>168</v>
+      </c>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
       <c r="D19" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E19" s="47"/>
+      <c r="E19" s="51"/>
       <c r="F19" s="14" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G19" s="14" t="s">
         <v>32</v>
@@ -9877,16 +9896,16 @@
     </row>
     <row r="20" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A20" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="B20" s="50"/>
-      <c r="C20" s="50"/>
+        <v>169</v>
+      </c>
+      <c r="B20" s="54"/>
+      <c r="C20" s="54"/>
       <c r="D20" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="E20" s="47"/>
+        <v>164</v>
+      </c>
+      <c r="E20" s="51"/>
       <c r="F20" s="11" t="s">
-        <v>122</v>
+        <v>278</v>
       </c>
       <c r="G20" s="15" t="s">
         <v>32</v>
@@ -9895,56 +9914,56 @@
     </row>
     <row r="21" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A21" s="35" t="s">
-        <v>253</v>
-      </c>
-      <c r="B21" s="50"/>
-      <c r="C21" s="50"/>
+        <v>242</v>
+      </c>
+      <c r="B21" s="54"/>
+      <c r="C21" s="54"/>
       <c r="D21" s="35" t="s">
-        <v>251</v>
-      </c>
-      <c r="E21" s="48"/>
+        <v>240</v>
+      </c>
+      <c r="E21" s="52"/>
       <c r="F21" s="36" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="G21" s="37" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="H21" s="37"/>
     </row>
     <row r="22" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A22" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="B22" s="50"/>
-      <c r="C22" s="50"/>
+        <v>170</v>
+      </c>
+      <c r="B22" s="54"/>
+      <c r="C22" s="54"/>
       <c r="D22" s="20" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="H22" s="21"/>
     </row>
     <row r="23" spans="1:8" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A23" s="20" t="s">
-        <v>254</v>
-      </c>
-      <c r="B23" s="51"/>
-      <c r="C23" s="51"/>
+        <v>243</v>
+      </c>
+      <c r="B23" s="55"/>
+      <c r="C23" s="55"/>
       <c r="D23" s="20" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="G23" s="21" t="s">
         <v>32</v>
@@ -9971,7 +9990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -9988,14 +10007,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="54"/>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
+      <c r="A1" s="58"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -10025,22 +10044,22 @@
     </row>
     <row r="3" spans="1:8" s="23" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="B3" s="55" t="s">
-        <v>221</v>
-      </c>
-      <c r="C3" s="55" t="s">
-        <v>145</v>
+        <v>219</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>210</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>134</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="E3" s="58" t="s">
-        <v>152</v>
+        <v>215</v>
+      </c>
+      <c r="E3" s="62" t="s">
+        <v>141</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>268</v>
+        <v>279</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>42</v>
@@ -10049,16 +10068,16 @@
     </row>
     <row r="4" spans="1:8" s="23" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
+        <v>220</v>
+      </c>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
       <c r="D4" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="E4" s="59"/>
+        <v>212</v>
+      </c>
+      <c r="E4" s="63"/>
       <c r="F4" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>43</v>
@@ -10067,16 +10086,16 @@
     </row>
     <row r="5" spans="1:8" s="23" customFormat="1" ht="114" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
+        <v>221</v>
+      </c>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
       <c r="D5" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="59"/>
+      <c r="E5" s="63"/>
       <c r="F5" s="6" t="s">
-        <v>269</v>
+        <v>280</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>41</v>
@@ -10085,16 +10104,16 @@
     </row>
     <row r="6" spans="1:8" s="23" customFormat="1" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
+        <v>222</v>
+      </c>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
       <c r="D6" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="59"/>
+      <c r="E6" s="63"/>
       <c r="F6" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G6" s="25" t="s">
         <v>41</v>
@@ -10103,16 +10122,16 @@
     </row>
     <row r="7" spans="1:8" s="23" customFormat="1" ht="156.75" x14ac:dyDescent="0.15">
       <c r="A7" s="29" t="s">
-        <v>234</v>
-      </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
+        <v>223</v>
+      </c>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
       <c r="D7" s="29" t="s">
-        <v>227</v>
-      </c>
-      <c r="E7" s="59"/>
+        <v>216</v>
+      </c>
+      <c r="E7" s="63"/>
       <c r="F7" s="29" t="s">
-        <v>270</v>
+        <v>281</v>
       </c>
       <c r="G7" s="30" t="s">
         <v>75</v>
@@ -10121,36 +10140,36 @@
     </row>
     <row r="8" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A8" s="38" t="s">
-        <v>258</v>
-      </c>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
+        <v>247</v>
+      </c>
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
       <c r="D8" s="35" t="s">
-        <v>261</v>
-      </c>
-      <c r="E8" s="60"/>
+        <v>250</v>
+      </c>
+      <c r="E8" s="64"/>
       <c r="F8" s="36" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="G8" s="39" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="H8" s="40"/>
     </row>
     <row r="9" spans="1:8" s="23" customFormat="1" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A9" s="20" t="s">
-        <v>235</v>
-      </c>
-      <c r="B9" s="56"/>
-      <c r="C9" s="56"/>
+        <v>224</v>
+      </c>
+      <c r="B9" s="60"/>
+      <c r="C9" s="60"/>
       <c r="D9" s="20" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="G9" s="21" t="s">
         <v>32</v>
@@ -10159,18 +10178,18 @@
     </row>
     <row r="10" spans="1:8" s="33" customFormat="1" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A10" s="20" t="s">
-        <v>257</v>
-      </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="57"/>
+        <v>246</v>
+      </c>
+      <c r="B10" s="61"/>
+      <c r="C10" s="61"/>
       <c r="D10" s="20" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="G10" s="21" t="s">
         <v>32</v>
@@ -10214,22 +10233,22 @@
     </row>
     <row r="13" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="B13" s="49" t="s">
-        <v>222</v>
-      </c>
-      <c r="C13" s="55" t="s">
-        <v>145</v>
+        <v>225</v>
+      </c>
+      <c r="B13" s="53" t="s">
+        <v>211</v>
+      </c>
+      <c r="C13" s="59" t="s">
+        <v>134</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="E13" s="46" t="s">
-        <v>138</v>
+        <v>213</v>
+      </c>
+      <c r="E13" s="50" t="s">
+        <v>127</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>271</v>
+        <v>282</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>32</v>
@@ -10238,16 +10257,16 @@
     </row>
     <row r="14" spans="1:8" ht="85.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="B14" s="50"/>
-      <c r="C14" s="56"/>
+        <v>226</v>
+      </c>
+      <c r="B14" s="54"/>
+      <c r="C14" s="60"/>
       <c r="D14" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="E14" s="47"/>
+        <v>214</v>
+      </c>
+      <c r="E14" s="51"/>
       <c r="F14" s="2" t="s">
-        <v>272</v>
+        <v>283</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>32</v>
@@ -10256,16 +10275,16 @@
     </row>
     <row r="15" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="B15" s="50"/>
-      <c r="C15" s="56"/>
+        <v>227</v>
+      </c>
+      <c r="B15" s="54"/>
+      <c r="C15" s="60"/>
       <c r="D15" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E15" s="47"/>
+      <c r="E15" s="51"/>
       <c r="F15" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>32</v>
@@ -10274,16 +10293,16 @@
     </row>
     <row r="16" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="B16" s="50"/>
-      <c r="C16" s="56"/>
+        <v>228</v>
+      </c>
+      <c r="B16" s="54"/>
+      <c r="C16" s="60"/>
       <c r="D16" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E16" s="47"/>
+      <c r="E16" s="51"/>
       <c r="F16" s="2" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>32</v>
@@ -10292,16 +10311,16 @@
     </row>
     <row r="17" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="B17" s="50"/>
-      <c r="C17" s="56"/>
+        <v>229</v>
+      </c>
+      <c r="B17" s="54"/>
+      <c r="C17" s="60"/>
       <c r="D17" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E17" s="47"/>
+      <c r="E17" s="51"/>
       <c r="F17" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>32</v>
@@ -10310,16 +10329,16 @@
     </row>
     <row r="18" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A18" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="B18" s="50"/>
-      <c r="C18" s="56"/>
+        <v>230</v>
+      </c>
+      <c r="B18" s="54"/>
+      <c r="C18" s="60"/>
       <c r="D18" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="E18" s="47"/>
+        <v>218</v>
+      </c>
+      <c r="E18" s="51"/>
       <c r="F18" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G18" s="12" t="s">
         <v>75</v>
@@ -10328,16 +10347,16 @@
     </row>
     <row r="19" spans="1:8" s="23" customFormat="1" ht="128.25" x14ac:dyDescent="0.15">
       <c r="A19" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="B19" s="50"/>
-      <c r="C19" s="56"/>
+        <v>231</v>
+      </c>
+      <c r="B19" s="54"/>
+      <c r="C19" s="60"/>
       <c r="D19" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="E19" s="47"/>
+        <v>217</v>
+      </c>
+      <c r="E19" s="51"/>
       <c r="F19" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G19" s="12" t="s">
         <v>32</v>
@@ -10346,56 +10365,56 @@
     </row>
     <row r="20" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A20" s="35" t="s">
-        <v>260</v>
-      </c>
-      <c r="B20" s="50"/>
-      <c r="C20" s="56"/>
+        <v>249</v>
+      </c>
+      <c r="B20" s="54"/>
+      <c r="C20" s="60"/>
       <c r="D20" s="35" t="s">
-        <v>262</v>
-      </c>
-      <c r="E20" s="48"/>
+        <v>251</v>
+      </c>
+      <c r="E20" s="52"/>
       <c r="F20" s="36" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="G20" s="41" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="H20" s="42"/>
     </row>
     <row r="21" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A21" s="20" t="s">
-        <v>243</v>
-      </c>
-      <c r="B21" s="50"/>
-      <c r="C21" s="56"/>
+        <v>232</v>
+      </c>
+      <c r="B21" s="54"/>
+      <c r="C21" s="60"/>
       <c r="D21" s="20" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="G21" s="21" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="H21" s="21"/>
     </row>
     <row r="22" spans="1:8" ht="142.5" x14ac:dyDescent="0.15">
       <c r="A22" s="20" t="s">
-        <v>256</v>
-      </c>
-      <c r="B22" s="51"/>
-      <c r="C22" s="57"/>
+        <v>245</v>
+      </c>
+      <c r="B22" s="55"/>
+      <c r="C22" s="61"/>
       <c r="D22" s="20" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="G22" s="21" t="s">
         <v>32</v>
@@ -10439,14 +10458,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="54"/>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
+      <c r="A1" s="58"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -10478,20 +10497,20 @@
       <c r="A3" s="22">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="49" t="s">
-        <v>146</v>
+      <c r="C3" s="53" t="s">
+        <v>135</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="46" t="s">
-        <v>282</v>
+      <c r="E3" s="50" t="s">
+        <v>261</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>45</v>
@@ -10502,14 +10521,14 @@
       <c r="A4" s="22">
         <v>5.2</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
       <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="47"/>
+      <c r="E4" s="51"/>
       <c r="F4" s="2" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>38</v>
@@ -10520,14 +10539,14 @@
       <c r="A5" s="22">
         <v>5.3</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
       <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="47"/>
+      <c r="E5" s="51"/>
       <c r="F5" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>33</v>
@@ -10538,14 +10557,14 @@
       <c r="A6" s="22">
         <v>5.4</v>
       </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
       <c r="D6" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="E6" s="48"/>
+        <v>260</v>
+      </c>
+      <c r="E6" s="52"/>
       <c r="F6" s="2" t="s">
-        <v>283</v>
+        <v>262</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>38</v>
@@ -10556,19 +10575,19 @@
       <c r="A7" s="27">
         <v>5.5</v>
       </c>
-      <c r="B7" s="51"/>
-      <c r="C7" s="51"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="55"/>
       <c r="D7" s="20" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="H7" s="21"/>
     </row>
@@ -10611,14 +10630,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="54"/>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
+      <c r="A1" s="58"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -10654,16 +10673,16 @@
         <v>20</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="E3" s="46" t="s">
-        <v>276</v>
+        <v>253</v>
+      </c>
+      <c r="E3" s="50" t="s">
+        <v>255</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>278</v>
+        <v>257</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>32</v>
@@ -10679,9 +10698,9 @@
       <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="47"/>
+      <c r="E4" s="51"/>
       <c r="F4" s="2" t="s">
-        <v>280</v>
+        <v>259</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>38</v>
@@ -10697,9 +10716,9 @@
       <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="48"/>
+      <c r="E5" s="52"/>
       <c r="F5" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>32</v>
@@ -10713,16 +10732,16 @@
       <c r="B6" s="43"/>
       <c r="C6" s="43"/>
       <c r="D6" s="6" t="s">
-        <v>275</v>
+        <v>254</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>277</v>
+        <v>256</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>279</v>
+        <v>258</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="H6" s="6"/>
     </row>
@@ -10733,16 +10752,16 @@
       <c r="B7" s="44"/>
       <c r="C7" s="44"/>
       <c r="D7" s="20" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="H7" s="21"/>
     </row>
@@ -10781,14 +10800,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="54"/>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
+      <c r="A1" s="58"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -10818,22 +10837,22 @@
     </row>
     <row r="3" spans="1:8" ht="99.75" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B3" s="49" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="49" t="s">
-        <v>148</v>
+      <c r="C3" s="53" t="s">
+        <v>137</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E3" s="46" t="s">
-        <v>118</v>
+      <c r="E3" s="50" t="s">
+        <v>115</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>124</v>
+        <v>285</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>36</v>
@@ -10842,14 +10861,14 @@
     </row>
     <row r="4" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
+        <v>176</v>
+      </c>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
       <c r="D4" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E4" s="47"/>
+      <c r="E4" s="51"/>
       <c r="F4" s="2" t="s">
         <v>76</v>
       </c>
@@ -10860,16 +10879,16 @@
     </row>
     <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
+        <v>177</v>
+      </c>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
       <c r="D5" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E5" s="47"/>
+      <c r="E5" s="51"/>
       <c r="F5" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>35</v>
@@ -10878,14 +10897,14 @@
     </row>
     <row r="6" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
+        <v>178</v>
+      </c>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
       <c r="D6" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E6" s="48"/>
+      <c r="E6" s="52"/>
       <c r="F6" s="6" t="s">
         <v>77</v>
       </c>
@@ -10896,18 +10915,18 @@
     </row>
     <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A7" s="20" t="s">
-        <v>190</v>
-      </c>
-      <c r="B7" s="51"/>
-      <c r="C7" s="51"/>
+        <v>179</v>
+      </c>
+      <c r="B7" s="55"/>
+      <c r="C7" s="55"/>
       <c r="D7" s="20" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="G7" s="21" t="s">
         <v>32</v>
@@ -10942,22 +10961,22 @@
     </row>
     <row r="10" spans="1:8" ht="114" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B10" s="49" t="s">
+        <v>180</v>
+      </c>
+      <c r="B10" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="53" t="s">
         <v>93</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E10" s="46" t="s">
-        <v>119</v>
+      <c r="E10" s="50" t="s">
+        <v>116</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>125</v>
+        <v>286</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>32</v>
@@ -10966,16 +10985,16 @@
     </row>
     <row r="11" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
+        <v>181</v>
+      </c>
+      <c r="B11" s="54"/>
+      <c r="C11" s="54"/>
       <c r="D11" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E11" s="47"/>
+      <c r="E11" s="51"/>
       <c r="F11" s="2" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>32</v>
@@ -10984,14 +11003,14 @@
     </row>
     <row r="12" spans="1:8" ht="71.25" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
+        <v>182</v>
+      </c>
+      <c r="B12" s="54"/>
+      <c r="C12" s="54"/>
       <c r="D12" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E12" s="47"/>
+      <c r="E12" s="51"/>
       <c r="F12" s="2" t="s">
         <v>85</v>
       </c>
@@ -11002,14 +11021,14 @@
     </row>
     <row r="13" spans="1:8" s="23" customFormat="1" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
+        <v>183</v>
+      </c>
+      <c r="B13" s="54"/>
+      <c r="C13" s="54"/>
       <c r="D13" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="E13" s="48"/>
+      <c r="E13" s="52"/>
       <c r="F13" s="6" t="s">
         <v>88</v>
       </c>
@@ -11020,21 +11039,21 @@
     </row>
     <row r="14" spans="1:8" ht="42.75" x14ac:dyDescent="0.15">
       <c r="A14" s="20" t="s">
-        <v>195</v>
-      </c>
-      <c r="B14" s="51"/>
-      <c r="C14" s="51"/>
+        <v>184</v>
+      </c>
+      <c r="B14" s="55"/>
+      <c r="C14" s="55"/>
       <c r="D14" s="20" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="H14" s="21"/>
     </row>
@@ -11074,14 +11093,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="54"/>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
+      <c r="A1" s="58"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -11113,38 +11132,38 @@
       <c r="A3" s="22">
         <v>8.1</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="49" t="s">
-        <v>149</v>
+      <c r="C3" s="53" t="s">
+        <v>138</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E3" s="46" t="s">
-        <v>140</v>
+        <v>185</v>
+      </c>
+      <c r="E3" s="50" t="s">
+        <v>129</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>126</v>
+        <v>287</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>32</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="85.5" x14ac:dyDescent="0.15">
       <c r="A4" s="22">
         <v>8.1999999999999993</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
       <c r="D4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="47"/>
+      <c r="E4" s="51"/>
       <c r="F4" s="2" t="s">
         <v>59</v>
       </c>
@@ -11157,14 +11176,14 @@
       <c r="A5" s="22">
         <v>8.3000000000000007</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
       <c r="D5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="48"/>
+      <c r="E5" s="52"/>
       <c r="F5" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>34</v>
@@ -11175,19 +11194,19 @@
       <c r="A6" s="27">
         <v>8.4</v>
       </c>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="55"/>
       <c r="D6" s="20" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="H6" s="21"/>
     </row>
@@ -11229,14 +11248,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="54"/>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
+      <c r="A1" s="58"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -11268,10 +11287,10 @@
       <c r="A3" s="22">
         <v>9.1</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="53" t="s">
         <v>47</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -11280,7 +11299,7 @@
       <c r="E3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="49" t="s">
+      <c r="F3" s="53" t="s">
         <v>52</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -11292,15 +11311,15 @@
       <c r="A4" s="22">
         <v>9.1999999999999993</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
       <c r="D4" s="2" t="s">
         <v>49</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="50"/>
+      <c r="F4" s="54"/>
       <c r="G4" s="2" t="s">
         <v>54</v>
       </c>
@@ -11310,15 +11329,15 @@
       <c r="A5" s="22">
         <v>9.3000000000000007</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
       <c r="D5" s="2" t="s">
         <v>50</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="50"/>
+      <c r="F5" s="54"/>
       <c r="G5" s="2" t="s">
         <v>54</v>
       </c>
@@ -11328,15 +11347,15 @@
       <c r="A6" s="22">
         <v>9.4</v>
       </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
       <c r="D6" s="2" t="s">
         <v>51</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="50"/>
+      <c r="F6" s="54"/>
       <c r="G6" s="5" t="s">
         <v>54</v>
       </c>
@@ -11346,15 +11365,15 @@
       <c r="A7" s="22">
         <v>9.5</v>
       </c>
-      <c r="B7" s="51"/>
-      <c r="C7" s="51"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="55"/>
       <c r="D7" s="2" t="s">
         <v>53</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="51"/>
+      <c r="F7" s="55"/>
       <c r="G7" s="5" t="s">
         <v>54</v>
       </c>

</xml_diff>